<commit_message>
changing extration list to oct2; dec4 2019
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4783E52-554E-924C-BE77-BFC55B88A219}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ACF27B1-3291-6F48-A452-CD09CEFFFBCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="2040" windowWidth="27640" windowHeight="16940" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="30">
   <si>
     <t>ColonyID</t>
   </si>
@@ -490,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1C6750-7F92-2244-B10F-B37DA4CD9192}">
-  <dimension ref="A1:G81"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,12 +998,9 @@
         <v>3</v>
       </c>
       <c r="E22" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F22" t="s">
-        <v>8</v>
-      </c>
-      <c r="G22" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1021,12 +1018,9 @@
         <v>9</v>
       </c>
       <c r="E23" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
-      </c>
-      <c r="G23" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1044,12 +1038,9 @@
         <v>3</v>
       </c>
       <c r="E24" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
-      </c>
-      <c r="G24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1067,12 +1058,9 @@
         <v>9</v>
       </c>
       <c r="E25" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1090,12 +1078,9 @@
         <v>3</v>
       </c>
       <c r="E26" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F26" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1113,12 +1098,9 @@
         <v>9</v>
       </c>
       <c r="E27" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F27" t="s">
-        <v>8</v>
-      </c>
-      <c r="G27" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1136,12 +1118,9 @@
         <v>3</v>
       </c>
       <c r="E28" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1159,12 +1138,9 @@
         <v>9</v>
       </c>
       <c r="E29" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1182,12 +1158,9 @@
         <v>3</v>
       </c>
       <c r="E30" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
-      </c>
-      <c r="G30" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1205,12 +1178,9 @@
         <v>9</v>
       </c>
       <c r="E31" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F31" t="s">
-        <v>8</v>
-      </c>
-      <c r="G31" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1228,16 +1198,13 @@
         <v>3</v>
       </c>
       <c r="E32" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F32" t="s">
         <v>8</v>
       </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>210</v>
       </c>
@@ -1251,16 +1218,13 @@
         <v>9</v>
       </c>
       <c r="E33" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F33" t="s">
         <v>8</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>211</v>
       </c>
@@ -1274,16 +1238,13 @@
         <v>3</v>
       </c>
       <c r="E34" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F34" t="s">
         <v>8</v>
       </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>212</v>
       </c>
@@ -1297,16 +1258,13 @@
         <v>9</v>
       </c>
       <c r="E35" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F35" t="s">
         <v>8</v>
       </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>217</v>
       </c>
@@ -1320,16 +1278,13 @@
         <v>3</v>
       </c>
       <c r="E36" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F36" t="s">
         <v>8</v>
       </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>218</v>
       </c>
@@ -1343,16 +1298,13 @@
         <v>9</v>
       </c>
       <c r="E37" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F37" t="s">
         <v>8</v>
       </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>219</v>
       </c>
@@ -1366,16 +1318,13 @@
         <v>3</v>
       </c>
       <c r="E38" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F38" t="s">
         <v>8</v>
       </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>220</v>
       </c>
@@ -1389,16 +1338,13 @@
         <v>9</v>
       </c>
       <c r="E39" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F39" t="s">
         <v>8</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>221</v>
       </c>
@@ -1412,16 +1358,13 @@
         <v>3</v>
       </c>
       <c r="E40" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F40" t="s">
         <v>8</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>222</v>
       </c>
@@ -1435,874 +1378,71 @@
         <v>9</v>
       </c>
       <c r="E41" s="1">
-        <v>43754</v>
+        <v>43803</v>
       </c>
       <c r="F41" t="s">
         <v>8</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>3</v>
-      </c>
-      <c r="B42" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42">
-        <v>13</v>
-      </c>
-      <c r="D42" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F42" t="s">
-        <v>8</v>
-      </c>
-      <c r="G42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>4</v>
-      </c>
-      <c r="B43" t="s">
-        <v>7</v>
-      </c>
-      <c r="C43">
-        <v>13</v>
-      </c>
-      <c r="D43" t="s">
-        <v>9</v>
-      </c>
-      <c r="E43" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
-      </c>
-      <c r="G43" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44">
-        <v>13</v>
-      </c>
-      <c r="D44" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F44" t="s">
-        <v>8</v>
-      </c>
-      <c r="G44" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>12</v>
-      </c>
-      <c r="B45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45">
-        <v>13</v>
-      </c>
-      <c r="D45" t="s">
-        <v>9</v>
-      </c>
-      <c r="E45" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F45" t="s">
-        <v>8</v>
-      </c>
-      <c r="G45" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>19</v>
-      </c>
-      <c r="B46" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46">
-        <v>13</v>
-      </c>
-      <c r="D46" t="s">
-        <v>3</v>
-      </c>
-      <c r="E46" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F46" t="s">
-        <v>8</v>
-      </c>
-      <c r="G46" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>20</v>
-      </c>
-      <c r="B47" t="s">
-        <v>7</v>
-      </c>
-      <c r="C47">
-        <v>13</v>
-      </c>
-      <c r="D47" t="s">
-        <v>9</v>
-      </c>
-      <c r="E47" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F47" t="s">
-        <v>8</v>
-      </c>
-      <c r="G47" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>201</v>
-      </c>
-      <c r="B48" t="s">
-        <v>7</v>
-      </c>
-      <c r="C48">
-        <v>13</v>
-      </c>
-      <c r="D48" t="s">
-        <v>3</v>
-      </c>
-      <c r="E48" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F48" t="s">
-        <v>8</v>
-      </c>
-      <c r="G48" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>202</v>
-      </c>
-      <c r="B49" t="s">
-        <v>7</v>
-      </c>
-      <c r="C49">
-        <v>13</v>
-      </c>
-      <c r="D49" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F49" t="s">
-        <v>8</v>
-      </c>
-      <c r="G49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>203</v>
-      </c>
-      <c r="B50" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50">
-        <v>13</v>
-      </c>
-      <c r="D50" t="s">
-        <v>3</v>
-      </c>
-      <c r="E50" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F50" t="s">
-        <v>8</v>
-      </c>
-      <c r="G50" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>204</v>
-      </c>
-      <c r="B51" t="s">
-        <v>7</v>
-      </c>
-      <c r="C51">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>9</v>
-      </c>
-      <c r="E51" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F51" t="s">
-        <v>8</v>
-      </c>
-      <c r="G51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>209</v>
-      </c>
-      <c r="B52" t="s">
-        <v>7</v>
-      </c>
-      <c r="C52">
-        <v>13</v>
-      </c>
-      <c r="D52" t="s">
-        <v>3</v>
-      </c>
-      <c r="E52" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F52" t="s">
-        <v>8</v>
-      </c>
-      <c r="G52" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>210</v>
-      </c>
-      <c r="B53" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53">
-        <v>13</v>
-      </c>
-      <c r="D53" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F53" t="s">
-        <v>8</v>
-      </c>
-      <c r="G53" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>211</v>
-      </c>
-      <c r="B54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C54">
-        <v>13</v>
-      </c>
-      <c r="D54" t="s">
-        <v>3</v>
-      </c>
-      <c r="E54" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F54" t="s">
-        <v>8</v>
-      </c>
-      <c r="G54" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>212</v>
-      </c>
-      <c r="B55" t="s">
-        <v>7</v>
-      </c>
-      <c r="C55">
-        <v>13</v>
-      </c>
-      <c r="D55" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F55" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>217</v>
-      </c>
-      <c r="B56" t="s">
-        <v>7</v>
-      </c>
-      <c r="C56">
-        <v>13</v>
-      </c>
-      <c r="D56" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F56" t="s">
-        <v>8</v>
-      </c>
-      <c r="G56" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>218</v>
-      </c>
-      <c r="B57" t="s">
-        <v>7</v>
-      </c>
-      <c r="C57">
-        <v>13</v>
-      </c>
-      <c r="D57" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F57" t="s">
-        <v>8</v>
-      </c>
-      <c r="G57" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>219</v>
-      </c>
-      <c r="B58" t="s">
-        <v>7</v>
-      </c>
-      <c r="C58">
-        <v>13</v>
-      </c>
-      <c r="D58" t="s">
-        <v>3</v>
-      </c>
-      <c r="E58" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F58" t="s">
-        <v>8</v>
-      </c>
-      <c r="G58" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>220</v>
-      </c>
-      <c r="B59" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59">
-        <v>13</v>
-      </c>
-      <c r="D59" t="s">
-        <v>9</v>
-      </c>
-      <c r="E59" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F59" t="s">
-        <v>8</v>
-      </c>
-      <c r="G59" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>221</v>
-      </c>
-      <c r="B60" t="s">
-        <v>7</v>
-      </c>
-      <c r="C60">
-        <v>13</v>
-      </c>
-      <c r="D60" t="s">
-        <v>3</v>
-      </c>
-      <c r="E60" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F60" t="s">
-        <v>8</v>
-      </c>
-      <c r="G60" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>222</v>
-      </c>
-      <c r="B61" t="s">
-        <v>7</v>
-      </c>
-      <c r="C61">
-        <v>13</v>
-      </c>
-      <c r="D61" t="s">
-        <v>9</v>
-      </c>
-      <c r="E61" s="1">
-        <v>43768</v>
-      </c>
-      <c r="F61" t="s">
-        <v>8</v>
-      </c>
-      <c r="G61" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>3</v>
-      </c>
-      <c r="B62" t="s">
-        <v>7</v>
-      </c>
-      <c r="C62">
-        <v>13</v>
-      </c>
-      <c r="D62" t="s">
-        <v>3</v>
-      </c>
-      <c r="E62" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F62" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>4</v>
-      </c>
-      <c r="B63" t="s">
-        <v>7</v>
-      </c>
-      <c r="C63">
-        <v>13</v>
-      </c>
-      <c r="D63" t="s">
-        <v>9</v>
-      </c>
-      <c r="E63" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F63" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>11</v>
-      </c>
-      <c r="B64" t="s">
-        <v>7</v>
-      </c>
-      <c r="C64">
-        <v>13</v>
-      </c>
-      <c r="D64" t="s">
-        <v>3</v>
-      </c>
-      <c r="E64" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F64" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65">
-        <v>12</v>
-      </c>
-      <c r="B65" t="s">
-        <v>7</v>
-      </c>
-      <c r="C65">
-        <v>13</v>
-      </c>
-      <c r="D65" t="s">
-        <v>9</v>
-      </c>
-      <c r="E65" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F65" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66">
-        <v>19</v>
-      </c>
-      <c r="B66" t="s">
-        <v>7</v>
-      </c>
-      <c r="C66">
-        <v>13</v>
-      </c>
-      <c r="D66" t="s">
-        <v>3</v>
-      </c>
-      <c r="E66" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F66" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67">
-        <v>20</v>
-      </c>
-      <c r="B67" t="s">
-        <v>7</v>
-      </c>
-      <c r="C67">
-        <v>13</v>
-      </c>
-      <c r="D67" t="s">
-        <v>9</v>
-      </c>
-      <c r="E67" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F67" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>201</v>
-      </c>
-      <c r="B68" t="s">
-        <v>7</v>
-      </c>
-      <c r="C68">
-        <v>13</v>
-      </c>
-      <c r="D68" t="s">
-        <v>3</v>
-      </c>
-      <c r="E68" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F68" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>202</v>
-      </c>
-      <c r="B69" t="s">
-        <v>7</v>
-      </c>
-      <c r="C69">
-        <v>13</v>
-      </c>
-      <c r="D69" t="s">
-        <v>9</v>
-      </c>
-      <c r="E69" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F69" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>203</v>
-      </c>
-      <c r="B70" t="s">
-        <v>7</v>
-      </c>
-      <c r="C70">
-        <v>13</v>
-      </c>
-      <c r="D70" t="s">
-        <v>3</v>
-      </c>
-      <c r="E70" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F70" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>204</v>
-      </c>
-      <c r="B71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C71">
-        <v>13</v>
-      </c>
-      <c r="D71" t="s">
-        <v>9</v>
-      </c>
-      <c r="E71" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F71" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72">
-        <v>209</v>
-      </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72">
-        <v>13</v>
-      </c>
-      <c r="D72" t="s">
-        <v>3</v>
-      </c>
-      <c r="E72" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F72" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73">
-        <v>210</v>
-      </c>
-      <c r="B73" t="s">
-        <v>7</v>
-      </c>
-      <c r="C73">
-        <v>13</v>
-      </c>
-      <c r="D73" t="s">
-        <v>9</v>
-      </c>
-      <c r="E73" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F73" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74">
-        <v>211</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74">
-        <v>13</v>
-      </c>
-      <c r="D74" t="s">
-        <v>3</v>
-      </c>
-      <c r="E74" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75">
-        <v>212</v>
-      </c>
-      <c r="B75" t="s">
-        <v>7</v>
-      </c>
-      <c r="C75">
-        <v>13</v>
-      </c>
-      <c r="D75" t="s">
-        <v>9</v>
-      </c>
-      <c r="E75" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F75" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76">
-        <v>217</v>
-      </c>
-      <c r="B76" t="s">
-        <v>7</v>
-      </c>
-      <c r="C76">
-        <v>13</v>
-      </c>
-      <c r="D76" t="s">
-        <v>3</v>
-      </c>
-      <c r="E76" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77">
-        <v>218</v>
-      </c>
-      <c r="B77" t="s">
-        <v>7</v>
-      </c>
-      <c r="C77">
-        <v>13</v>
-      </c>
-      <c r="D77" t="s">
-        <v>9</v>
-      </c>
-      <c r="E77" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F77" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78">
-        <v>219</v>
-      </c>
-      <c r="B78" t="s">
-        <v>7</v>
-      </c>
-      <c r="C78">
-        <v>13</v>
-      </c>
-      <c r="D78" t="s">
-        <v>3</v>
-      </c>
-      <c r="E78" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F78" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79">
-        <v>220</v>
-      </c>
-      <c r="B79" t="s">
-        <v>7</v>
-      </c>
-      <c r="C79">
-        <v>13</v>
-      </c>
-      <c r="D79" t="s">
-        <v>9</v>
-      </c>
-      <c r="E79" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F79" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80">
-        <v>221</v>
-      </c>
-      <c r="B80" t="s">
-        <v>7</v>
-      </c>
-      <c r="C80">
-        <v>13</v>
-      </c>
-      <c r="D80" t="s">
-        <v>3</v>
-      </c>
-      <c r="E80" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F80" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81">
-        <v>222</v>
-      </c>
-      <c r="B81" t="s">
-        <v>7</v>
-      </c>
-      <c r="C81">
-        <v>13</v>
-      </c>
-      <c r="D81" t="s">
-        <v>9</v>
-      </c>
-      <c r="E81" s="1">
-        <v>43803</v>
-      </c>
-      <c r="F81" t="s">
-        <v>8</v>
-      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="1"/>
+    </row>
+    <row r="53" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E53" s="1"/>
+    </row>
+    <row r="54" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E58" s="1"/>
+    </row>
+    <row r="59" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E59" s="1"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E60" s="1"/>
+    </row>
+    <row r="61" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E61" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tape and gel image ext 2025
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D055D96-BA61-F74F-A27B-9BDDD02D30D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EE2740-34F7-2A41-8DA5-4101709BD976}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5960" yWindow="740" windowWidth="27640" windowHeight="17000" activeTab="1" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5960" yWindow="740" windowWidth="27640" windowHeight="17000" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="57">
   <si>
     <t>ColonyID</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>2019-09-16</t>
+  </si>
+  <si>
+    <t>Degraded; but potential here</t>
+  </si>
+  <si>
+    <t>M-209</t>
+  </si>
+  <si>
+    <t>M-4</t>
+  </si>
+  <si>
+    <t>M-217</t>
   </si>
 </sst>
 </file>
@@ -233,7 +245,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -243,6 +255,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -268,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -287,6 +305,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,14 +639,14 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -675,13 +695,16 @@
         <v>3</v>
       </c>
       <c r="F2" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
+      </c>
+      <c r="I2">
+        <v>20210210</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -701,13 +724,16 @@
         <v>9</v>
       </c>
       <c r="F3" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
       <c r="H3" t="s">
         <v>8</v>
+      </c>
+      <c r="I3">
+        <v>20210225</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -727,7 +753,7 @@
         <v>3</v>
       </c>
       <c r="F4" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -753,7 +779,7 @@
         <v>9</v>
       </c>
       <c r="F5" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -779,13 +805,16 @@
         <v>3</v>
       </c>
       <c r="F6" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
+      </c>
+      <c r="I6">
+        <v>20210210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -805,7 +834,7 @@
         <v>9</v>
       </c>
       <c r="F7" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
@@ -831,7 +860,7 @@
         <v>3</v>
       </c>
       <c r="F8" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
@@ -857,13 +886,16 @@
         <v>9</v>
       </c>
       <c r="F9" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
       <c r="H9" t="s">
         <v>8</v>
+      </c>
+      <c r="I9">
+        <v>20210225</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -883,7 +915,7 @@
         <v>3</v>
       </c>
       <c r="F10" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
@@ -909,7 +941,7 @@
         <v>9</v>
       </c>
       <c r="F11" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G11" t="s">
         <v>8</v>
@@ -935,13 +967,16 @@
         <v>3</v>
       </c>
       <c r="F12" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G12" t="s">
         <v>8</v>
       </c>
       <c r="H12" t="s">
         <v>8</v>
+      </c>
+      <c r="I12">
+        <v>20210225</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -961,7 +996,7 @@
         <v>9</v>
       </c>
       <c r="F13" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G13" t="s">
         <v>8</v>
@@ -987,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -1013,7 +1048,7 @@
         <v>9</v>
       </c>
       <c r="F15" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G15" t="s">
         <v>8</v>
@@ -1039,7 +1074,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G16" t="s">
         <v>8</v>
@@ -1065,7 +1100,7 @@
         <v>9</v>
       </c>
       <c r="F17" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G17" t="s">
         <v>8</v>
@@ -1091,7 +1126,7 @@
         <v>3</v>
       </c>
       <c r="F18" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G18" t="s">
         <v>8</v>
@@ -1117,7 +1152,7 @@
         <v>9</v>
       </c>
       <c r="F19" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1143,7 +1178,7 @@
         <v>3</v>
       </c>
       <c r="F20" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1169,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="F21" s="1">
-        <v>43740</v>
+        <v>43768</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
@@ -1205,29 +1240,32 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="A23" s="4">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>13</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="4">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="11">
         <v>43803</v>
       </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" t="s">
-        <v>30</v>
+      <c r="G23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="4">
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1473,7 +1511,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>210</v>
       </c>
@@ -1499,7 +1537,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>211</v>
       </c>
@@ -1525,59 +1563,65 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="4">
         <v>212</v>
       </c>
-      <c r="B35" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35">
-        <v>13</v>
-      </c>
-      <c r="D35">
+      <c r="B35" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="4">
+        <v>13</v>
+      </c>
+      <c r="D35" s="4">
         <v>12</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="1">
+      <c r="F35" s="11">
         <v>43803</v>
       </c>
-      <c r="G35" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36">
+      <c r="G35" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="4">
         <v>217</v>
       </c>
-      <c r="B36" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36">
-        <v>13</v>
-      </c>
-      <c r="D36">
-        <v>13</v>
-      </c>
-      <c r="E36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="1">
+      <c r="B36" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="4">
+        <v>13</v>
+      </c>
+      <c r="D36" s="4">
+        <v>13</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F36" s="11">
         <v>43803</v>
       </c>
-      <c r="G36" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G36" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="4">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>218</v>
       </c>
@@ -1603,7 +1647,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>219</v>
       </c>
@@ -1629,7 +1673,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>220</v>
       </c>
@@ -1655,7 +1699,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>221</v>
       </c>
@@ -1681,7 +1725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>222</v>
       </c>
@@ -1715,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AD3CB-63E2-694C-817E-F91992571833}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,7 +1902,7 @@
         <v>20.2</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H13" si="0">(F3+G3)/2</f>
+        <f t="shared" ref="H3:H19" si="0">(F3+G3)/2</f>
         <v>20.299999999999997</v>
       </c>
       <c r="I3" s="4">
@@ -1868,7 +1912,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K13" si="1">(I3+J3)/2</f>
+        <f t="shared" ref="K3:K19" si="1">(I3+J3)/2</f>
         <v>22</v>
       </c>
       <c r="L3" s="4">
@@ -2081,101 +2125,101 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="8">
-        <v>7</v>
-      </c>
-      <c r="E8" s="8">
+      <c r="C8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <v>7</v>
+      </c>
+      <c r="E8" s="12">
         <v>20210210</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="12">
         <v>17.3</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="12">
         <v>17.2</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="12">
         <f t="shared" si="0"/>
         <v>17.25</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="12">
         <v>31.2</v>
       </c>
-      <c r="J8" s="8">
+      <c r="J8" s="12">
         <v>31</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="12">
         <f t="shared" si="1"/>
         <v>31.1</v>
       </c>
-      <c r="L8" s="8">
+      <c r="L8" s="12">
         <v>6.3</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>45</v>
+      <c r="N8" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8">
-        <v>8</v>
-      </c>
-      <c r="E9" s="8">
+      <c r="C9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="12">
+        <v>8</v>
+      </c>
+      <c r="E9" s="12">
         <v>20210210</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="12">
         <v>20.6</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="12">
         <v>20.6</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="12">
         <f t="shared" si="0"/>
         <v>20.6</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="12">
         <v>22.2</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9" s="12">
         <v>22.2</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="12">
         <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="12">
         <v>7.3</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>45</v>
+      <c r="N9" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="12" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -2374,9 +2418,303 @@
         <v>45</v>
       </c>
     </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="12">
+        <v>13</v>
+      </c>
+      <c r="E14" s="12">
+        <v>20210225</v>
+      </c>
+      <c r="F14" s="12">
+        <v>31.8</v>
+      </c>
+      <c r="G14" s="12">
+        <v>31.6</v>
+      </c>
+      <c r="H14" s="12">
+        <f t="shared" si="0"/>
+        <v>31.700000000000003</v>
+      </c>
+      <c r="I14" s="12">
+        <v>29.2</v>
+      </c>
+      <c r="J14" s="12">
+        <v>29.2</v>
+      </c>
+      <c r="K14" s="12">
+        <f t="shared" si="1"/>
+        <v>29.2</v>
+      </c>
+      <c r="L14" s="12">
+        <v>5</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="8">
+        <v>14</v>
+      </c>
+      <c r="E15" s="8">
+        <v>20210225</v>
+      </c>
+      <c r="F15" s="8">
+        <v>28.2</v>
+      </c>
+      <c r="G15" s="8">
+        <v>28.2</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>28.2</v>
+      </c>
+      <c r="I15" s="8">
+        <v>26</v>
+      </c>
+      <c r="J15" s="8">
+        <v>26</v>
+      </c>
+      <c r="K15" s="8">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="L15" s="8">
+        <v>3.6</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="12">
+        <v>15</v>
+      </c>
+      <c r="E16" s="12">
+        <v>20210225</v>
+      </c>
+      <c r="F16" s="12">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="G16" s="12">
+        <v>18.5</v>
+      </c>
+      <c r="H16" s="12">
+        <f t="shared" si="0"/>
+        <v>18.55</v>
+      </c>
+      <c r="I16" s="12">
+        <v>34</v>
+      </c>
+      <c r="J16" s="12">
+        <v>34</v>
+      </c>
+      <c r="K16" s="12">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="L16" s="12">
+        <v>5</v>
+      </c>
+      <c r="M16" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="4">
+        <v>16</v>
+      </c>
+      <c r="E17" s="4">
+        <v>20210225</v>
+      </c>
+      <c r="F17" s="4">
+        <v>36.6</v>
+      </c>
+      <c r="G17" s="4">
+        <v>36.4</v>
+      </c>
+      <c r="H17" s="4">
+        <f t="shared" si="0"/>
+        <v>36.5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>34</v>
+      </c>
+      <c r="J17" s="4">
+        <v>34</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="L17" s="4">
+        <v>7.7</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N17" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4">
+        <v>17</v>
+      </c>
+      <c r="E18" s="4">
+        <v>20210225</v>
+      </c>
+      <c r="F18" s="4">
+        <v>33</v>
+      </c>
+      <c r="G18" s="4">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="H18" s="4">
+        <f t="shared" si="0"/>
+        <v>32.9</v>
+      </c>
+      <c r="I18" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="J18" s="4">
+        <v>30.8</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="1"/>
+        <v>30.8</v>
+      </c>
+      <c r="L18" s="4">
+        <v>8.5</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="4">
+        <v>18</v>
+      </c>
+      <c r="E19" s="4">
+        <v>20210225</v>
+      </c>
+      <c r="F19" s="4">
+        <v>31.4</v>
+      </c>
+      <c r="G19" s="4">
+        <v>31.2</v>
+      </c>
+      <c r="H19" s="4">
+        <f t="shared" si="0"/>
+        <v>31.299999999999997</v>
+      </c>
+      <c r="I19" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="J19" s="4">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="K19" s="4">
+        <f t="shared" si="1"/>
+        <v>16.399999999999999</v>
+      </c>
+      <c r="L19" s="4">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="N1:N7 N14:N1048576">
+  <conditionalFormatting sqref="N1:N7 N15:N1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
march 3rd extractions for dec 4 2019 frags
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640616E2-E302-4D47-90D2-C5C528F984AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F14FFDA-3C83-334F-ABAA-A70FEC831E22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5960" yWindow="740" windowWidth="27640" windowHeight="17000" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="60">
   <si>
     <t>ColonyID</t>
   </si>
@@ -210,6 +210,15 @@
   </si>
   <si>
     <t>M-217</t>
+  </si>
+  <si>
+    <t>M-210</t>
+  </si>
+  <si>
+    <t>M-20</t>
+  </si>
+  <si>
+    <t>M-220</t>
   </si>
 </sst>
 </file>
@@ -265,7 +274,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -282,13 +291,120 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -304,10 +420,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,8 +778,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -650,1107 +788,1148 @@
     <col min="9" max="9" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="30" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="A2" s="22">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>13</v>
-      </c>
-      <c r="D2">
+      <c r="B2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="14">
+        <v>13</v>
+      </c>
+      <c r="D2" s="14">
         <v>1</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="15">
         <v>43768</v>
       </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2">
+      <c r="G2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="23">
         <v>20210210</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="A3" s="22">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
-      <c r="D3">
+      <c r="B3" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="14">
+        <v>13</v>
+      </c>
+      <c r="D3" s="14">
         <v>1</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="15">
         <v>43768</v>
       </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3">
+      <c r="G3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="23">
         <v>20210225</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="A4" s="22">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="14">
+        <v>13</v>
+      </c>
+      <c r="D4" s="14">
         <v>2</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="15">
         <v>43768</v>
       </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
+      <c r="G4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="23"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="A5" s="22">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="14">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14">
         <v>2</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="15">
         <v>43768</v>
       </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
+      <c r="G5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="23"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="A6" s="22">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>13</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="14">
+        <v>13</v>
+      </c>
+      <c r="D6" s="14">
         <v>3</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="15">
         <v>43768</v>
       </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6">
+      <c r="G6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="23">
         <v>20210210</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="A7" s="22">
         <v>20</v>
       </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
-      <c r="D7">
+      <c r="B7" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="14">
+        <v>13</v>
+      </c>
+      <c r="D7" s="14">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="15">
         <v>43768</v>
       </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
+      <c r="G7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="23"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="A8" s="22">
         <v>201</v>
       </c>
-      <c r="B8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8">
-        <v>13</v>
-      </c>
-      <c r="D8">
+      <c r="B8" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="14">
+        <v>13</v>
+      </c>
+      <c r="D8" s="14">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="15">
         <v>43768</v>
       </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
+      <c r="G8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="23"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="A9" s="22">
         <v>202</v>
       </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9">
-        <v>13</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="14">
+        <v>13</v>
+      </c>
+      <c r="D9" s="14">
         <v>9</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="15">
         <v>43768</v>
       </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9">
+      <c r="G9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="23">
         <v>20210225</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="22">
         <v>203</v>
       </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>13</v>
-      </c>
-      <c r="D10">
+      <c r="B10" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="14">
+        <v>13</v>
+      </c>
+      <c r="D10" s="14">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="15">
         <v>43768</v>
       </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
+      <c r="G10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="23"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="A11" s="22">
         <v>204</v>
       </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11">
-        <v>13</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="14">
+        <v>13</v>
+      </c>
+      <c r="D11" s="14">
         <v>10</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="15">
         <v>43768</v>
       </c>
-      <c r="G11" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
+      <c r="G11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="23"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="A12" s="22">
         <v>209</v>
       </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12">
-        <v>13</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="14">
+        <v>13</v>
+      </c>
+      <c r="D12" s="14">
         <v>11</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="15">
         <v>43768</v>
       </c>
-      <c r="G12" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12">
+      <c r="G12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="23">
         <v>20210225</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="A13" s="22">
         <v>210</v>
       </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="14">
+        <v>13</v>
+      </c>
+      <c r="D13" s="14">
         <v>11</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="15">
         <v>43768</v>
       </c>
-      <c r="G13" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" t="s">
-        <v>8</v>
-      </c>
+      <c r="G13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="23"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="A14" s="22">
         <v>211</v>
       </c>
-      <c r="B14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14">
-        <v>13</v>
-      </c>
-      <c r="D14">
+      <c r="B14" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="14">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14">
         <v>12</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="15">
         <v>43768</v>
       </c>
-      <c r="G14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" t="s">
-        <v>8</v>
-      </c>
+      <c r="G14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="23"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="A15" s="22">
         <v>212</v>
       </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="14">
+        <v>13</v>
+      </c>
+      <c r="D15" s="14">
         <v>12</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="15">
         <v>43768</v>
       </c>
-      <c r="G15" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" t="s">
-        <v>8</v>
-      </c>
+      <c r="G15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="23"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="A16" s="22">
         <v>217</v>
       </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16">
-        <v>13</v>
-      </c>
-      <c r="D16">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="B16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14">
+        <v>13</v>
+      </c>
+      <c r="D16" s="14">
+        <v>13</v>
+      </c>
+      <c r="E16" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="15">
         <v>43768</v>
       </c>
-      <c r="G16" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" t="s">
-        <v>8</v>
-      </c>
+      <c r="G16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="23"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="A17" s="22">
         <v>218</v>
       </c>
-      <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17">
-        <v>13</v>
-      </c>
-      <c r="D17">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="B17" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="14">
+        <v>13</v>
+      </c>
+      <c r="D17" s="14">
+        <v>13</v>
+      </c>
+      <c r="E17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="15">
         <v>43768</v>
       </c>
-      <c r="G17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" t="s">
-        <v>8</v>
-      </c>
+      <c r="G17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="23"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="A18" s="22">
         <v>219</v>
       </c>
-      <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18">
-        <v>13</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="14">
+        <v>13</v>
+      </c>
+      <c r="D18" s="14">
         <v>14</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="15">
         <v>43768</v>
       </c>
-      <c r="G18" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" t="s">
-        <v>8</v>
-      </c>
+      <c r="G18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="A19" s="22">
         <v>220</v>
       </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
-        <v>13</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="14">
+        <v>13</v>
+      </c>
+      <c r="D19" s="14">
         <v>14</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="15">
         <v>43768</v>
       </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" t="s">
-        <v>8</v>
-      </c>
+      <c r="G19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="A20" s="22">
         <v>221</v>
       </c>
-      <c r="B20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20">
-        <v>13</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="14">
+        <v>13</v>
+      </c>
+      <c r="D20" s="14">
         <v>15</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="15">
         <v>43768</v>
       </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" t="s">
-        <v>8</v>
-      </c>
+      <c r="G20" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="A21" s="24">
         <v>222</v>
       </c>
-      <c r="B21" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21">
-        <v>13</v>
-      </c>
-      <c r="D21">
+      <c r="B21" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="25">
+        <v>13</v>
+      </c>
+      <c r="D21" s="25">
         <v>15</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="26">
         <v>43768</v>
       </c>
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" t="s">
-        <v>8</v>
-      </c>
+      <c r="G21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="27"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="A22" s="16">
         <v>3</v>
       </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22">
-        <v>13</v>
-      </c>
-      <c r="D22">
+      <c r="B22" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="17">
+        <v>13</v>
+      </c>
+      <c r="D22" s="17">
         <v>1</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="18">
         <v>43803</v>
       </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" t="s">
-        <v>30</v>
-      </c>
+      <c r="G22" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="4">
+      <c r="A23" s="20">
         <v>4</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="4">
-        <v>13</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="B23" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="12">
+        <v>13</v>
+      </c>
+      <c r="D23" s="12">
         <v>1</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F23" s="11">
+      <c r="F23" s="13">
         <v>43803</v>
       </c>
-      <c r="G23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" s="4">
+      <c r="G23" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I23" s="21">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="4">
+      <c r="A24" s="20">
         <v>11</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="4">
-        <v>13</v>
-      </c>
-      <c r="D24" s="4">
+      <c r="B24" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="12">
+        <v>13</v>
+      </c>
+      <c r="D24" s="12">
         <v>2</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="E24" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="11">
+      <c r="F24" s="13">
         <v>43803</v>
       </c>
-      <c r="G24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" s="4">
+      <c r="G24" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I24" s="21">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="A25" s="22">
         <v>12</v>
       </c>
-      <c r="B25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25">
-        <v>13</v>
-      </c>
-      <c r="D25">
+      <c r="B25" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="14">
+        <v>13</v>
+      </c>
+      <c r="D25" s="14">
         <v>2</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="15">
         <v>43803</v>
       </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" t="s">
-        <v>30</v>
-      </c>
+      <c r="G25" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H25" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="23"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="A26" s="22">
         <v>19</v>
       </c>
-      <c r="B26" t="s">
-        <v>7</v>
-      </c>
-      <c r="C26">
-        <v>13</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="14">
+        <v>13</v>
+      </c>
+      <c r="D26" s="14">
         <v>3</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="1">
+      <c r="F26" s="15">
         <v>43803</v>
       </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" t="s">
-        <v>30</v>
-      </c>
+      <c r="G26" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="A27" s="20">
         <v>20</v>
       </c>
-      <c r="B27" t="s">
-        <v>7</v>
-      </c>
-      <c r="C27">
-        <v>13</v>
-      </c>
-      <c r="D27">
+      <c r="B27" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="12">
+        <v>13</v>
+      </c>
+      <c r="D27" s="12">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="13">
         <v>43803</v>
       </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" t="s">
-        <v>30</v>
+      <c r="G27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="21">
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="4">
+      <c r="A28" s="20">
         <v>201</v>
       </c>
-      <c r="B28" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="4">
-        <v>13</v>
-      </c>
-      <c r="D28" s="4">
+      <c r="B28" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="12">
+        <v>13</v>
+      </c>
+      <c r="D28" s="12">
         <v>9</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F28" s="11">
+      <c r="F28" s="13">
         <v>43803</v>
       </c>
-      <c r="G28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="4">
+      <c r="G28" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="21">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="4">
+      <c r="A29" s="20">
         <v>202</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="4">
-        <v>13</v>
-      </c>
-      <c r="D29" s="4">
+      <c r="B29" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="12">
+        <v>13</v>
+      </c>
+      <c r="D29" s="12">
         <v>9</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F29" s="11">
+      <c r="F29" s="13">
         <v>43803</v>
       </c>
-      <c r="G29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I29" s="4">
+      <c r="G29" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I29" s="21">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="A30" s="22">
         <v>203</v>
       </c>
-      <c r="B30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30">
-        <v>13</v>
-      </c>
-      <c r="D30">
+      <c r="B30" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="14">
+        <v>13</v>
+      </c>
+      <c r="D30" s="14">
         <v>10</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F30" s="15">
         <v>43803</v>
       </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" t="s">
-        <v>30</v>
-      </c>
+      <c r="G30" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="A31" s="22">
         <v>204</v>
       </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31">
-        <v>13</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="14">
+        <v>13</v>
+      </c>
+      <c r="D31" s="14">
         <v>10</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="1">
+      <c r="F31" s="15">
         <v>43803</v>
       </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" t="s">
-        <v>30</v>
-      </c>
+      <c r="G31" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="A32" s="20">
         <v>209</v>
       </c>
-      <c r="B32" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32">
-        <v>13</v>
-      </c>
-      <c r="D32">
+      <c r="B32" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="12">
+        <v>13</v>
+      </c>
+      <c r="D32" s="12">
         <v>11</v>
       </c>
-      <c r="E32" t="s">
+      <c r="E32" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F32" s="1">
+      <c r="F32" s="13">
         <v>43803</v>
       </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" t="s">
-        <v>30</v>
+      <c r="G32" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="21">
+        <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33">
+      <c r="A33" s="20">
         <v>210</v>
       </c>
-      <c r="B33" t="s">
-        <v>7</v>
-      </c>
-      <c r="C33">
-        <v>13</v>
-      </c>
-      <c r="D33">
+      <c r="B33" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C33" s="12">
+        <v>13</v>
+      </c>
+      <c r="D33" s="12">
         <v>11</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="1">
+      <c r="F33" s="13">
         <v>43803</v>
       </c>
-      <c r="G33" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" t="s">
-        <v>30</v>
+      <c r="G33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="21">
+        <v>19</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34">
+      <c r="A34" s="22">
         <v>211</v>
       </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34">
-        <v>13</v>
-      </c>
-      <c r="D34">
+      <c r="B34" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" s="14">
+        <v>13</v>
+      </c>
+      <c r="D34" s="14">
         <v>12</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E34" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="1">
+      <c r="F34" s="15">
         <v>43803</v>
       </c>
-      <c r="G34" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" t="s">
-        <v>30</v>
-      </c>
+      <c r="G34" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="23"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="4">
+      <c r="A35" s="20">
         <v>212</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C35" s="4">
-        <v>13</v>
-      </c>
-      <c r="D35" s="4">
+      <c r="B35" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C35" s="12">
+        <v>13</v>
+      </c>
+      <c r="D35" s="12">
         <v>12</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F35" s="11">
+      <c r="F35" s="13">
         <v>43803</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I35" s="4">
+      <c r="G35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="21">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="4">
+      <c r="A36" s="20">
         <v>217</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="4">
-        <v>13</v>
-      </c>
-      <c r="D36" s="4">
-        <v>13</v>
-      </c>
-      <c r="E36" s="4" t="s">
+      <c r="B36" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="12">
+        <v>13</v>
+      </c>
+      <c r="D36" s="12">
+        <v>13</v>
+      </c>
+      <c r="E36" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F36" s="11">
+      <c r="F36" s="13">
         <v>43803</v>
       </c>
-      <c r="G36" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I36" s="4">
+      <c r="G36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="21">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A37">
+      <c r="A37" s="20">
         <v>218</v>
       </c>
-      <c r="B37" t="s">
-        <v>7</v>
-      </c>
-      <c r="C37">
-        <v>13</v>
-      </c>
-      <c r="D37">
-        <v>13</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="B37" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C37" s="12">
+        <v>13</v>
+      </c>
+      <c r="D37" s="12">
+        <v>13</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="1">
+      <c r="F37" s="13">
         <v>43803</v>
       </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" t="s">
-        <v>30</v>
+      <c r="G37" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="21">
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38">
+      <c r="A38" s="20">
         <v>219</v>
       </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38">
-        <v>13</v>
-      </c>
-      <c r="D38">
+      <c r="B38" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C38" s="12">
+        <v>13</v>
+      </c>
+      <c r="D38" s="12">
         <v>14</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F38" s="13">
         <v>43803</v>
       </c>
-      <c r="G38" t="s">
-        <v>8</v>
-      </c>
-      <c r="H38" t="s">
-        <v>30</v>
+      <c r="G38" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="21">
+        <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39">
+      <c r="A39" s="20">
         <v>220</v>
       </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39">
-        <v>13</v>
-      </c>
-      <c r="D39">
+      <c r="B39" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" s="12">
+        <v>13</v>
+      </c>
+      <c r="D39" s="12">
         <v>14</v>
       </c>
-      <c r="E39" t="s">
+      <c r="E39" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F39" s="1">
+      <c r="F39" s="13">
         <v>43803</v>
       </c>
-      <c r="G39" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" t="s">
-        <v>30</v>
+      <c r="G39" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="21">
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40">
+      <c r="A40" s="22">
         <v>221</v>
       </c>
-      <c r="B40" t="s">
-        <v>7</v>
-      </c>
-      <c r="C40">
-        <v>13</v>
-      </c>
-      <c r="D40">
+      <c r="B40" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C40" s="14">
+        <v>13</v>
+      </c>
+      <c r="D40" s="14">
         <v>15</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E40" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F40" s="15">
         <v>43803</v>
       </c>
-      <c r="G40" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" t="s">
-        <v>30</v>
-      </c>
+      <c r="G40" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H40" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="23"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41">
+      <c r="A41" s="24">
         <v>222</v>
       </c>
-      <c r="B41" t="s">
-        <v>7</v>
-      </c>
-      <c r="C41">
-        <v>13</v>
-      </c>
-      <c r="D41">
+      <c r="B41" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" s="25">
+        <v>13</v>
+      </c>
+      <c r="D41" s="25">
         <v>15</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="1">
+      <c r="F41" s="26">
         <v>43803</v>
       </c>
-      <c r="G41" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" t="s">
-        <v>30</v>
-      </c>
+      <c r="G41" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1760,956 +1939,1238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AD3CB-63E2-694C-817E-F91992571833}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="2" max="3" width="16.6640625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="8" customWidth="1"/>
-    <col min="8" max="8" width="15.83203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15" style="8" customWidth="1"/>
-    <col min="10" max="11" width="15.5" style="8" customWidth="1"/>
-    <col min="12" max="12" width="10" style="8" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="8"/>
-    <col min="14" max="14" width="18.83203125" style="8" customWidth="1"/>
-    <col min="15" max="15" width="41" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="10.83203125" style="7"/>
+    <col min="2" max="3" width="16.6640625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="7" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="15" style="7" customWidth="1"/>
+    <col min="10" max="11" width="15.5" style="7" customWidth="1"/>
+    <col min="12" max="12" width="10" style="7" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="7"/>
+    <col min="14" max="14" width="18.83203125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="41" style="7" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:15" s="9" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="K1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>1</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>20210131</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>5.84</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="7">
         <v>5.78</v>
       </c>
-      <c r="H2" s="8">
+      <c r="H2" s="7">
         <f>(F2+G2)/2</f>
         <v>5.8100000000000005</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="7">
         <v>43.2</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2" s="7">
         <v>43</v>
       </c>
-      <c r="K2" s="8">
+      <c r="K2" s="7">
         <f>(I2+J2)/2</f>
         <v>43.1</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="7">
         <v>3.4</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="M2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="N2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>2</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>20210131</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>20.399999999999999</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>20.2</v>
       </c>
-      <c r="H3" s="4">
-        <f t="shared" ref="H3:H19" si="0">(F3+G3)/2</f>
+      <c r="H3" s="3">
+        <f t="shared" ref="H3:H25" si="0">(F3+G3)/2</f>
         <v>20.299999999999997</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>22</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>22</v>
       </c>
-      <c r="K3" s="4">
-        <f t="shared" ref="K3:K19" si="1">(I3+J3)/2</f>
+      <c r="K3" s="3">
+        <f t="shared" ref="K3:K25" si="1">(I3+J3)/2</f>
         <v>22</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="3">
         <v>8.5</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>3</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>20210131</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>7.06</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="7">
         <v>7.04</v>
       </c>
-      <c r="H4" s="8">
+      <c r="H4" s="7">
         <f t="shared" si="0"/>
         <v>7.05</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="7">
         <v>66.400000000000006</v>
       </c>
-      <c r="J4" s="8">
+      <c r="J4" s="7">
         <v>66.400000000000006</v>
       </c>
-      <c r="K4" s="8">
+      <c r="K4" s="7">
         <f t="shared" si="1"/>
         <v>66.400000000000006</v>
       </c>
-      <c r="L4" s="8">
+      <c r="L4" s="7">
         <v>2.6</v>
       </c>
-      <c r="M4" s="8" t="s">
+      <c r="M4" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="8" t="s">
+      <c r="N4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>4</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>20210131</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>14.7</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>14.6</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <f t="shared" si="0"/>
         <v>14.649999999999999</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>21.4</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>21.4</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f t="shared" si="1"/>
         <v>21.4</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>8.6</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O5" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>5</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>20210131</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>57.8</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>57.6</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>57.7</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="7">
         <v>36.6</v>
       </c>
-      <c r="J6" s="8">
+      <c r="J6" s="7">
         <v>36.6</v>
       </c>
-      <c r="K6" s="8">
+      <c r="K6" s="7">
         <f t="shared" si="1"/>
         <v>36.6</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="7">
         <v>6</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O6" s="8" t="s">
+      <c r="N6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>6</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>20210131</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>24.6</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>24.4</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>21.4</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>21.2</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="1"/>
         <v>21.299999999999997</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>8.1999999999999993</v>
       </c>
-      <c r="M7" s="4" t="s">
+      <c r="M7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N7" s="4" t="s">
+      <c r="N7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="4" t="s">
+      <c r="O7" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="12">
-        <v>7</v>
-      </c>
-      <c r="E8" s="12">
+      <c r="D8" s="10">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10">
         <v>20210210</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>17.3</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>17.2</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <f t="shared" si="0"/>
         <v>17.25</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <v>31.2</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="10">
         <v>31</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="10">
         <f t="shared" si="1"/>
         <v>31.1</v>
       </c>
-      <c r="L8" s="12">
+      <c r="L8" s="10">
         <v>6.3</v>
       </c>
-      <c r="M8" s="12" t="s">
+      <c r="M8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O8" s="12" t="s">
+      <c r="N8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="12">
-        <v>8</v>
-      </c>
-      <c r="E9" s="12">
+      <c r="D9" s="10">
+        <v>8</v>
+      </c>
+      <c r="E9" s="10">
         <v>20210210</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="10">
         <v>20.6</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="10">
         <v>20.6</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="10">
         <f t="shared" si="0"/>
         <v>20.6</v>
       </c>
-      <c r="I9" s="12">
+      <c r="I9" s="10">
         <v>22.2</v>
       </c>
-      <c r="J9" s="12">
+      <c r="J9" s="10">
         <v>22.2</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="10">
         <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
-      <c r="L9" s="12">
+      <c r="L9" s="10">
         <v>7.3</v>
       </c>
-      <c r="M9" s="12" t="s">
+      <c r="M9" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N9" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O9" s="12" t="s">
+      <c r="N9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="7">
         <v>9</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="7">
         <v>20210210</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="7">
         <v>8.08</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="7">
         <v>8.02</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="7">
         <f t="shared" si="0"/>
         <v>8.0500000000000007</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="7">
         <v>45.6</v>
       </c>
-      <c r="J10" s="8">
+      <c r="J10" s="7">
         <v>45.6</v>
       </c>
-      <c r="K10" s="8">
+      <c r="K10" s="7">
         <f t="shared" si="1"/>
         <v>45.6</v>
       </c>
-      <c r="L10" s="8">
+      <c r="L10" s="7">
         <v>2.9</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O10" s="8" t="s">
+      <c r="N10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="7">
         <v>10</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="7">
         <v>20210210</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
         <v>6.78</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="7">
         <v>6.76</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="7">
         <f t="shared" si="0"/>
         <v>6.77</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="7">
         <v>15.3</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11" s="7">
         <v>15.3</v>
       </c>
-      <c r="K11" s="8">
+      <c r="K11" s="7">
         <f t="shared" si="1"/>
         <v>15.3</v>
       </c>
-      <c r="L11" s="8">
+      <c r="L11" s="7">
         <v>3.2</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N11" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O11" s="8" t="s">
+      <c r="N11" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="7">
         <v>11</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="7">
         <v>20210210</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12" s="7">
         <v>4.4800000000000004</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
         <v>4.4400000000000004</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="7">
         <f t="shared" si="0"/>
         <v>4.4600000000000009</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="7">
         <v>54</v>
       </c>
-      <c r="J12" s="8">
+      <c r="J12" s="7">
         <v>53.8</v>
       </c>
-      <c r="K12" s="8">
+      <c r="K12" s="7">
         <f t="shared" si="1"/>
         <v>53.9</v>
       </c>
-      <c r="L12" s="8">
+      <c r="L12" s="7">
         <v>3.2</v>
       </c>
-      <c r="M12" s="8" t="s">
+      <c r="M12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N12" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O12" s="8" t="s">
+      <c r="N12" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="7">
         <v>12</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="7">
         <v>20210210</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="7">
         <v>21</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="7">
         <v>21</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="7">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="7">
         <v>37.799999999999997</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="7">
         <v>37.799999999999997</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="7">
         <f t="shared" si="1"/>
         <v>37.799999999999997</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="7">
         <v>5.3</v>
       </c>
-      <c r="M13" s="8" t="s">
+      <c r="M13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O13" s="8" t="s">
+      <c r="N13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O13" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="12">
-        <v>13</v>
-      </c>
-      <c r="E14" s="12">
+      <c r="D14" s="10">
+        <v>13</v>
+      </c>
+      <c r="E14" s="10">
         <v>20210225</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="10">
         <v>31.8</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="10">
         <v>31.6</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="10">
         <f t="shared" si="0"/>
         <v>31.700000000000003</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="10">
         <v>29.2</v>
       </c>
-      <c r="J14" s="12">
+      <c r="J14" s="10">
         <v>29.2</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="10">
         <f t="shared" si="1"/>
         <v>29.2</v>
       </c>
-      <c r="L14" s="12">
+      <c r="L14" s="10">
         <v>5</v>
       </c>
-      <c r="M14" s="12" t="s">
+      <c r="M14" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N14" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O14" s="12" t="s">
+      <c r="N14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O14" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="7">
         <v>14</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="7">
         <v>20210225</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="7">
         <v>28.2</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="7">
         <v>28.2</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="7">
         <f t="shared" si="0"/>
         <v>28.2</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="7">
         <v>26</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15" s="7">
         <v>26</v>
       </c>
-      <c r="K15" s="8">
+      <c r="K15" s="7">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="L15" s="8">
+      <c r="L15" s="7">
         <v>3.6</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="N15" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="O15" s="8" t="s">
+      <c r="N15" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="7" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="10">
         <v>15</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="10">
         <v>20210225</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="10">
         <v>18.600000000000001</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="10">
         <v>18.5</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H16" s="10">
         <f t="shared" si="0"/>
         <v>18.55</v>
       </c>
-      <c r="I16" s="12">
+      <c r="I16" s="10">
         <v>34</v>
       </c>
-      <c r="J16" s="12">
+      <c r="J16" s="10">
         <v>34</v>
       </c>
-      <c r="K16" s="12">
+      <c r="K16" s="10">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="L16" s="12">
+      <c r="L16" s="10">
         <v>5</v>
       </c>
-      <c r="M16" s="12" t="s">
+      <c r="M16" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="N16" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O16" s="12" t="s">
+      <c r="N16" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="10" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>16</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>20210225</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>36.6</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>36.4</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>34</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>34</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <v>7.7</v>
       </c>
-      <c r="M17" s="4" t="s">
+      <c r="M17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N17" s="4" t="s">
+      <c r="N17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="4" t="s">
+      <c r="O17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="3">
         <v>17</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>20210225</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <v>33</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>32.799999999999997</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="3">
         <f t="shared" si="0"/>
         <v>32.9</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="3">
         <v>30.8</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="3">
         <v>30.8</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <f t="shared" si="1"/>
         <v>30.8</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="3">
         <v>8.5</v>
       </c>
-      <c r="M18" s="4" t="s">
+      <c r="M18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N18" s="4" t="s">
+      <c r="N18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O18" s="4" t="s">
+      <c r="O18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D19" s="4">
+      <c r="D19" s="3">
         <v>18</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>20210225</v>
       </c>
-      <c r="F19" s="4">
+      <c r="F19" s="3">
         <v>31.4</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>31.2</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="3">
         <f t="shared" si="0"/>
         <v>31.299999999999997</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="3">
         <v>16.399999999999999</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <f t="shared" si="1"/>
         <v>16.399999999999999</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="3">
         <v>8.6999999999999993</v>
       </c>
-      <c r="M19" s="4" t="s">
+      <c r="M19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="N19" s="4" t="s">
+      <c r="N19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O19" s="4" t="s">
+      <c r="O19" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="3">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F20" s="3">
+        <v>58.4</v>
+      </c>
+      <c r="G20" s="3">
+        <v>58.2</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>58.3</v>
+      </c>
+      <c r="I20" s="3">
+        <v>30</v>
+      </c>
+      <c r="J20" s="3">
+        <v>30.2</v>
+      </c>
+      <c r="K20" s="3">
+        <f t="shared" si="1"/>
+        <v>30.1</v>
+      </c>
+      <c r="L20" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O20" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" s="3">
+        <v>20</v>
+      </c>
+      <c r="E21" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F21" s="3">
+        <v>64</v>
+      </c>
+      <c r="G21" s="3">
+        <v>63.8</v>
+      </c>
+      <c r="H21" s="3">
+        <f t="shared" si="0"/>
+        <v>63.9</v>
+      </c>
+      <c r="I21" s="3">
+        <v>48.8</v>
+      </c>
+      <c r="J21" s="3">
+        <v>48.8</v>
+      </c>
+      <c r="K21" s="3">
+        <f t="shared" si="1"/>
+        <v>48.8</v>
+      </c>
+      <c r="L21" s="3">
+        <v>7.4</v>
+      </c>
+      <c r="M21" s="3"/>
+      <c r="N21" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O21" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="3">
+        <v>21</v>
+      </c>
+      <c r="E22" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F22" s="3">
+        <v>54.6</v>
+      </c>
+      <c r="G22" s="3">
+        <v>54.4</v>
+      </c>
+      <c r="H22" s="3">
+        <f t="shared" si="0"/>
+        <v>54.5</v>
+      </c>
+      <c r="I22" s="3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J22" s="3">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="K22" s="3">
+        <f t="shared" si="1"/>
+        <v>36.799999999999997</v>
+      </c>
+      <c r="L22" s="3">
+        <v>8.1</v>
+      </c>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O22" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3">
+        <v>22</v>
+      </c>
+      <c r="E23" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F23" s="3">
+        <v>51.2</v>
+      </c>
+      <c r="G23" s="3">
+        <v>51</v>
+      </c>
+      <c r="H23" s="3">
+        <f t="shared" si="0"/>
+        <v>51.1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="J23" s="3">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="K23" s="3">
+        <f t="shared" si="1"/>
+        <v>37.799999999999997</v>
+      </c>
+      <c r="L23" s="3">
+        <v>8.5</v>
+      </c>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D24" s="3">
+        <v>23</v>
+      </c>
+      <c r="E24" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F24" s="3">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="G24" s="3">
+        <v>35.6</v>
+      </c>
+      <c r="H24" s="3">
+        <f t="shared" si="0"/>
+        <v>35.700000000000003</v>
+      </c>
+      <c r="I24" s="3">
+        <v>30</v>
+      </c>
+      <c r="J24" s="3">
+        <v>30</v>
+      </c>
+      <c r="K24" s="3">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="L24" s="3">
+        <v>9.1</v>
+      </c>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O24" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="3">
+        <v>24</v>
+      </c>
+      <c r="E25" s="3">
+        <v>20210303</v>
+      </c>
+      <c r="F25" s="3">
+        <v>69</v>
+      </c>
+      <c r="G25" s="3">
+        <v>68.8</v>
+      </c>
+      <c r="H25" s="3">
+        <f t="shared" si="0"/>
+        <v>68.900000000000006</v>
+      </c>
+      <c r="I25" s="3">
+        <v>44.8</v>
+      </c>
+      <c r="J25" s="3">
+        <v>44.8</v>
+      </c>
+      <c r="K25" s="3">
+        <f t="shared" si="1"/>
+        <v>44.8</v>
+      </c>
+      <c r="L25" s="3">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="M25" s="3"/>
+      <c r="N25" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O25" s="3" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2727,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4509281-ADDB-3047-892C-1B7433A9593A}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2739,10 +3200,10 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
+    <col min="6" max="6" width="16" style="33" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2755,140 +3216,266 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>2</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>20210131</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>22</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="32">
         <f>500/E2</f>
         <v>22.727272727272727</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>4</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>20210131</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>21.4</v>
       </c>
-      <c r="F3" s="14">
+      <c r="F3" s="32">
         <f t="shared" ref="F3:F6" si="0">500/E3</f>
         <v>23.364485981308412</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>6</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>20210131</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>21.299999999999997</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="32">
         <f t="shared" si="0"/>
         <v>23.474178403755872</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>16</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>20210225</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>34</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="32">
         <f t="shared" si="0"/>
         <v>14.705882352941176</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>17</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>20210225</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>30.8</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="32">
         <f t="shared" si="0"/>
         <v>16.233766233766232</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>18</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="7">
         <v>20210225</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>16.399999999999999</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="32">
         <f>500/E7</f>
         <v>30.487804878048784</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E8" s="7">
+        <v>30.1</v>
+      </c>
+      <c r="F8" s="32">
+        <f>500/E8</f>
+        <v>16.611295681063122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E9" s="7">
+        <v>48.8</v>
+      </c>
+      <c r="F9" s="32">
+        <f>500/E9</f>
+        <v>10.245901639344263</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="7">
+        <v>21</v>
+      </c>
+      <c r="D10" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E10" s="7">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F10" s="32">
+        <f>500/E10</f>
+        <v>13.586956521739131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E11" s="7">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F11" s="32">
+        <f>500/E11</f>
+        <v>13.227513227513228</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7">
+        <v>23</v>
+      </c>
+      <c r="D12" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E12" s="7">
+        <v>30</v>
+      </c>
+      <c r="F12" s="32">
+        <f>500/E12</f>
+        <v>16.666666666666668</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="7">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E13" s="7">
+        <v>44.8</v>
+      </c>
+      <c r="F13" s="32">
+        <f>500/E13</f>
+        <v>11.160714285714286</v>
       </c>
     </row>
   </sheetData>
@@ -2899,10 +3486,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5632F44-864C-D14F-B6F0-4FB922CD9C04}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2930,23 +3517,227 @@
       <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="F1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="7">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7">
+        <v>20210131</v>
+      </c>
+      <c r="E2" s="7">
+        <v>20.299999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7">
+        <v>4</v>
+      </c>
+      <c r="D3" s="7">
+        <v>20210131</v>
+      </c>
+      <c r="E3" s="7">
+        <v>14.649999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7">
+        <v>20210131</v>
+      </c>
+      <c r="E4" s="7">
+        <v>24.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="7">
+        <v>16</v>
+      </c>
+      <c r="D5" s="7">
+        <v>20210225</v>
+      </c>
+      <c r="E5" s="7">
+        <v>36.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="7">
+        <v>17</v>
+      </c>
+      <c r="D6" s="7">
+        <v>20210225</v>
+      </c>
+      <c r="E6" s="7">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="7">
+        <v>18</v>
+      </c>
+      <c r="D7" s="7">
+        <v>20210225</v>
+      </c>
+      <c r="E7" s="7">
+        <v>31.299999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="7">
+        <v>19</v>
+      </c>
+      <c r="D8" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E8" s="7">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="7">
+        <v>20</v>
+      </c>
+      <c r="D9" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E9" s="7">
+        <v>63.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="7">
+        <v>21</v>
+      </c>
+      <c r="D10" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E10" s="7">
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7">
+        <v>22</v>
+      </c>
+      <c r="D11" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E11" s="7">
+        <v>51.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="7">
+        <v>23</v>
+      </c>
+      <c r="D12" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E12" s="7">
+        <v>35.700000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="7">
+        <v>24</v>
+      </c>
+      <c r="D13" s="7">
+        <v>20210303</v>
+      </c>
+      <c r="E13" s="7">
+        <v>68.900000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final dec 4 2019 ext info
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16487DA-C1A4-594F-A1DB-6A2AB5F7FBE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25BE1FD-F10A-154D-9514-7C50A41C1C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28020" windowHeight="18860" activeTab="1" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28020" windowHeight="18860" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="66">
   <si>
     <t>ColonyID</t>
   </si>
@@ -421,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -444,17 +444,12 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -464,15 +459,31 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -800,8 +811,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -811,613 +822,325 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="29" t="s">
+      <c r="H1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="25" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="22">
+      <c r="A2" s="18"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="19"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="18"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="18"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="18"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="18"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="19"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="18"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="19"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="18"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="19"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="18"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="19"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="18"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="19"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="18"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="18"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="19"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="19"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="18"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="19"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="18"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="19"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="18"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="19"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="18"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="19"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="18"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="19"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="18"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="14"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="19"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="18"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="19"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="15">
+        <v>43662</v>
+      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="22"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="29">
         <v>3</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B22" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C22" s="30">
         <v>13</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D22" s="30">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E22" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G2" s="14" t="s">
+      <c r="F22" s="31">
+        <v>43803</v>
+      </c>
+      <c r="G22" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="23">
-        <v>20210210</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="22">
-        <v>4</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="14">
-        <v>13</v>
-      </c>
-      <c r="D3" s="14">
-        <v>1</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" s="23">
-        <v>20210225</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="22">
-        <v>11</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="14">
-        <v>13</v>
-      </c>
-      <c r="D4" s="14">
-        <v>2</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" s="23"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="22">
-        <v>12</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="14">
-        <v>13</v>
-      </c>
-      <c r="D5" s="14">
-        <v>2</v>
-      </c>
-      <c r="E5" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" s="23"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="22">
-        <v>19</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="14">
-        <v>13</v>
-      </c>
-      <c r="D6" s="14">
-        <v>3</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" s="23">
-        <v>20210210</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="22">
-        <v>20</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="14">
-        <v>13</v>
-      </c>
-      <c r="D7" s="14">
-        <v>3</v>
-      </c>
-      <c r="E7" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="22">
-        <v>201</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="14">
-        <v>13</v>
-      </c>
-      <c r="D8" s="14">
-        <v>9</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F8" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" s="23"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="22">
-        <v>202</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="14">
-        <v>13</v>
-      </c>
-      <c r="D9" s="14">
-        <v>9</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" s="23">
-        <v>20210225</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="22">
-        <v>203</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="14">
-        <v>13</v>
-      </c>
-      <c r="D10" s="14">
-        <v>10</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="23"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="22">
-        <v>204</v>
-      </c>
-      <c r="B11" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="14">
-        <v>13</v>
-      </c>
-      <c r="D11" s="14">
-        <v>10</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F11" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I11" s="23"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="22">
-        <v>209</v>
-      </c>
-      <c r="B12" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" s="14">
-        <v>13</v>
-      </c>
-      <c r="D12" s="14">
-        <v>11</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F12" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I12" s="23">
-        <v>20210225</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="22">
-        <v>210</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="14">
-        <v>13</v>
-      </c>
-      <c r="D13" s="14">
-        <v>11</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I13" s="23"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="22">
-        <v>211</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="14">
-        <v>13</v>
-      </c>
-      <c r="D14" s="14">
-        <v>12</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F14" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I14" s="23"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="22">
-        <v>212</v>
-      </c>
-      <c r="B15" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="14">
-        <v>13</v>
-      </c>
-      <c r="D15" s="14">
-        <v>12</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F15" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H15" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I15" s="23"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="22">
-        <v>217</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="14">
-        <v>13</v>
-      </c>
-      <c r="D16" s="14">
-        <v>13</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F16" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H16" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="22">
-        <v>218</v>
-      </c>
-      <c r="B17" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="14">
-        <v>13</v>
-      </c>
-      <c r="D17" s="14">
-        <v>13</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F17" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G17" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I17" s="23"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="22">
-        <v>219</v>
-      </c>
-      <c r="B18" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C18" s="14">
-        <v>13</v>
-      </c>
-      <c r="D18" s="14">
-        <v>14</v>
-      </c>
-      <c r="E18" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="22">
-        <v>220</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="14">
-        <v>13</v>
-      </c>
-      <c r="D19" s="14">
-        <v>14</v>
-      </c>
-      <c r="E19" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="22">
-        <v>221</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="14">
-        <v>13</v>
-      </c>
-      <c r="D20" s="14">
-        <v>15</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F20" s="15">
-        <v>43768</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="I20" s="23"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="24">
-        <v>222</v>
-      </c>
-      <c r="B21" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C21" s="25">
-        <v>13</v>
-      </c>
-      <c r="D21" s="25">
-        <v>15</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="F21" s="26">
-        <v>43768</v>
-      </c>
-      <c r="G21" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="25" t="s">
-        <v>8</v>
-      </c>
-      <c r="I21" s="27"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="16">
-        <v>3</v>
-      </c>
-      <c r="B22" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="17">
-        <v>13</v>
-      </c>
-      <c r="D22" s="17">
-        <v>1</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="18">
-        <v>43803</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="19"/>
+      <c r="H22" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="32">
+        <v>35</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="20">
+      <c r="A23" s="16">
         <v>4</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -1441,12 +1164,12 @@
       <c r="H23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="21">
+      <c r="I23" s="17">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="20">
+      <c r="A24" s="16">
         <v>11</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -1470,66 +1193,70 @@
       <c r="H24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="21">
+      <c r="I24" s="17">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="22">
+      <c r="A25" s="16">
         <v>12</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="14">
+      <c r="C25" s="12">
         <v>13</v>
       </c>
-      <c r="D25" s="14">
+      <c r="D25" s="12">
         <v>2</v>
       </c>
-      <c r="E25" s="14" t="s">
+      <c r="E25" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F25" s="15">
+      <c r="F25" s="13">
         <v>43803</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H25" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" s="23"/>
+      <c r="H25" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="17">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+      <c r="A26" s="16">
         <v>19</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="12">
         <v>13</v>
       </c>
-      <c r="D26" s="14">
+      <c r="D26" s="12">
         <v>3</v>
       </c>
-      <c r="E26" s="14" t="s">
+      <c r="E26" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F26" s="15">
+      <c r="F26" s="13">
         <v>43803</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="G26" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" s="23"/>
+      <c r="H26" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="17">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="20">
+      <c r="A27" s="16">
         <v>20</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -1553,12 +1280,12 @@
       <c r="H27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="21">
+      <c r="I27" s="17">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="20">
+      <c r="A28" s="16">
         <v>201</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1582,12 +1309,12 @@
       <c r="H28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="21">
+      <c r="I28" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="20">
+      <c r="A29" s="16">
         <v>202</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1611,66 +1338,70 @@
       <c r="H29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="21">
+      <c r="I29" s="17">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="22">
+      <c r="A30" s="16">
         <v>203</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="12">
         <v>13</v>
       </c>
-      <c r="D30" s="14">
+      <c r="D30" s="12">
         <v>10</v>
       </c>
-      <c r="E30" s="14" t="s">
+      <c r="E30" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F30" s="15">
+      <c r="F30" s="13">
         <v>43803</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H30" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I30" s="23"/>
+      <c r="H30" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I30" s="17">
+        <v>31</v>
+      </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="22">
+      <c r="A31" s="16">
         <v>204</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="12">
         <v>13</v>
       </c>
-      <c r="D31" s="14">
+      <c r="D31" s="12">
         <v>10</v>
       </c>
-      <c r="E31" s="14" t="s">
+      <c r="E31" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F31" s="13">
         <v>43803</v>
       </c>
-      <c r="G31" s="14" t="s">
+      <c r="G31" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H31" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I31" s="23"/>
+      <c r="H31" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I31" s="17">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="20">
+      <c r="A32" s="16">
         <v>209</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -1694,66 +1425,70 @@
       <c r="H32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="21">
+      <c r="I32" s="17">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="34">
+      <c r="A33" s="16">
         <v>210</v>
       </c>
-      <c r="B33" s="35" t="s">
+      <c r="B33" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="35">
+      <c r="C33" s="12">
         <v>13</v>
       </c>
-      <c r="D33" s="35">
+      <c r="D33" s="12">
         <v>11</v>
       </c>
-      <c r="E33" s="35" t="s">
+      <c r="E33" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F33" s="36">
+      <c r="F33" s="13">
         <v>43803</v>
       </c>
-      <c r="G33" s="35" t="s">
+      <c r="G33" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H33" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="I33" s="37"/>
+      <c r="H33" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="17">
+        <v>34</v>
+      </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="22">
+      <c r="A34" s="16">
         <v>211</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C34" s="12">
         <v>13</v>
       </c>
-      <c r="D34" s="14">
+      <c r="D34" s="12">
         <v>12</v>
       </c>
-      <c r="E34" s="14" t="s">
+      <c r="E34" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F34" s="15">
+      <c r="F34" s="13">
         <v>43803</v>
       </c>
-      <c r="G34" s="14" t="s">
+      <c r="G34" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I34" s="23"/>
+      <c r="H34" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="17">
+        <v>32</v>
+      </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="20">
+      <c r="A35" s="16">
         <v>212</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -1777,12 +1512,12 @@
       <c r="H35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="21">
+      <c r="I35" s="17">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="20">
+      <c r="A36" s="16">
         <v>217</v>
       </c>
       <c r="B36" s="12" t="s">
@@ -1806,39 +1541,41 @@
       <c r="H36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="21">
+      <c r="I36" s="17">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="34">
+      <c r="A37" s="16">
         <v>218</v>
       </c>
-      <c r="B37" s="35" t="s">
+      <c r="B37" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="35">
+      <c r="C37" s="12">
         <v>13</v>
       </c>
-      <c r="D37" s="35">
+      <c r="D37" s="12">
         <v>13</v>
       </c>
-      <c r="E37" s="35" t="s">
+      <c r="E37" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="F37" s="36">
+      <c r="F37" s="13">
         <v>43803</v>
       </c>
-      <c r="G37" s="35" t="s">
+      <c r="G37" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H37" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="I37" s="37"/>
+      <c r="H37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="17">
+        <v>33</v>
+      </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="20">
+      <c r="A38" s="16">
         <v>219</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -1862,12 +1599,12 @@
       <c r="H38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="21">
+      <c r="I38" s="17">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="20">
+      <c r="A39" s="16">
         <v>220</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -1891,63 +1628,67 @@
       <c r="H39" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="21">
+      <c r="I39" s="17">
         <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="22">
+      <c r="A40" s="16">
         <v>221</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="12">
         <v>13</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="12">
         <v>15</v>
       </c>
-      <c r="E40" s="14" t="s">
+      <c r="E40" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="F40" s="15">
+      <c r="F40" s="13">
         <v>43803</v>
       </c>
-      <c r="G40" s="14" t="s">
+      <c r="G40" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="H40" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I40" s="23"/>
+      <c r="H40" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="I40" s="17">
+        <v>28</v>
+      </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="24">
+      <c r="A41" s="33">
         <v>222</v>
       </c>
-      <c r="B41" s="25" t="s">
+      <c r="B41" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="25">
+      <c r="C41" s="34">
         <v>13</v>
       </c>
-      <c r="D41" s="25">
+      <c r="D41" s="34">
         <v>15</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="34" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="26">
+      <c r="F41" s="35">
         <v>43803</v>
       </c>
-      <c r="G41" s="25" t="s">
+      <c r="G41" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="H41" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="27"/>
+      <c r="H41" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="36">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1957,10 +1698,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AD3CB-63E2-694C-817E-F91992571833}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2100,7 +1841,7 @@
         <v>20.2</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H33" si="0">(F3+G3)/2</f>
+        <f t="shared" ref="H3:H36" si="0">(F3+G3)/2</f>
         <v>20.299999999999997</v>
       </c>
       <c r="I3" s="3">
@@ -2110,7 +1851,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K33" si="1">(I3+J3)/2</f>
+        <f t="shared" ref="K3:K36" si="1">(I3+J3)/2</f>
         <v>22</v>
       </c>
       <c r="L3" s="3">
@@ -3243,50 +2984,58 @@
       <c r="L26" s="3">
         <v>7.3</v>
       </c>
-      <c r="M26" s="3"/>
+      <c r="M26" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="N26" s="3" t="s">
         <v>41</v>
       </c>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="7" t="s">
+    <row r="27" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B27" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="B27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="3">
         <v>26</v>
       </c>
-      <c r="E27" s="7">
+      <c r="E27" s="3">
         <v>20210305</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="3">
         <v>46.2</v>
       </c>
-      <c r="G27" s="7">
+      <c r="G27" s="3">
         <v>45.8</v>
       </c>
-      <c r="H27" s="7">
+      <c r="H27" s="3">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="3">
         <v>28.8</v>
       </c>
-      <c r="J27" s="7">
+      <c r="J27" s="3">
         <v>28.6</v>
       </c>
-      <c r="K27" s="7">
+      <c r="K27" s="3">
         <f t="shared" si="1"/>
         <v>28.700000000000003</v>
       </c>
-      <c r="L27" s="7">
+      <c r="L27" s="3">
         <v>6.8</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N27" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -3328,6 +3077,9 @@
       <c r="L28" s="7" t="s">
         <v>30</v>
       </c>
+      <c r="M28" s="7" t="s">
+        <v>41</v>
+      </c>
       <c r="N28" s="7" t="s">
         <v>42</v>
       </c>
@@ -3335,211 +3087,384 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="7" t="s">
+    <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="8" t="s">
+      <c r="B29" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="3">
         <v>28</v>
       </c>
-      <c r="E29" s="7">
+      <c r="E29" s="3">
         <v>20210305</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="3">
         <v>30.4</v>
       </c>
-      <c r="G29" s="7">
+      <c r="G29" s="3">
         <v>30.8</v>
       </c>
-      <c r="H29" s="7">
+      <c r="H29" s="3">
         <f t="shared" si="0"/>
         <v>30.6</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="3">
         <v>30.8</v>
       </c>
-      <c r="J29" s="7">
+      <c r="J29" s="3">
         <v>30.6</v>
       </c>
-      <c r="K29" s="7">
+      <c r="K29" s="3">
         <f t="shared" si="1"/>
         <v>30.700000000000003</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="3">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="7" t="s">
+      <c r="M29" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B30" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" s="8" t="s">
+      <c r="B30" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="3">
         <v>29</v>
       </c>
-      <c r="E30" s="7">
+      <c r="E30" s="3">
         <v>20210305</v>
       </c>
-      <c r="F30" s="7">
+      <c r="F30" s="3">
         <v>64.2</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="3">
         <v>63.4</v>
       </c>
-      <c r="H30" s="7">
+      <c r="H30" s="3">
         <f t="shared" si="0"/>
         <v>63.8</v>
       </c>
-      <c r="I30" s="7">
+      <c r="I30" s="3">
         <v>51.6</v>
       </c>
-      <c r="J30" s="7">
+      <c r="J30" s="3">
         <v>51.2</v>
       </c>
-      <c r="K30" s="7">
+      <c r="K30" s="3">
         <f t="shared" si="1"/>
         <v>51.400000000000006</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="3">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="7" t="s">
+      <c r="M30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C31" s="8" t="s">
+      <c r="B31" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D31" s="7">
-        <v>30</v>
-      </c>
-      <c r="E31" s="7">
+      <c r="D31" s="3">
+        <v>30</v>
+      </c>
+      <c r="E31" s="3">
         <v>20210305</v>
       </c>
-      <c r="F31" s="7">
+      <c r="F31" s="3">
         <v>37.6</v>
       </c>
-      <c r="G31" s="7">
+      <c r="G31" s="3">
         <v>37.4</v>
       </c>
-      <c r="H31" s="7">
+      <c r="H31" s="3">
         <f t="shared" si="0"/>
         <v>37.5</v>
       </c>
-      <c r="I31" s="7">
+      <c r="I31" s="3">
         <v>31.8</v>
       </c>
-      <c r="J31" s="7">
+      <c r="J31" s="3">
         <v>31.6</v>
       </c>
-      <c r="K31" s="7">
+      <c r="K31" s="3">
         <f t="shared" si="1"/>
         <v>31.700000000000003</v>
       </c>
-      <c r="L31" s="7">
+      <c r="L31" s="3">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="M31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D32" s="7">
+      <c r="D32" s="3">
         <v>31</v>
       </c>
-      <c r="E32" s="7">
+      <c r="E32" s="3">
         <v>20210305</v>
       </c>
-      <c r="F32" s="7">
+      <c r="F32" s="3">
         <v>21.2</v>
       </c>
-      <c r="G32" s="7">
+      <c r="G32" s="3">
         <v>21.2</v>
       </c>
-      <c r="H32" s="7">
+      <c r="H32" s="3">
         <f t="shared" si="0"/>
         <v>21.2</v>
       </c>
-      <c r="I32" s="7">
+      <c r="I32" s="3">
         <v>23</v>
       </c>
-      <c r="J32" s="7">
+      <c r="J32" s="3">
         <v>23</v>
       </c>
-      <c r="K32" s="7">
+      <c r="K32" s="3">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="L32" s="7">
+      <c r="L32" s="3">
         <v>8.6999999999999993</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="7" t="s">
+      <c r="M32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="8" t="s">
+      <c r="B33" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D33" s="7">
+      <c r="D33" s="3">
         <v>32</v>
       </c>
-      <c r="E33" s="7">
+      <c r="E33" s="3">
         <v>20210305</v>
       </c>
-      <c r="F33" s="7">
+      <c r="F33" s="3">
         <v>27</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G33" s="3">
         <v>26.8</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H33" s="3">
         <f t="shared" si="0"/>
         <v>26.9</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I33" s="3">
         <v>18.7</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J33" s="3">
         <v>18.7</v>
       </c>
-      <c r="K33" s="7">
+      <c r="K33" s="3">
         <f t="shared" si="1"/>
         <v>18.7</v>
       </c>
-      <c r="L33" s="7">
+      <c r="L33" s="3">
         <v>9.1999999999999993</v>
+      </c>
+      <c r="M33" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N33" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="3">
+        <v>33</v>
+      </c>
+      <c r="E34" s="3">
+        <v>20210316</v>
+      </c>
+      <c r="F34" s="3">
+        <v>89.6</v>
+      </c>
+      <c r="G34" s="3">
+        <v>89.2</v>
+      </c>
+      <c r="H34" s="3">
+        <f t="shared" si="0"/>
+        <v>89.4</v>
+      </c>
+      <c r="I34" s="3">
+        <v>56.8</v>
+      </c>
+      <c r="J34" s="3">
+        <v>56.8</v>
+      </c>
+      <c r="K34" s="3">
+        <f t="shared" si="1"/>
+        <v>56.8</v>
+      </c>
+      <c r="L34" s="3">
+        <v>8.4</v>
+      </c>
+      <c r="M34" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="3">
+        <v>34</v>
+      </c>
+      <c r="E35" s="3">
+        <v>20210316</v>
+      </c>
+      <c r="F35" s="3">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="G35" s="3">
+        <v>37</v>
+      </c>
+      <c r="H35" s="3">
+        <f t="shared" si="0"/>
+        <v>37.15</v>
+      </c>
+      <c r="I35" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="J35" s="3">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="K35" s="3">
+        <f t="shared" si="1"/>
+        <v>18.600000000000001</v>
+      </c>
+      <c r="L35" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="M35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="3">
+        <v>35</v>
+      </c>
+      <c r="E36" s="3">
+        <v>20210316</v>
+      </c>
+      <c r="F36" s="3">
+        <v>32.200000000000003</v>
+      </c>
+      <c r="G36" s="3">
+        <v>32</v>
+      </c>
+      <c r="H36" s="3">
+        <f t="shared" si="0"/>
+        <v>32.1</v>
+      </c>
+      <c r="I36" s="3">
+        <v>17.3</v>
+      </c>
+      <c r="J36" s="3">
+        <v>17.2</v>
+      </c>
+      <c r="K36" s="3">
+        <f t="shared" si="1"/>
+        <v>17.25</v>
+      </c>
+      <c r="L36" s="3">
+        <v>8.9</v>
+      </c>
+      <c r="M36" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="N1:N7 N15:N1048576">
+  <conditionalFormatting sqref="N1:N7 N37:N1048576 N15:N28">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N29:N36">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",N29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3561,7 +3486,7 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16" style="33" customWidth="1"/>
+    <col min="6" max="6" width="16" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3580,7 +3505,7 @@
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="26" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3603,7 +3528,7 @@
       <c r="E2" s="7">
         <v>22</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="27">
         <f>500/E2</f>
         <v>22.727272727272727</v>
       </c>
@@ -3624,7 +3549,7 @@
       <c r="E3" s="7">
         <v>21.4</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="27">
         <f t="shared" ref="F3:F6" si="0">500/E3</f>
         <v>23.364485981308412</v>
       </c>
@@ -3645,7 +3570,7 @@
       <c r="E4" s="7">
         <v>21.299999999999997</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="27">
         <f t="shared" si="0"/>
         <v>23.474178403755872</v>
       </c>
@@ -3666,7 +3591,7 @@
       <c r="E5" s="7">
         <v>34</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="27">
         <f t="shared" si="0"/>
         <v>14.705882352941176</v>
       </c>
@@ -3687,7 +3612,7 @@
       <c r="E6" s="7">
         <v>30.8</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="27">
         <f t="shared" si="0"/>
         <v>16.233766233766232</v>
       </c>
@@ -3708,7 +3633,7 @@
       <c r="E7" s="7">
         <v>16.399999999999999</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="27">
         <f t="shared" ref="F7:F13" si="1">500/E7</f>
         <v>30.487804878048784</v>
       </c>
@@ -3729,7 +3654,7 @@
       <c r="E8" s="7">
         <v>30.1</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="27">
         <f t="shared" si="1"/>
         <v>16.611295681063122</v>
       </c>
@@ -3750,7 +3675,7 @@
       <c r="E9" s="7">
         <v>48.8</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="27">
         <f t="shared" si="1"/>
         <v>10.245901639344263</v>
       </c>
@@ -3771,7 +3696,7 @@
       <c r="E10" s="7">
         <v>36.799999999999997</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="27">
         <f t="shared" si="1"/>
         <v>13.586956521739131</v>
       </c>
@@ -3792,7 +3717,7 @@
       <c r="E11" s="7">
         <v>37.799999999999997</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="27">
         <f t="shared" si="1"/>
         <v>13.227513227513228</v>
       </c>
@@ -3813,7 +3738,7 @@
       <c r="E12" s="7">
         <v>30</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="27">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
@@ -3834,7 +3759,7 @@
       <c r="E13" s="7">
         <v>44.8</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="27">
         <f t="shared" si="1"/>
         <v>11.160714285714286</v>
       </c>

</xml_diff>

<commit_message>
tapestation screenshot and pdf
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C25BE1FD-F10A-154D-9514-7C50A41C1C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4069F110-574C-9642-AE1E-252C1C04DACE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5560" yWindow="460" windowWidth="28020" windowHeight="18860" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5560" yWindow="460" windowWidth="28020" windowHeight="18860" activeTab="1" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="68">
   <si>
     <t>ColonyID</t>
   </si>
@@ -237,13 +237,19 @@
   </si>
   <si>
     <t>RNA and RIN score too low</t>
+  </si>
+  <si>
+    <t>2019-07-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RIN too low </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,6 +273,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -421,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -442,14 +455,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -467,6 +476,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -811,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -822,325 +832,605 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="24" t="s">
+      <c r="E1" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="21" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="18"/>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="14">
         <v>43662</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="19"/>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="17"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15">
+      <c r="A3">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>13</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="14">
         <v>43662</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="19"/>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="18"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15">
+      <c r="A4">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14">
         <v>43662</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="19"/>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15">
+      <c r="A5">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="14">
         <v>43662</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="19"/>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="17"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="18"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15">
+      <c r="A6">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="14">
         <v>43662</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="19"/>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="17"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="18"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15">
+      <c r="A7">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="14">
         <v>43662</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="19"/>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" s="17"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="18"/>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15">
+      <c r="A8">
+        <v>201</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>13</v>
+      </c>
+      <c r="D8">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="14">
         <v>43662</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="19"/>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="17"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="18"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="15">
+      <c r="A9">
+        <v>202</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>9</v>
+      </c>
+      <c r="E9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="14">
         <v>43662</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="19"/>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="18"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15">
+      <c r="A10">
+        <v>203</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="14">
         <v>43662</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="19"/>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="17"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="18"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="15">
+      <c r="A11">
+        <v>204</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="14">
         <v>43662</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="19"/>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="18"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15">
+      <c r="A12">
+        <v>209</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="14">
         <v>43662</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="19"/>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" t="s">
+        <v>8</v>
+      </c>
+      <c r="I12" s="17"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="15">
+      <c r="A13">
+        <v>210</v>
+      </c>
+      <c r="B13" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="14">
         <v>43662</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="19"/>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I13" s="17"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="18"/>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="15">
+      <c r="A14">
+        <v>211</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="14">
         <v>43662</v>
       </c>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="19"/>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14" s="17"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="18"/>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15">
+      <c r="A15">
+        <v>212</v>
+      </c>
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="14">
         <v>43662</v>
       </c>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="19"/>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" t="s">
+        <v>8</v>
+      </c>
+      <c r="I15" s="17"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="18"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15">
+      <c r="A16">
+        <v>217</v>
+      </c>
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>13</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" s="14">
         <v>43662</v>
       </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="19"/>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16" t="s">
+        <v>8</v>
+      </c>
+      <c r="I16" s="17"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A17" s="18"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="15">
+      <c r="A17">
+        <v>218</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="14">
         <v>43662</v>
       </c>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="19"/>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="17"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A18" s="18"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15">
+      <c r="A18">
+        <v>219</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="14">
         <v>43662</v>
       </c>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="19"/>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" t="s">
+        <v>8</v>
+      </c>
+      <c r="I18" s="17"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A19" s="18"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="15">
+      <c r="A19">
+        <v>220</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="14">
         <v>43662</v>
       </c>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="19"/>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+      <c r="H19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="17"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="18"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="15">
+      <c r="A20">
+        <v>221</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>15</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="14">
         <v>43662</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="19"/>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+      <c r="H20" t="s">
+        <v>8</v>
+      </c>
+      <c r="I20" s="17"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="15">
+      <c r="A21">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="14">
         <v>43662</v>
       </c>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="22"/>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" t="s">
+        <v>8</v>
+      </c>
+      <c r="I21" s="18"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="29">
-        <v>3</v>
-      </c>
-      <c r="B22" s="30" t="s">
+      <c r="A22" s="25">
+        <v>3</v>
+      </c>
+      <c r="B22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="30">
-        <v>13</v>
-      </c>
-      <c r="D22" s="30">
+      <c r="C22" s="26">
+        <v>13</v>
+      </c>
+      <c r="D22" s="26">
         <v>1</v>
       </c>
-      <c r="E22" s="30" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="31">
+      <c r="E22" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" s="27">
         <v>43803</v>
       </c>
-      <c r="G22" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="32">
+      <c r="G22" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="I22" s="28">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A23" s="16">
+      <c r="A23" s="15">
         <v>4</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -1164,12 +1454,12 @@
       <c r="H23" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="17">
+      <c r="I23" s="16">
         <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="16">
+      <c r="A24" s="15">
         <v>11</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -1193,12 +1483,12 @@
       <c r="H24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I24" s="17">
+      <c r="I24" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A25" s="16">
+      <c r="A25" s="15">
         <v>12</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -1222,12 +1512,12 @@
       <c r="H25" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I25" s="17">
+      <c r="I25" s="16">
         <v>25</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+      <c r="A26" s="15">
         <v>19</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -1251,12 +1541,12 @@
       <c r="H26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="16">
         <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A27" s="16">
+      <c r="A27" s="15">
         <v>20</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -1280,12 +1570,12 @@
       <c r="H27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I27" s="17">
+      <c r="I27" s="16">
         <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A28" s="16">
+      <c r="A28" s="15">
         <v>201</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -1309,12 +1599,12 @@
       <c r="H28" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I28" s="17">
+      <c r="I28" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A29" s="16">
+      <c r="A29" s="15">
         <v>202</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -1338,12 +1628,12 @@
       <c r="H29" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I29" s="17">
+      <c r="I29" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A30" s="16">
+      <c r="A30" s="15">
         <v>203</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -1367,12 +1657,12 @@
       <c r="H30" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I30" s="17">
+      <c r="I30" s="16">
         <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A31" s="16">
+      <c r="A31" s="15">
         <v>204</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -1396,12 +1686,12 @@
       <c r="H31" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I31" s="17">
+      <c r="I31" s="16">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="16">
+      <c r="A32" s="15">
         <v>209</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -1425,12 +1715,12 @@
       <c r="H32" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I32" s="17">
+      <c r="I32" s="16">
         <v>22</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="16">
+      <c r="A33" s="15">
         <v>210</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -1454,12 +1744,12 @@
       <c r="H33" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I33" s="17">
+      <c r="I33" s="16">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="16">
+      <c r="A34" s="15">
         <v>211</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -1483,12 +1773,12 @@
       <c r="H34" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="16">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A35" s="16">
+      <c r="A35" s="15">
         <v>212</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -1512,12 +1802,12 @@
       <c r="H35" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I35" s="17">
+      <c r="I35" s="16">
         <v>17</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="16">
+      <c r="A36" s="15">
         <v>217</v>
       </c>
       <c r="B36" s="12" t="s">
@@ -1541,12 +1831,12 @@
       <c r="H36" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I36" s="17">
+      <c r="I36" s="16">
         <v>16</v>
       </c>
     </row>
     <row r="37" spans="1:9" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
+      <c r="A37" s="15">
         <v>218</v>
       </c>
       <c r="B37" s="12" t="s">
@@ -1570,12 +1860,12 @@
       <c r="H37" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I37" s="17">
+      <c r="I37" s="16">
         <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A38" s="16">
+      <c r="A38" s="15">
         <v>219</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -1599,12 +1889,12 @@
       <c r="H38" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I38" s="17">
+      <c r="I38" s="16">
         <v>23</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="16">
+      <c r="A39" s="15">
         <v>220</v>
       </c>
       <c r="B39" s="12" t="s">
@@ -1628,12 +1918,12 @@
       <c r="H39" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I39" s="17">
+      <c r="I39" s="16">
         <v>24</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="16">
+      <c r="A40" s="15">
         <v>221</v>
       </c>
       <c r="B40" s="12" t="s">
@@ -1657,51 +1947,51 @@
       <c r="H40" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="I40" s="17">
+      <c r="I40" s="16">
         <v>28</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="33">
+      <c r="A41" s="29">
         <v>222</v>
       </c>
-      <c r="B41" s="34" t="s">
+      <c r="B41" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="34">
-        <v>13</v>
-      </c>
-      <c r="D41" s="34">
+      <c r="C41" s="30">
+        <v>13</v>
+      </c>
+      <c r="D41" s="30">
         <v>15</v>
       </c>
-      <c r="E41" s="34" t="s">
+      <c r="E41" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F41" s="35">
+      <c r="F41" s="31">
         <v>43803</v>
       </c>
-      <c r="G41" s="34" t="s">
-        <v>8</v>
-      </c>
-      <c r="H41" s="34" t="s">
-        <v>30</v>
-      </c>
-      <c r="I41" s="36">
+      <c r="G41" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="I41" s="32">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="89" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="78" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AD3CB-63E2-694C-817E-F91992571833}">
-  <dimension ref="A1:O36"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1841,7 +2131,7 @@
         <v>20.2</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H36" si="0">(F3+G3)/2</f>
+        <f t="shared" ref="H3:H39" si="0">(F3+G3)/2</f>
         <v>20.299999999999997</v>
       </c>
       <c r="I3" s="3">
@@ -1851,7 +2141,7 @@
         <v>22</v>
       </c>
       <c r="K3" s="3">
-        <f t="shared" ref="K3:K36" si="1">(I3+J3)/2</f>
+        <f t="shared" ref="K3:K39" si="1">(I3+J3)/2</f>
         <v>22</v>
       </c>
       <c r="L3" s="3">
@@ -2990,7 +3280,9 @@
       <c r="N26" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O26" s="3"/>
+      <c r="O26" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
@@ -3037,6 +3329,9 @@
       <c r="N27" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="O27" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
@@ -3132,6 +3427,9 @@
       <c r="N29" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="O29" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="30" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -3178,6 +3476,9 @@
       <c r="N30" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="O30" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="31" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
@@ -3224,6 +3525,9 @@
       <c r="N31" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="O31" s="3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
@@ -3270,8 +3574,11 @@
       <c r="N32" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="O32" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>64</v>
       </c>
@@ -3316,8 +3623,11 @@
       <c r="N33" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O33" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>50</v>
       </c>
@@ -3362,8 +3672,11 @@
       <c r="N34" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O34" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -3408,8 +3721,11 @@
       <c r="N35" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O35" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>47</v>
       </c>
@@ -3453,6 +3769,135 @@
       </c>
       <c r="N36" s="3" t="s">
         <v>41</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="7">
+        <v>36</v>
+      </c>
+      <c r="E37" s="7">
+        <v>20210430</v>
+      </c>
+      <c r="F37" s="7">
+        <v>28.4</v>
+      </c>
+      <c r="G37" s="7">
+        <v>28.2</v>
+      </c>
+      <c r="H37" s="7">
+        <f t="shared" si="0"/>
+        <v>28.299999999999997</v>
+      </c>
+      <c r="I37" s="7">
+        <v>64.8</v>
+      </c>
+      <c r="J37" s="7">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="K37" s="7">
+        <f t="shared" si="1"/>
+        <v>64.599999999999994</v>
+      </c>
+      <c r="L37" s="7">
+        <v>5.6</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O37" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="7">
+        <v>37</v>
+      </c>
+      <c r="E38" s="7">
+        <v>20210430</v>
+      </c>
+      <c r="F38" s="7">
+        <v>34</v>
+      </c>
+      <c r="G38" s="7">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="H38" s="7">
+        <f t="shared" si="0"/>
+        <v>33.9</v>
+      </c>
+      <c r="I38" s="7">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="J38" s="7">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="K38" s="7">
+        <f t="shared" si="1"/>
+        <v>32.799999999999997</v>
+      </c>
+      <c r="L38" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="7">
+        <v>38</v>
+      </c>
+      <c r="E39" s="7">
+        <v>20210430</v>
+      </c>
+      <c r="F39" s="7">
+        <v>15.2</v>
+      </c>
+      <c r="G39" s="7">
+        <v>15</v>
+      </c>
+      <c r="H39" s="7">
+        <f t="shared" si="0"/>
+        <v>15.1</v>
+      </c>
+      <c r="I39" s="7">
+        <v>13.5</v>
+      </c>
+      <c r="J39" s="7">
+        <v>13.6</v>
+      </c>
+      <c r="K39" s="7">
+        <f t="shared" si="1"/>
+        <v>13.55</v>
+      </c>
+      <c r="L39" s="7">
+        <v>8.4</v>
       </c>
     </row>
   </sheetData>
@@ -3486,7 +3931,7 @@
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
-    <col min="6" max="6" width="16" style="28" customWidth="1"/>
+    <col min="6" max="6" width="16" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.2">
@@ -3505,7 +3950,7 @@
       <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="22" t="s">
         <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -3528,7 +3973,7 @@
       <c r="E2" s="7">
         <v>22</v>
       </c>
-      <c r="F2" s="27">
+      <c r="F2" s="23">
         <f>500/E2</f>
         <v>22.727272727272727</v>
       </c>
@@ -3549,7 +3994,7 @@
       <c r="E3" s="7">
         <v>21.4</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="23">
         <f t="shared" ref="F3:F6" si="0">500/E3</f>
         <v>23.364485981308412</v>
       </c>
@@ -3570,7 +4015,7 @@
       <c r="E4" s="7">
         <v>21.299999999999997</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="23">
         <f t="shared" si="0"/>
         <v>23.474178403755872</v>
       </c>
@@ -3591,7 +4036,7 @@
       <c r="E5" s="7">
         <v>34</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="23">
         <f t="shared" si="0"/>
         <v>14.705882352941176</v>
       </c>
@@ -3612,7 +4057,7 @@
       <c r="E6" s="7">
         <v>30.8</v>
       </c>
-      <c r="F6" s="27">
+      <c r="F6" s="23">
         <f t="shared" si="0"/>
         <v>16.233766233766232</v>
       </c>
@@ -3633,7 +4078,7 @@
       <c r="E7" s="7">
         <v>16.399999999999999</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="23">
         <f t="shared" ref="F7:F13" si="1">500/E7</f>
         <v>30.487804878048784</v>
       </c>
@@ -3654,7 +4099,7 @@
       <c r="E8" s="7">
         <v>30.1</v>
       </c>
-      <c r="F8" s="27">
+      <c r="F8" s="23">
         <f t="shared" si="1"/>
         <v>16.611295681063122</v>
       </c>
@@ -3675,7 +4120,7 @@
       <c r="E9" s="7">
         <v>48.8</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="23">
         <f t="shared" si="1"/>
         <v>10.245901639344263</v>
       </c>
@@ -3696,7 +4141,7 @@
       <c r="E10" s="7">
         <v>36.799999999999997</v>
       </c>
-      <c r="F10" s="27">
+      <c r="F10" s="23">
         <f t="shared" si="1"/>
         <v>13.586956521739131</v>
       </c>
@@ -3717,7 +4162,7 @@
       <c r="E11" s="7">
         <v>37.799999999999997</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="23">
         <f t="shared" si="1"/>
         <v>13.227513227513228</v>
       </c>
@@ -3738,7 +4183,7 @@
       <c r="E12" s="7">
         <v>30</v>
       </c>
-      <c r="F12" s="27">
+      <c r="F12" s="23">
         <f t="shared" si="1"/>
         <v>16.666666666666668</v>
       </c>
@@ -3759,7 +4204,7 @@
       <c r="E13" s="7">
         <v>44.8</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="23">
         <f t="shared" si="1"/>
         <v>11.160714285714286</v>
       </c>

</xml_diff>

<commit_message>
molecular work for july 2019 ext
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4069F110-574C-9642-AE1E-252C1C04DACE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2724A63-3A1F-F248-A95D-DB8DA464BABF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5560" yWindow="460" windowWidth="28020" windowHeight="18860" activeTab="1" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="70">
   <si>
     <t>ColonyID</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t xml:space="preserve">RIN too low </t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>maybe re-do this one b/c the DNA quality is low</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -477,6 +483,7 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,7 +829,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1077,31 +1084,33 @@
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>203</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="3">
         <v>13</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>10</v>
       </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="14">
+      <c r="E10" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="13">
         <v>43662</v>
       </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I10" s="17"/>
+      <c r="G10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I10" s="16">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1990,8 +1999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{694AD3CB-63E2-694C-817E-F91992571833}">
   <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3813,6 +3822,9 @@
       <c r="L37" s="7">
         <v>5.6</v>
       </c>
+      <c r="M37" s="7" t="s">
+        <v>42</v>
+      </c>
       <c r="N37" s="7" t="s">
         <v>42</v>
       </c>
@@ -3859,45 +3871,63 @@
       <c r="L38" s="7">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A39" s="7" t="s">
+      <c r="M38" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="O38" s="7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="33" t="s">
+      <c r="B39" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="C39" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D39" s="7">
+      <c r="C39" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D39" s="3">
         <v>38</v>
       </c>
-      <c r="E39" s="7">
+      <c r="E39" s="3">
         <v>20210430</v>
       </c>
-      <c r="F39" s="7">
+      <c r="F39" s="3">
         <v>15.2</v>
       </c>
-      <c r="G39" s="7">
+      <c r="G39" s="3">
         <v>15</v>
       </c>
-      <c r="H39" s="7">
+      <c r="H39" s="3">
         <f t="shared" si="0"/>
         <v>15.1</v>
       </c>
-      <c r="I39" s="7">
+      <c r="I39" s="3">
         <v>13.5</v>
       </c>
-      <c r="J39" s="7">
+      <c r="J39" s="3">
         <v>13.6</v>
       </c>
-      <c r="K39" s="7">
+      <c r="K39" s="3">
         <f t="shared" si="1"/>
         <v>13.55</v>
       </c>
-      <c r="L39" s="7">
+      <c r="L39" s="3">
         <v>8.4</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="N39" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O39" s="3" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added RNA remaining to tag seq prep tab
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7030CA11-9F9D-CA43-8965-9F7411A8FCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153ACD7-A090-9949-9A49-85E39B9DFE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35780" yWindow="1780" windowWidth="27860" windowHeight="18960" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="84">
   <si>
     <t>ColonyID</t>
   </si>
@@ -288,6 +288,9 @@
   </si>
   <si>
     <t>Platemap to ship (by extraction ID)</t>
+  </si>
+  <si>
+    <t>RNA remaining (uL)</t>
   </si>
 </sst>
 </file>
@@ -599,15 +602,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2258,7 +2259,7 @@
         <v>5.78</v>
       </c>
       <c r="H2" s="5">
-        <f>(F2+G2)/2</f>
+        <f t="shared" ref="H2:H33" si="0">(F2+G2)/2</f>
         <v>5.8100000000000005</v>
       </c>
       <c r="I2" s="5">
@@ -2268,7 +2269,7 @@
         <v>43</v>
       </c>
       <c r="K2" s="5">
-        <f>(I2+J2)/2</f>
+        <f t="shared" ref="K2:K33" si="1">(I2+J2)/2</f>
         <v>43.1</v>
       </c>
       <c r="L2" s="5">
@@ -2307,7 +2308,7 @@
         <v>7.04</v>
       </c>
       <c r="H3" s="5">
-        <f>(F3+G3)/2</f>
+        <f t="shared" si="0"/>
         <v>7.05</v>
       </c>
       <c r="I3" s="5">
@@ -2317,7 +2318,7 @@
         <v>66.400000000000006</v>
       </c>
       <c r="K3" s="5">
-        <f>(I3+J3)/2</f>
+        <f t="shared" si="1"/>
         <v>66.400000000000006</v>
       </c>
       <c r="L3" s="5">
@@ -2356,7 +2357,7 @@
         <v>57.6</v>
       </c>
       <c r="H4" s="5">
-        <f>(F4+G4)/2</f>
+        <f t="shared" si="0"/>
         <v>57.7</v>
       </c>
       <c r="I4" s="5">
@@ -2366,7 +2367,7 @@
         <v>36.6</v>
       </c>
       <c r="K4" s="5">
-        <f>(I4+J4)/2</f>
+        <f t="shared" si="1"/>
         <v>36.6</v>
       </c>
       <c r="L4" s="5">
@@ -2405,7 +2406,7 @@
         <v>17.2</v>
       </c>
       <c r="H5" s="8">
-        <f>(F5+G5)/2</f>
+        <f t="shared" si="0"/>
         <v>17.25</v>
       </c>
       <c r="I5" s="8">
@@ -2415,7 +2416,7 @@
         <v>31</v>
       </c>
       <c r="K5" s="8">
-        <f>(I5+J5)/2</f>
+        <f t="shared" si="1"/>
         <v>31.1</v>
       </c>
       <c r="L5" s="8">
@@ -2454,7 +2455,7 @@
         <v>20.6</v>
       </c>
       <c r="H6" s="8">
-        <f>(F6+G6)/2</f>
+        <f t="shared" si="0"/>
         <v>20.6</v>
       </c>
       <c r="I6" s="8">
@@ -2464,7 +2465,7 @@
         <v>22.2</v>
       </c>
       <c r="K6" s="8">
-        <f>(I6+J6)/2</f>
+        <f t="shared" si="1"/>
         <v>22.2</v>
       </c>
       <c r="L6" s="8">
@@ -2503,7 +2504,7 @@
         <v>8.02</v>
       </c>
       <c r="H7" s="5">
-        <f>(F7+G7)/2</f>
+        <f t="shared" si="0"/>
         <v>8.0500000000000007</v>
       </c>
       <c r="I7" s="5">
@@ -2513,7 +2514,7 @@
         <v>45.6</v>
       </c>
       <c r="K7" s="5">
-        <f>(I7+J7)/2</f>
+        <f t="shared" si="1"/>
         <v>45.6</v>
       </c>
       <c r="L7" s="5">
@@ -2552,7 +2553,7 @@
         <v>6.76</v>
       </c>
       <c r="H8" s="5">
-        <f>(F8+G8)/2</f>
+        <f t="shared" si="0"/>
         <v>6.77</v>
       </c>
       <c r="I8" s="5">
@@ -2562,7 +2563,7 @@
         <v>15.3</v>
       </c>
       <c r="K8" s="5">
-        <f>(I8+J8)/2</f>
+        <f t="shared" si="1"/>
         <v>15.3</v>
       </c>
       <c r="L8" s="5">
@@ -2601,7 +2602,7 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="H9" s="5">
-        <f>(F9+G9)/2</f>
+        <f t="shared" si="0"/>
         <v>4.4600000000000009</v>
       </c>
       <c r="I9" s="5">
@@ -2611,7 +2612,7 @@
         <v>53.8</v>
       </c>
       <c r="K9" s="5">
-        <f>(I9+J9)/2</f>
+        <f t="shared" si="1"/>
         <v>53.9</v>
       </c>
       <c r="L9" s="5">
@@ -2650,7 +2651,7 @@
         <v>21</v>
       </c>
       <c r="H10" s="5">
-        <f>(F10+G10)/2</f>
+        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="I10" s="5">
@@ -2660,7 +2661,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="K10" s="5">
-        <f>(I10+J10)/2</f>
+        <f t="shared" si="1"/>
         <v>37.799999999999997</v>
       </c>
       <c r="L10" s="5">
@@ -2699,7 +2700,7 @@
         <v>31.6</v>
       </c>
       <c r="H11" s="8">
-        <f>(F11+G11)/2</f>
+        <f t="shared" si="0"/>
         <v>31.700000000000003</v>
       </c>
       <c r="I11" s="8">
@@ -2709,7 +2710,7 @@
         <v>29.2</v>
       </c>
       <c r="K11" s="8">
-        <f>(I11+J11)/2</f>
+        <f t="shared" si="1"/>
         <v>29.2</v>
       </c>
       <c r="L11" s="8">
@@ -2748,7 +2749,7 @@
         <v>28.2</v>
       </c>
       <c r="H12" s="5">
-        <f>(F12+G12)/2</f>
+        <f t="shared" si="0"/>
         <v>28.2</v>
       </c>
       <c r="I12" s="5">
@@ -2758,7 +2759,7 @@
         <v>26</v>
       </c>
       <c r="K12" s="5">
-        <f>(I12+J12)/2</f>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="L12" s="5">
@@ -2797,7 +2798,7 @@
         <v>18.5</v>
       </c>
       <c r="H13" s="8">
-        <f>(F13+G13)/2</f>
+        <f t="shared" si="0"/>
         <v>18.55</v>
       </c>
       <c r="I13" s="8">
@@ -2807,7 +2808,7 @@
         <v>34</v>
       </c>
       <c r="K13" s="8">
-        <f>(I13+J13)/2</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="L13" s="8">
@@ -2846,7 +2847,7 @@
         <v>58.2</v>
       </c>
       <c r="H14" s="5">
-        <f>(F14+G14)/2</f>
+        <f t="shared" si="0"/>
         <v>58.3</v>
       </c>
       <c r="I14" s="5">
@@ -2856,7 +2857,7 @@
         <v>30.2</v>
       </c>
       <c r="K14" s="5">
-        <f>(I14+J14)/2</f>
+        <f t="shared" si="1"/>
         <v>30.1</v>
       </c>
       <c r="L14" s="5">
@@ -2895,7 +2896,7 @@
         <v>63.8</v>
       </c>
       <c r="H15" s="5">
-        <f>(F15+G15)/2</f>
+        <f t="shared" si="0"/>
         <v>63.9</v>
       </c>
       <c r="I15" s="5">
@@ -2905,7 +2906,7 @@
         <v>48.8</v>
       </c>
       <c r="K15" s="5">
-        <f>(I15+J15)/2</f>
+        <f t="shared" si="1"/>
         <v>48.8</v>
       </c>
       <c r="L15" s="5">
@@ -2944,7 +2945,7 @@
         <v>20.8</v>
       </c>
       <c r="H16" s="5">
-        <f>(F16+G16)/2</f>
+        <f t="shared" si="0"/>
         <v>20.9</v>
       </c>
       <c r="I16" s="5">
@@ -2954,7 +2955,7 @@
         <v>12.3</v>
       </c>
       <c r="K16" s="5">
-        <f>(I16+J16)/2</f>
+        <f t="shared" si="1"/>
         <v>12.25</v>
       </c>
       <c r="L16" s="5" t="s">
@@ -2993,7 +2994,7 @@
         <v>28.2</v>
       </c>
       <c r="H17" s="5">
-        <f>(F17+G17)/2</f>
+        <f t="shared" si="0"/>
         <v>28.299999999999997</v>
       </c>
       <c r="I17" s="5">
@@ -3003,7 +3004,7 @@
         <v>64.400000000000006</v>
       </c>
       <c r="K17" s="5">
-        <f>(I17+J17)/2</f>
+        <f t="shared" si="1"/>
         <v>64.599999999999994</v>
       </c>
       <c r="L17" s="5">
@@ -3042,7 +3043,7 @@
         <v>148</v>
       </c>
       <c r="H18" s="5">
-        <f>(F18+G18)/2</f>
+        <f t="shared" si="0"/>
         <v>148.5</v>
       </c>
       <c r="I18" s="5">
@@ -3052,7 +3053,7 @@
         <v>95.8</v>
       </c>
       <c r="K18" s="5">
-        <f>(I18+J18)/2</f>
+        <f t="shared" si="1"/>
         <v>96.35</v>
       </c>
       <c r="L18" s="5">
@@ -3091,7 +3092,7 @@
         <v>17.5</v>
       </c>
       <c r="H19" s="5">
-        <f>(F19+G19)/2</f>
+        <f t="shared" si="0"/>
         <v>17.600000000000001</v>
       </c>
       <c r="I19" s="5">
@@ -3101,7 +3102,7 @@
         <v>21.4</v>
       </c>
       <c r="K19" s="5">
-        <f>(I19+J19)/2</f>
+        <f t="shared" si="1"/>
         <v>21.4</v>
       </c>
       <c r="L19" s="5">
@@ -3140,7 +3141,7 @@
         <v>55.4</v>
       </c>
       <c r="H20" s="5">
-        <f>(F20+G20)/2</f>
+        <f t="shared" si="0"/>
         <v>55.4</v>
       </c>
       <c r="I20" s="5">
@@ -3150,7 +3151,7 @@
         <v>60.8</v>
       </c>
       <c r="K20" s="5">
-        <f>(I20+J20)/2</f>
+        <f t="shared" si="1"/>
         <v>60.8</v>
       </c>
       <c r="L20" s="5">
@@ -3189,7 +3190,7 @@
         <v>20.2</v>
       </c>
       <c r="H21" s="1">
-        <f>(F21+G21)/2</f>
+        <f t="shared" si="0"/>
         <v>20.299999999999997</v>
       </c>
       <c r="I21" s="1">
@@ -3199,7 +3200,7 @@
         <v>22</v>
       </c>
       <c r="K21" s="1">
-        <f>(I21+J21)/2</f>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="L21" s="1">
@@ -3238,7 +3239,7 @@
         <v>14.6</v>
       </c>
       <c r="H22" s="1">
-        <f>(F22+G22)/2</f>
+        <f t="shared" si="0"/>
         <v>14.649999999999999</v>
       </c>
       <c r="I22" s="1">
@@ -3248,7 +3249,7 @@
         <v>21.4</v>
       </c>
       <c r="K22" s="1">
-        <f>(I22+J22)/2</f>
+        <f t="shared" si="1"/>
         <v>21.4</v>
       </c>
       <c r="L22" s="1">
@@ -3287,7 +3288,7 @@
         <v>24.4</v>
       </c>
       <c r="H23" s="1">
-        <f>(F23+G23)/2</f>
+        <f t="shared" si="0"/>
         <v>24.5</v>
       </c>
       <c r="I23" s="1">
@@ -3297,7 +3298,7 @@
         <v>21.2</v>
       </c>
       <c r="K23" s="1">
-        <f>(I23+J23)/2</f>
+        <f t="shared" si="1"/>
         <v>21.299999999999997</v>
       </c>
       <c r="L23" s="1">
@@ -3336,7 +3337,7 @@
         <v>36.4</v>
       </c>
       <c r="H24" s="1">
-        <f>(F24+G24)/2</f>
+        <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
       <c r="I24" s="1">
@@ -3346,7 +3347,7 @@
         <v>34</v>
       </c>
       <c r="K24" s="1">
-        <f>(I24+J24)/2</f>
+        <f t="shared" si="1"/>
         <v>34</v>
       </c>
       <c r="L24" s="1">
@@ -3385,7 +3386,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="H25" s="1">
-        <f>(F25+G25)/2</f>
+        <f t="shared" si="0"/>
         <v>32.9</v>
       </c>
       <c r="I25" s="1">
@@ -3395,7 +3396,7 @@
         <v>30.8</v>
       </c>
       <c r="K25" s="1">
-        <f>(I25+J25)/2</f>
+        <f t="shared" si="1"/>
         <v>30.8</v>
       </c>
       <c r="L25" s="1">
@@ -3434,7 +3435,7 @@
         <v>31.2</v>
       </c>
       <c r="H26" s="1">
-        <f>(F26+G26)/2</f>
+        <f t="shared" si="0"/>
         <v>31.299999999999997</v>
       </c>
       <c r="I26" s="1">
@@ -3444,7 +3445,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="K26" s="1">
-        <f>(I26+J26)/2</f>
+        <f t="shared" si="1"/>
         <v>16.399999999999999</v>
       </c>
       <c r="L26" s="1">
@@ -3483,7 +3484,7 @@
         <v>54.4</v>
       </c>
       <c r="H27" s="1">
-        <f>(F27+G27)/2</f>
+        <f t="shared" si="0"/>
         <v>54.5</v>
       </c>
       <c r="I27" s="1">
@@ -3493,7 +3494,7 @@
         <v>36.799999999999997</v>
       </c>
       <c r="K27" s="1">
-        <f>(I27+J27)/2</f>
+        <f t="shared" si="1"/>
         <v>36.799999999999997</v>
       </c>
       <c r="L27" s="1">
@@ -3532,7 +3533,7 @@
         <v>51</v>
       </c>
       <c r="H28" s="1">
-        <f>(F28+G28)/2</f>
+        <f t="shared" si="0"/>
         <v>51.1</v>
       </c>
       <c r="I28" s="1">
@@ -3542,7 +3543,7 @@
         <v>37.799999999999997</v>
       </c>
       <c r="K28" s="1">
-        <f>(I28+J28)/2</f>
+        <f t="shared" si="1"/>
         <v>37.799999999999997</v>
       </c>
       <c r="L28" s="1">
@@ -3581,7 +3582,7 @@
         <v>35.6</v>
       </c>
       <c r="H29" s="1">
-        <f>(F29+G29)/2</f>
+        <f t="shared" si="0"/>
         <v>35.700000000000003</v>
       </c>
       <c r="I29" s="1">
@@ -3591,7 +3592,7 @@
         <v>30</v>
       </c>
       <c r="K29" s="1">
-        <f>(I29+J29)/2</f>
+        <f t="shared" si="1"/>
         <v>30</v>
       </c>
       <c r="L29" s="1">
@@ -3630,7 +3631,7 @@
         <v>68.8</v>
       </c>
       <c r="H30" s="1">
-        <f>(F30+G30)/2</f>
+        <f t="shared" si="0"/>
         <v>68.900000000000006</v>
       </c>
       <c r="I30" s="1">
@@ -3640,7 +3641,7 @@
         <v>44.8</v>
       </c>
       <c r="K30" s="1">
-        <f>(I30+J30)/2</f>
+        <f t="shared" si="1"/>
         <v>44.8</v>
       </c>
       <c r="L30" s="1">
@@ -3679,7 +3680,7 @@
         <v>31</v>
       </c>
       <c r="H31" s="1">
-        <f>(F31+G31)/2</f>
+        <f t="shared" si="0"/>
         <v>31.2</v>
       </c>
       <c r="I31" s="1">
@@ -3689,7 +3690,7 @@
         <v>29</v>
       </c>
       <c r="K31" s="1">
-        <f>(I31+J31)/2</f>
+        <f t="shared" si="1"/>
         <v>29.1</v>
       </c>
       <c r="L31" s="1">
@@ -3728,7 +3729,7 @@
         <v>45.8</v>
       </c>
       <c r="H32" s="1">
-        <f>(F32+G32)/2</f>
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="I32" s="1">
@@ -3738,7 +3739,7 @@
         <v>28.6</v>
       </c>
       <c r="K32" s="1">
-        <f>(I32+J32)/2</f>
+        <f t="shared" si="1"/>
         <v>28.700000000000003</v>
       </c>
       <c r="L32" s="1">
@@ -3777,7 +3778,7 @@
         <v>30.8</v>
       </c>
       <c r="H33" s="1">
-        <f>(F33+G33)/2</f>
+        <f t="shared" si="0"/>
         <v>30.6</v>
       </c>
       <c r="I33" s="1">
@@ -3787,7 +3788,7 @@
         <v>30.6</v>
       </c>
       <c r="K33" s="1">
-        <f>(I33+J33)/2</f>
+        <f t="shared" si="1"/>
         <v>30.700000000000003</v>
       </c>
       <c r="L33" s="1">
@@ -3826,7 +3827,7 @@
         <v>63.4</v>
       </c>
       <c r="H34" s="1">
-        <f>(F34+G34)/2</f>
+        <f t="shared" ref="H34:H65" si="2">(F34+G34)/2</f>
         <v>63.8</v>
       </c>
       <c r="I34" s="1">
@@ -3836,7 +3837,7 @@
         <v>51.2</v>
       </c>
       <c r="K34" s="1">
-        <f>(I34+J34)/2</f>
+        <f t="shared" ref="K34:K65" si="3">(I34+J34)/2</f>
         <v>51.400000000000006</v>
       </c>
       <c r="L34" s="1">
@@ -3875,7 +3876,7 @@
         <v>37.4</v>
       </c>
       <c r="H35" s="1">
-        <f>(F35+G35)/2</f>
+        <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
       <c r="I35" s="1">
@@ -3885,7 +3886,7 @@
         <v>31.6</v>
       </c>
       <c r="K35" s="1">
-        <f>(I35+J35)/2</f>
+        <f t="shared" si="3"/>
         <v>31.700000000000003</v>
       </c>
       <c r="L35" s="1">
@@ -3924,7 +3925,7 @@
         <v>21.2</v>
       </c>
       <c r="H36" s="1">
-        <f>(F36+G36)/2</f>
+        <f t="shared" si="2"/>
         <v>21.2</v>
       </c>
       <c r="I36" s="1">
@@ -3934,7 +3935,7 @@
         <v>23</v>
       </c>
       <c r="K36" s="1">
-        <f>(I36+J36)/2</f>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="L36" s="1">
@@ -3973,7 +3974,7 @@
         <v>26.8</v>
       </c>
       <c r="H37" s="1">
-        <f>(F37+G37)/2</f>
+        <f t="shared" si="2"/>
         <v>26.9</v>
       </c>
       <c r="I37" s="1">
@@ -3983,7 +3984,7 @@
         <v>18.7</v>
       </c>
       <c r="K37" s="1">
-        <f>(I37+J37)/2</f>
+        <f t="shared" si="3"/>
         <v>18.7</v>
       </c>
       <c r="L37" s="1">
@@ -4022,7 +4023,7 @@
         <v>89.2</v>
       </c>
       <c r="H38" s="1">
-        <f>(F38+G38)/2</f>
+        <f t="shared" si="2"/>
         <v>89.4</v>
       </c>
       <c r="I38" s="1">
@@ -4032,7 +4033,7 @@
         <v>56.8</v>
       </c>
       <c r="K38" s="1">
-        <f>(I38+J38)/2</f>
+        <f t="shared" si="3"/>
         <v>56.8</v>
       </c>
       <c r="L38" s="1">
@@ -4071,7 +4072,7 @@
         <v>37</v>
       </c>
       <c r="H39" s="1">
-        <f>(F39+G39)/2</f>
+        <f t="shared" si="2"/>
         <v>37.15</v>
       </c>
       <c r="I39" s="1">
@@ -4081,7 +4082,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="K39" s="1">
-        <f>(I39+J39)/2</f>
+        <f t="shared" si="3"/>
         <v>18.600000000000001</v>
       </c>
       <c r="L39" s="1">
@@ -4120,7 +4121,7 @@
         <v>32</v>
       </c>
       <c r="H40" s="1">
-        <f>(F40+G40)/2</f>
+        <f t="shared" si="2"/>
         <v>32.1</v>
       </c>
       <c r="I40" s="1">
@@ -4130,7 +4131,7 @@
         <v>17.2</v>
       </c>
       <c r="K40" s="1">
-        <f>(I40+J40)/2</f>
+        <f t="shared" si="3"/>
         <v>17.25</v>
       </c>
       <c r="L40" s="1">
@@ -4169,7 +4170,7 @@
         <v>33.799999999999997</v>
       </c>
       <c r="H41" s="1">
-        <f>(F41+G41)/2</f>
+        <f t="shared" si="2"/>
         <v>33.9</v>
       </c>
       <c r="I41" s="1">
@@ -4179,7 +4180,7 @@
         <v>32.799999999999997</v>
       </c>
       <c r="K41" s="1">
-        <f>(I41+J41)/2</f>
+        <f t="shared" si="3"/>
         <v>32.799999999999997</v>
       </c>
       <c r="L41" s="1">
@@ -4218,7 +4219,7 @@
         <v>15</v>
       </c>
       <c r="H42" s="1">
-        <f>(F42+G42)/2</f>
+        <f t="shared" si="2"/>
         <v>15.1</v>
       </c>
       <c r="I42" s="1">
@@ -4228,7 +4229,7 @@
         <v>13.6</v>
       </c>
       <c r="K42" s="1">
-        <f>(I42+J42)/2</f>
+        <f t="shared" si="3"/>
         <v>13.55</v>
       </c>
       <c r="L42" s="1">
@@ -4267,7 +4268,7 @@
         <v>103</v>
       </c>
       <c r="H43" s="1">
-        <f>(F43+G43)/2</f>
+        <f t="shared" si="2"/>
         <v>104</v>
       </c>
       <c r="I43" s="1">
@@ -4277,7 +4278,7 @@
         <v>72.8</v>
       </c>
       <c r="K43" s="1">
-        <f>(I43+J43)/2</f>
+        <f t="shared" si="3"/>
         <v>73.199999999999989</v>
       </c>
       <c r="L43" s="1">
@@ -4314,7 +4315,7 @@
         <v>39.799999999999997</v>
       </c>
       <c r="H44" s="1">
-        <f>(F44+G44)/2</f>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="I44" s="1">
@@ -4324,7 +4325,7 @@
         <v>16</v>
       </c>
       <c r="K44" s="1">
-        <f>(I44+J44)/2</f>
+        <f t="shared" si="3"/>
         <v>16.05</v>
       </c>
       <c r="L44" s="1">
@@ -4361,7 +4362,7 @@
         <v>28.4</v>
       </c>
       <c r="H45" s="1">
-        <f>(F45+G45)/2</f>
+        <f t="shared" si="2"/>
         <v>28.6</v>
       </c>
       <c r="I45" s="1">
@@ -4371,7 +4372,7 @@
         <v>11.2</v>
       </c>
       <c r="K45" s="1">
-        <f>(I45+J45)/2</f>
+        <f t="shared" si="3"/>
         <v>11.2</v>
       </c>
       <c r="L45" s="1">
@@ -4408,7 +4409,7 @@
         <v>79.8</v>
       </c>
       <c r="H46" s="1">
-        <f>(F46+G46)/2</f>
+        <f t="shared" si="2"/>
         <v>80.199999999999989</v>
       </c>
       <c r="I46" s="1">
@@ -4418,7 +4419,7 @@
         <v>37</v>
       </c>
       <c r="K46" s="1">
-        <f>(I46+J46)/2</f>
+        <f t="shared" si="3"/>
         <v>36.9</v>
       </c>
       <c r="L46" s="1">
@@ -4455,7 +4456,7 @@
         <v>47.2</v>
       </c>
       <c r="H47" s="1">
-        <f>(F47+G47)/2</f>
+        <f t="shared" si="2"/>
         <v>47.400000000000006</v>
       </c>
       <c r="I47" s="1">
@@ -4465,7 +4466,7 @@
         <v>26</v>
       </c>
       <c r="K47" s="1">
-        <f>(I47+J47)/2</f>
+        <f t="shared" si="3"/>
         <v>26</v>
       </c>
       <c r="L47" s="1">
@@ -4502,7 +4503,7 @@
         <v>37</v>
       </c>
       <c r="H48" s="1">
-        <f>(F48+G48)/2</f>
+        <f t="shared" si="2"/>
         <v>37.1</v>
       </c>
       <c r="I48" s="1">
@@ -4512,7 +4513,7 @@
         <v>12.7</v>
       </c>
       <c r="K48" s="1">
-        <f>(I48+J48)/2</f>
+        <f t="shared" si="3"/>
         <v>12.75</v>
       </c>
       <c r="L48" s="1">
@@ -4549,7 +4550,7 @@
         <v>73.2</v>
       </c>
       <c r="H49" s="1">
-        <f>(F49+G49)/2</f>
+        <f t="shared" si="2"/>
         <v>73.5</v>
       </c>
       <c r="I49" s="1">
@@ -4559,7 +4560,7 @@
         <v>76.2</v>
       </c>
       <c r="K49" s="1">
-        <f>(I49+J49)/2</f>
+        <f t="shared" si="3"/>
         <v>76.400000000000006</v>
       </c>
       <c r="L49" s="1">
@@ -4598,7 +4599,7 @@
         <v>88.2</v>
       </c>
       <c r="H50" s="1">
-        <f>(F50+G50)/2</f>
+        <f t="shared" si="2"/>
         <v>88.6</v>
       </c>
       <c r="I50" s="1">
@@ -4608,7 +4609,7 @@
         <v>71.400000000000006</v>
       </c>
       <c r="K50" s="1">
-        <f>(I50+J50)/2</f>
+        <f t="shared" si="3"/>
         <v>71.599999999999994</v>
       </c>
       <c r="L50" s="1">
@@ -4645,7 +4646,7 @@
         <v>79.599999999999994</v>
       </c>
       <c r="H51" s="1">
-        <f>(F51+G51)/2</f>
+        <f t="shared" si="2"/>
         <v>80</v>
       </c>
       <c r="I51" s="1">
@@ -4655,7 +4656,7 @@
         <v>45.8</v>
       </c>
       <c r="K51" s="1">
-        <f>(I51+J51)/2</f>
+        <f t="shared" si="3"/>
         <v>45.9</v>
       </c>
       <c r="L51" s="1">
@@ -4692,7 +4693,7 @@
         <v>69</v>
       </c>
       <c r="H52" s="1">
-        <f>(F52+G52)/2</f>
+        <f t="shared" si="2"/>
         <v>69.3</v>
       </c>
       <c r="I52" s="1">
@@ -4702,7 +4703,7 @@
         <v>44.2</v>
       </c>
       <c r="K52" s="1">
-        <f>(I52+J52)/2</f>
+        <f t="shared" si="3"/>
         <v>44.3</v>
       </c>
       <c r="L52" s="1">
@@ -4739,7 +4740,7 @@
         <v>40.200000000000003</v>
       </c>
       <c r="H53" s="1">
-        <f>(F53+G53)/2</f>
+        <f t="shared" si="2"/>
         <v>40.299999999999997</v>
       </c>
       <c r="I53" s="1">
@@ -4749,7 +4750,7 @@
         <v>24.6</v>
       </c>
       <c r="K53" s="1">
-        <f>(I53+J53)/2</f>
+        <f t="shared" si="3"/>
         <v>24.6</v>
       </c>
       <c r="L53" s="1">
@@ -4786,7 +4787,7 @@
         <v>74.400000000000006</v>
       </c>
       <c r="H54" s="1">
-        <f>(F54+G54)/2</f>
+        <f t="shared" si="2"/>
         <v>74.7</v>
       </c>
       <c r="I54" s="1">
@@ -4796,7 +4797,7 @@
         <v>40</v>
       </c>
       <c r="K54" s="1">
-        <f>(I54+J54)/2</f>
+        <f t="shared" si="3"/>
         <v>40.1</v>
       </c>
       <c r="L54" s="1">
@@ -4832,7 +4833,7 @@
         <v>21.2</v>
       </c>
       <c r="H55" s="1">
-        <f>(F55+G55)/2</f>
+        <f t="shared" si="2"/>
         <v>21.299999999999997</v>
       </c>
       <c r="I55" s="1">
@@ -4842,7 +4843,7 @@
         <v>10.3</v>
       </c>
       <c r="K55" s="1">
-        <f>(I55+J55)/2</f>
+        <f t="shared" si="3"/>
         <v>10.25</v>
       </c>
       <c r="L55" s="1" t="s">
@@ -4879,7 +4880,7 @@
         <v>111</v>
       </c>
       <c r="H56" s="1">
-        <f>(F56+G56)/2</f>
+        <f t="shared" si="2"/>
         <v>111.5</v>
       </c>
       <c r="I56" s="1">
@@ -4889,7 +4890,7 @@
         <v>72</v>
       </c>
       <c r="K56" s="1">
-        <f>(I56+J56)/2</f>
+        <f t="shared" si="3"/>
         <v>72.2</v>
       </c>
       <c r="L56" s="1">
@@ -4926,7 +4927,7 @@
         <v>72</v>
       </c>
       <c r="H57" s="1">
-        <f>(F57+G57)/2</f>
+        <f t="shared" si="2"/>
         <v>72.400000000000006</v>
       </c>
       <c r="I57" s="1">
@@ -4936,7 +4937,7 @@
         <v>55.4</v>
       </c>
       <c r="K57" s="1">
-        <f>(I57+J57)/2</f>
+        <f t="shared" si="3"/>
         <v>55.5</v>
       </c>
       <c r="L57" s="1">
@@ -4973,7 +4974,7 @@
         <v>81.400000000000006</v>
       </c>
       <c r="H58" s="1">
-        <f>(F58+G58)/2</f>
+        <f t="shared" si="2"/>
         <v>81.800000000000011</v>
       </c>
       <c r="I58" s="1">
@@ -4983,7 +4984,7 @@
         <v>60.4</v>
       </c>
       <c r="K58" s="1">
-        <f>(I58+J58)/2</f>
+        <f t="shared" si="3"/>
         <v>60.4</v>
       </c>
       <c r="L58" s="1">
@@ -5020,7 +5021,7 @@
         <v>65.2</v>
       </c>
       <c r="H59" s="1">
-        <f>(F59+G59)/2</f>
+        <f t="shared" si="2"/>
         <v>65.400000000000006</v>
       </c>
       <c r="I59" s="1">
@@ -5030,7 +5031,7 @@
         <v>34.799999999999997</v>
       </c>
       <c r="K59" s="1">
-        <f>(I59+J59)/2</f>
+        <f t="shared" si="3"/>
         <v>34.799999999999997</v>
       </c>
       <c r="L59" s="1">
@@ -5067,7 +5068,7 @@
         <v>18.3</v>
       </c>
       <c r="H60" s="1">
-        <f>(F60+G60)/2</f>
+        <f t="shared" si="2"/>
         <v>18.350000000000001</v>
       </c>
       <c r="I60" s="1">
@@ -5077,7 +5078,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="K60" s="1">
-        <f>(I60+J60)/2</f>
+        <f t="shared" si="3"/>
         <v>19.95</v>
       </c>
       <c r="L60" s="1">
@@ -5117,7 +5118,7 @@
   <dimension ref="A1:U42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5126,6 +5127,7 @@
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -5136,7 +5138,8 @@
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
-      <c r="F1" s="39"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
@@ -5157,6 +5160,9 @@
       <c r="F2" s="30" t="s">
         <v>72</v>
       </c>
+      <c r="G2" s="39" t="s">
+        <v>83</v>
+      </c>
       <c r="I2" s="36" t="s">
         <v>82</v>
       </c>
@@ -5182,6 +5188,10 @@
         <f>50-E3</f>
         <v>27.272727272727273</v>
       </c>
+      <c r="G3" s="31">
+        <f>90-E3</f>
+        <v>67.27272727272728</v>
+      </c>
       <c r="I3" s="32"/>
       <c r="J3" s="33">
         <v>1</v>
@@ -5241,6 +5251,10 @@
         <f t="shared" ref="F4:F42" si="1">50-E4</f>
         <v>26.635514018691588</v>
       </c>
+      <c r="G4" s="31">
+        <f t="shared" ref="G4:G42" si="2">90-E4</f>
+        <v>66.635514018691595</v>
+      </c>
       <c r="I4" s="34" t="s">
         <v>73</v>
       </c>
@@ -5302,6 +5316,10 @@
         <f t="shared" si="1"/>
         <v>26.525821596244132</v>
       </c>
+      <c r="G5" s="31">
+        <f t="shared" si="2"/>
+        <v>66.525821596244128</v>
+      </c>
       <c r="I5" s="34" t="s">
         <v>75</v>
       </c>
@@ -5363,6 +5381,10 @@
         <f t="shared" si="1"/>
         <v>35.294117647058826</v>
       </c>
+      <c r="G6" s="31">
+        <f t="shared" si="2"/>
+        <v>75.294117647058826</v>
+      </c>
       <c r="I6" s="34" t="s">
         <v>76</v>
       </c>
@@ -5424,6 +5446,10 @@
         <f t="shared" si="1"/>
         <v>33.766233766233768</v>
       </c>
+      <c r="G7" s="31">
+        <f t="shared" si="2"/>
+        <v>73.766233766233768</v>
+      </c>
       <c r="I7" s="34" t="s">
         <v>77</v>
       </c>
@@ -5485,6 +5511,10 @@
         <f t="shared" si="1"/>
         <v>19.512195121951216</v>
       </c>
+      <c r="G8" s="31">
+        <f t="shared" si="2"/>
+        <v>59.512195121951216</v>
+      </c>
       <c r="I8" s="34" t="s">
         <v>78</v>
       </c>
@@ -5546,6 +5576,10 @@
         <f t="shared" si="1"/>
         <v>36.413043478260867</v>
       </c>
+      <c r="G9" s="31">
+        <f t="shared" si="2"/>
+        <v>76.413043478260875</v>
+      </c>
       <c r="I9" s="34" t="s">
         <v>79</v>
       </c>
@@ -5607,6 +5641,10 @@
         <f t="shared" si="1"/>
         <v>36.772486772486772</v>
       </c>
+      <c r="G10" s="31">
+        <f t="shared" si="2"/>
+        <v>76.772486772486772</v>
+      </c>
       <c r="I10" s="34" t="s">
         <v>80</v>
       </c>
@@ -5668,6 +5706,10 @@
         <f t="shared" si="1"/>
         <v>33.333333333333329</v>
       </c>
+      <c r="G11" s="31">
+        <f t="shared" si="2"/>
+        <v>73.333333333333329</v>
+      </c>
       <c r="I11" s="34" t="s">
         <v>81</v>
       </c>
@@ -5729,6 +5771,10 @@
         <f t="shared" si="1"/>
         <v>38.839285714285715</v>
       </c>
+      <c r="G12" s="31">
+        <f t="shared" si="2"/>
+        <v>78.839285714285708</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
@@ -5751,6 +5797,10 @@
         <f t="shared" si="1"/>
         <v>32.817869415807564</v>
       </c>
+      <c r="G13" s="31">
+        <f t="shared" si="2"/>
+        <v>72.817869415807564</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
@@ -5773,6 +5823,10 @@
         <f t="shared" si="1"/>
         <v>32.57839721254355</v>
       </c>
+      <c r="G14" s="31">
+        <f t="shared" si="2"/>
+        <v>72.57839721254355</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -5795,6 +5849,10 @@
         <f t="shared" si="1"/>
         <v>33.713355048859938</v>
       </c>
+      <c r="G15" s="31">
+        <f t="shared" si="2"/>
+        <v>73.713355048859938</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
@@ -5817,8 +5875,12 @@
         <f t="shared" si="1"/>
         <v>40.27237354085603</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="31">
+        <f t="shared" si="2"/>
+        <v>80.272373540856023</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>25</v>
       </c>
@@ -5839,8 +5901,12 @@
         <f t="shared" si="1"/>
         <v>34.227129337539431</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="31">
+        <f t="shared" si="2"/>
+        <v>74.227129337539438</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>31</v>
       </c>
@@ -5861,8 +5927,12 @@
         <f t="shared" si="1"/>
         <v>28.260869565217391</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="31">
+        <f t="shared" si="2"/>
+        <v>68.260869565217391</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>56</v>
       </c>
@@ -5883,8 +5953,12 @@
         <f t="shared" si="1"/>
         <v>23.262032085561497</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="31">
+        <f t="shared" si="2"/>
+        <v>63.262032085561501</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>42</v>
       </c>
@@ -5905,8 +5979,12 @@
         <f t="shared" si="1"/>
         <v>41.197183098591552</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="31">
+        <f t="shared" si="2"/>
+        <v>81.197183098591552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>49</v>
       </c>
@@ -5927,8 +6005,12 @@
         <f t="shared" si="1"/>
         <v>23.118279569892476</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="31">
+        <f t="shared" si="2"/>
+        <v>63.118279569892479</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
@@ -5949,8 +6031,12 @@
         <f t="shared" si="1"/>
         <v>21.014492753623188</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="31">
+        <f t="shared" si="2"/>
+        <v>61.014492753623188</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>41</v>
       </c>
@@ -5971,8 +6057,12 @@
         <f t="shared" si="1"/>
         <v>34.756097560975604</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="31">
+        <f t="shared" si="2"/>
+        <v>74.756097560975604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
@@ -5993,8 +6083,12 @@
         <f t="shared" si="1"/>
         <v>13.099630996309962</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G24" s="31">
+        <f t="shared" si="2"/>
+        <v>53.099630996309962</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
         <v>29</v>
       </c>
@@ -6015,8 +6109,12 @@
         <f t="shared" si="1"/>
         <v>43.169398907103826</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="31">
+        <f t="shared" si="2"/>
+        <v>83.169398907103826</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
         <v>46</v>
       </c>
@@ -6037,8 +6135,12 @@
         <f t="shared" si="1"/>
         <v>18.84735202492212</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="31">
+        <f t="shared" si="2"/>
+        <v>58.847352024922117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
         <v>39</v>
       </c>
@@ -6059,8 +6161,12 @@
         <f t="shared" si="1"/>
         <v>5.3571428571428541</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="31">
+        <f t="shared" si="2"/>
+        <v>45.357142857142854</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
         <v>53</v>
       </c>
@@ -6081,8 +6187,12 @@
         <f t="shared" si="1"/>
         <v>36.449864498644985</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="31">
+        <f t="shared" si="2"/>
+        <v>76.449864498644985</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
         <v>49</v>
       </c>
@@ -6103,8 +6213,12 @@
         <f t="shared" si="1"/>
         <v>30.76923076923077</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="31">
+        <f t="shared" si="2"/>
+        <v>70.769230769230774</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" s="5" t="s">
         <v>27</v>
       </c>
@@ -6125,8 +6239,12 @@
         <f t="shared" si="1"/>
         <v>10.784313725490193</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="31">
+        <f t="shared" si="2"/>
+        <v>50.784313725490193</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="5" t="s">
         <v>30</v>
       </c>
@@ -6147,8 +6265,12 @@
         <f t="shared" si="1"/>
         <v>43.455497382198956</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="31">
+        <f t="shared" si="2"/>
+        <v>83.455497382198956</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
         <v>32</v>
       </c>
@@ -6169,8 +6291,12 @@
         <f t="shared" si="1"/>
         <v>43.016759776536311</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="31">
+        <f t="shared" si="2"/>
+        <v>83.016759776536318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
         <v>48</v>
       </c>
@@ -6191,8 +6317,12 @@
         <f t="shared" si="1"/>
         <v>39.106753812636164</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="31">
+        <f t="shared" si="2"/>
+        <v>79.106753812636171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="5" t="s">
         <v>25</v>
       </c>
@@ -6213,8 +6343,12 @@
         <f t="shared" si="1"/>
         <v>38.713318284424375</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="31">
+        <f t="shared" si="2"/>
+        <v>78.713318284424375</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="5" t="s">
         <v>54</v>
       </c>
@@ -6235,8 +6369,12 @@
         <f t="shared" si="1"/>
         <v>29.674796747967481</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G35" s="31">
+        <f t="shared" si="2"/>
+        <v>69.674796747967477</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
         <v>56</v>
       </c>
@@ -6257,8 +6395,12 @@
         <f t="shared" si="1"/>
         <v>37.531172069825438</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G36" s="31">
+        <f t="shared" si="2"/>
+        <v>77.531172069825431</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
         <v>51</v>
       </c>
@@ -6279,8 +6421,12 @@
         <f t="shared" si="1"/>
         <v>1.2195121951219505</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G37" s="31">
+        <f t="shared" si="2"/>
+        <v>41.219512195121951</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
         <v>47</v>
       </c>
@@ -6301,8 +6447,12 @@
         <f t="shared" si="1"/>
         <v>43.074792243767313</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G38" s="31">
+        <f t="shared" si="2"/>
+        <v>83.07479224376732</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
         <v>52</v>
       </c>
@@ -6323,8 +6473,12 @@
         <f t="shared" si="1"/>
         <v>40.990990990990994</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G39" s="31">
+        <f t="shared" si="2"/>
+        <v>80.990990990990994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="5" t="s">
         <v>42</v>
       </c>
@@ -6345,8 +6499,12 @@
         <f t="shared" si="1"/>
         <v>41.721854304635762</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G40" s="31">
+        <f t="shared" si="2"/>
+        <v>81.721854304635755</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="5" t="s">
         <v>55</v>
       </c>
@@ -6367,8 +6525,12 @@
         <f t="shared" si="1"/>
         <v>35.632183908045974</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G41" s="31">
+        <f t="shared" si="2"/>
+        <v>75.632183908045974</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="5" t="s">
         <v>50</v>
       </c>
@@ -6389,10 +6551,14 @@
         <f t="shared" si="1"/>
         <v>24.937343358395989</v>
       </c>
+      <c r="G42" s="31">
+        <f t="shared" si="2"/>
+        <v>64.937343358395992</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
reextractions to the molecular labwork spreadsheet
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3153ACD7-A090-9949-9A49-85E39B9DFE3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D2EEB-77AB-5F48-A52A-8AB54291BAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
     <sheet name="DNARNA-Extractions" sheetId="2" r:id="rId2"/>
-    <sheet name="Tag-Seq-Prep" sheetId="3" r:id="rId3"/>
+    <sheet name="Gene-Exp-Prep" sheetId="3" r:id="rId3"/>
+    <sheet name="Re-extractions" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNARNA-Extractions'!$A$1:$O$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Master-ID-List'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Re-extractions'!$A$1:$N$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,8 +40,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={73296C14-D2C9-424E-8C07-D4EA2F848CA6}</author>
+  </authors>
+  <commentList>
+    <comment ref="H3" authorId="0" shapeId="0" xr:uid="{73296C14-D2C9-424E-8C07-D4EA2F848CA6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    RNASeq = 1.2 ug needed</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="97">
   <si>
     <t>ColonyID</t>
   </si>
@@ -287,10 +307,49 @@
     <t>H</t>
   </si>
   <si>
-    <t>Platemap to ship (by extraction ID)</t>
-  </si>
-  <si>
     <t>RNA remaining (uL)</t>
+  </si>
+  <si>
+    <t>RNA remaining (ug)</t>
+  </si>
+  <si>
+    <t>TagSeq Prep</t>
+  </si>
+  <si>
+    <t>Remaining after TagSeq</t>
+  </si>
+  <si>
+    <t>TagSeq platemap to ship (by extraction ID)</t>
+  </si>
+  <si>
+    <t>Sample information</t>
+  </si>
+  <si>
+    <t>RNASeq Prep</t>
+  </si>
+  <si>
+    <t>1.2 ug required</t>
+  </si>
+  <si>
+    <t>Re-extraction ID</t>
+  </si>
+  <si>
+    <t>Re-extraction Date</t>
+  </si>
+  <si>
+    <t>RNASeq platemap to ship (by extraction ID)</t>
+  </si>
+  <si>
+    <t>Not enough - reextract</t>
+  </si>
+  <si>
+    <t>Couldn’t find this fragment - we may not have any left. Just send the RNA we have from the first round</t>
+  </si>
+  <si>
+    <t>DNA is much more degraded than the December fragments</t>
+  </si>
+  <si>
+    <t>TBD</t>
   </si>
 </sst>
 </file>
@@ -355,7 +414,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +439,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -507,17 +578,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -533,27 +593,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -562,7 +605,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -593,27 +636,60 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -649,6 +725,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Emma Strand" id="{F73CA9BE-36C0-FD41-835C-C556E7F3470F}" userId="S::emma_strand@uri.edu::7f67b1d4-a6d0-4bf6-a787-44c695b65a06" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -946,6 +1028,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H3" dT="2021-10-25T14:49:35.14" personId="{F73CA9BE-36C0-FD41-835C-C556E7F3470F}" id="{73296C14-D2C9-424E-8C07-D4EA2F848CA6}">
+    <text>RNASeq = 1.2 ug needed</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B1C6750-7F92-2244-B10F-B37DA4CD9192}">
   <sheetPr>
@@ -2168,7 +2258,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3827,7 +3917,7 @@
         <v>63.4</v>
       </c>
       <c r="H34" s="1">
-        <f t="shared" ref="H34:H65" si="2">(F34+G34)/2</f>
+        <f t="shared" ref="H34:H60" si="2">(F34+G34)/2</f>
         <v>63.8</v>
       </c>
       <c r="I34" s="1">
@@ -3837,7 +3927,7 @@
         <v>51.2</v>
       </c>
       <c r="K34" s="1">
-        <f t="shared" ref="K34:K65" si="3">(I34+J34)/2</f>
+        <f t="shared" ref="K34:K60" si="3">(I34+J34)/2</f>
         <v>51.400000000000006</v>
       </c>
       <c r="L34" s="1">
@@ -5099,12 +5189,12 @@
   </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="N1:N7 N15:N28 N37:N1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N29:N36">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",N29)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5114,11 +5204,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036899D6-E256-F041-A042-E7C6544A897B}">
-  <dimension ref="A1:U42"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{036899D6-E256-F041-A042-E7C6544A897B}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:W43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5128,1438 +5221,2589 @@
     <col min="5" max="5" width="16.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.5" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="9" width="18.83203125" customWidth="1"/>
+    <col min="10" max="10" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="J1" s="41"/>
+    </row>
+    <row r="2" spans="1:23" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="44"/>
+      <c r="I2" s="41" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="41"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="I3" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27">
+        <v>22</v>
+      </c>
+      <c r="E4" s="28">
+        <f>500/D4</f>
+        <v>22.727272727272727</v>
+      </c>
+      <c r="F4" s="28">
+        <f>50-E4</f>
+        <v>27.272727272727273</v>
+      </c>
+      <c r="G4" s="28">
+        <f>90-E4</f>
+        <v>67.27272727272728</v>
+      </c>
+      <c r="H4" s="28">
+        <f>(D4*G4)/1000</f>
+        <v>1.4800000000000002</v>
+      </c>
+      <c r="I4" s="28">
+        <f>1.2/(D4/1000)</f>
+        <v>54.545454545454547</v>
+      </c>
+      <c r="K4" s="29"/>
+      <c r="L4" s="30">
+        <v>1</v>
+      </c>
+      <c r="M4" s="30">
+        <v>2</v>
+      </c>
+      <c r="N4" s="30">
+        <v>3</v>
+      </c>
+      <c r="O4" s="30">
+        <v>4</v>
+      </c>
+      <c r="P4" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>6</v>
+      </c>
+      <c r="R4" s="30">
+        <v>7</v>
+      </c>
+      <c r="S4" s="30">
+        <v>8</v>
+      </c>
+      <c r="T4" s="30">
+        <v>9</v>
+      </c>
+      <c r="U4" s="30">
+        <v>10</v>
+      </c>
+      <c r="V4" s="30">
+        <v>11</v>
+      </c>
+      <c r="W4" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27">
+        <v>21.4</v>
+      </c>
+      <c r="E5" s="28">
+        <f t="shared" ref="E5:E43" si="0">500/D5</f>
+        <v>23.364485981308412</v>
+      </c>
+      <c r="F5" s="28">
+        <f t="shared" ref="F5:F43" si="1">50-E5</f>
+        <v>26.635514018691588</v>
+      </c>
+      <c r="G5" s="28">
+        <f t="shared" ref="G5:G43" si="2">90-E5</f>
+        <v>66.635514018691595</v>
+      </c>
+      <c r="H5" s="28">
+        <f t="shared" ref="H5:H43" si="3">(D5*G5)/1000</f>
+        <v>1.4259999999999999</v>
+      </c>
+      <c r="I5" s="28">
+        <f t="shared" ref="I5:I43" si="4">1.2/(D5/1000)</f>
+        <v>56.074766355140184</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L5" s="32">
+        <v>2</v>
+      </c>
+      <c r="M5" s="32">
+        <v>23</v>
+      </c>
+      <c r="N5" s="32">
+        <v>32</v>
+      </c>
+      <c r="O5" s="32">
+        <v>41</v>
+      </c>
+      <c r="P5" s="32">
+        <v>51</v>
+      </c>
+      <c r="Q5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="27">
+        <v>6</v>
+      </c>
+      <c r="D6" s="27">
+        <v>21.3</v>
+      </c>
+      <c r="E6" s="28">
+        <f t="shared" si="0"/>
+        <v>23.474178403755868</v>
+      </c>
+      <c r="F6" s="28">
+        <f t="shared" si="1"/>
+        <v>26.525821596244132</v>
+      </c>
+      <c r="G6" s="28">
+        <f t="shared" si="2"/>
+        <v>66.525821596244128</v>
+      </c>
+      <c r="H6" s="28">
+        <f t="shared" si="3"/>
+        <v>1.417</v>
+      </c>
+      <c r="I6" s="28">
+        <f t="shared" si="4"/>
+        <v>56.338028169014081</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="32">
+        <v>4</v>
+      </c>
+      <c r="M6" s="32">
+        <v>24</v>
+      </c>
+      <c r="N6" s="32">
+        <v>33</v>
+      </c>
+      <c r="O6" s="32">
+        <v>42</v>
+      </c>
+      <c r="P6" s="32">
+        <v>52</v>
+      </c>
+      <c r="Q6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V6" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W6" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="27">
+        <v>16</v>
+      </c>
+      <c r="D7" s="27">
+        <v>34</v>
+      </c>
+      <c r="E7" s="28">
+        <f t="shared" si="0"/>
+        <v>14.705882352941176</v>
+      </c>
+      <c r="F7" s="28">
+        <f t="shared" si="1"/>
+        <v>35.294117647058826</v>
+      </c>
+      <c r="G7" s="28">
+        <f t="shared" si="2"/>
+        <v>75.294117647058826</v>
+      </c>
+      <c r="H7" s="28">
+        <f t="shared" si="3"/>
+        <v>2.56</v>
+      </c>
+      <c r="I7" s="28">
+        <f t="shared" si="4"/>
+        <v>35.294117647058819</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="L7" s="32">
+        <v>6</v>
+      </c>
+      <c r="M7" s="32">
+        <v>25</v>
+      </c>
+      <c r="N7" s="32">
+        <v>34</v>
+      </c>
+      <c r="O7" s="32">
+        <v>43</v>
+      </c>
+      <c r="P7" s="32">
+        <v>53</v>
+      </c>
+      <c r="Q7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V7" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W7" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="27">
+        <v>17</v>
+      </c>
+      <c r="D8" s="27">
+        <v>30.8</v>
+      </c>
+      <c r="E8" s="28">
+        <f t="shared" si="0"/>
+        <v>16.233766233766232</v>
+      </c>
+      <c r="F8" s="28">
+        <f t="shared" si="1"/>
+        <v>33.766233766233768</v>
+      </c>
+      <c r="G8" s="28">
+        <f t="shared" si="2"/>
+        <v>73.766233766233768</v>
+      </c>
+      <c r="H8" s="28">
+        <f t="shared" si="3"/>
+        <v>2.2719999999999998</v>
+      </c>
+      <c r="I8" s="28">
+        <f t="shared" si="4"/>
+        <v>38.961038961038959</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="L8" s="32">
+        <v>16</v>
+      </c>
+      <c r="M8" s="32">
+        <v>26</v>
+      </c>
+      <c r="N8" s="32">
+        <v>35</v>
+      </c>
+      <c r="O8" s="32">
+        <v>44</v>
+      </c>
+      <c r="P8" s="32">
+        <v>54</v>
+      </c>
+      <c r="Q8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V8" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W8" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="27">
+        <v>18</v>
+      </c>
+      <c r="D9" s="27">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="E9" s="28">
+        <f t="shared" si="0"/>
+        <v>30.487804878048784</v>
+      </c>
+      <c r="F9" s="28">
+        <f t="shared" si="1"/>
+        <v>19.512195121951216</v>
+      </c>
+      <c r="G9" s="28">
+        <f t="shared" si="2"/>
+        <v>59.512195121951216</v>
+      </c>
+      <c r="H9" s="28">
+        <f t="shared" si="3"/>
+        <v>0.97599999999999987</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L9" s="32">
+        <v>17</v>
+      </c>
+      <c r="M9" s="32">
+        <v>28</v>
+      </c>
+      <c r="N9" s="32">
+        <v>37</v>
+      </c>
+      <c r="O9" s="32">
+        <v>45</v>
+      </c>
+      <c r="P9" s="32">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V9" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W9" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="27">
+        <v>21</v>
+      </c>
+      <c r="D10" s="27">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="E10" s="28">
+        <f t="shared" si="0"/>
+        <v>13.586956521739131</v>
+      </c>
+      <c r="F10" s="28">
+        <f t="shared" si="1"/>
+        <v>36.413043478260867</v>
+      </c>
+      <c r="G10" s="28">
+        <f t="shared" si="2"/>
+        <v>76.413043478260875</v>
+      </c>
+      <c r="H10" s="28">
+        <f t="shared" si="3"/>
+        <v>2.8119999999999998</v>
+      </c>
+      <c r="I10" s="28">
+        <f t="shared" si="4"/>
+        <v>32.608695652173914</v>
+      </c>
+      <c r="K10" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L10" s="32">
+        <v>18</v>
+      </c>
+      <c r="M10" s="32">
+        <v>29</v>
+      </c>
+      <c r="N10" s="32">
+        <v>38</v>
+      </c>
+      <c r="O10" s="32">
+        <v>46</v>
+      </c>
+      <c r="P10" s="32">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V10" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W10" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="27">
+        <v>22</v>
+      </c>
+      <c r="D11" s="27">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="E11" s="28">
+        <f t="shared" si="0"/>
+        <v>13.227513227513228</v>
+      </c>
+      <c r="F11" s="28">
+        <f t="shared" si="1"/>
+        <v>36.772486772486772</v>
+      </c>
+      <c r="G11" s="28">
+        <f t="shared" si="2"/>
+        <v>76.772486772486772</v>
+      </c>
+      <c r="H11" s="28">
+        <f t="shared" si="3"/>
+        <v>2.9019999999999997</v>
+      </c>
+      <c r="I11" s="28">
+        <f t="shared" si="4"/>
+        <v>31.746031746031743</v>
+      </c>
+      <c r="K11" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L11" s="32">
+        <v>21</v>
+      </c>
+      <c r="M11" s="32">
+        <v>30</v>
+      </c>
+      <c r="N11" s="32">
+        <v>39</v>
+      </c>
+      <c r="O11" s="32">
+        <v>47</v>
+      </c>
+      <c r="P11" s="32">
+        <v>57</v>
+      </c>
+      <c r="Q11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V11" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W11" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="27">
+        <v>23</v>
+      </c>
+      <c r="D12" s="27">
+        <v>30</v>
+      </c>
+      <c r="E12" s="28">
+        <f t="shared" si="0"/>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="F12" s="28">
+        <f t="shared" si="1"/>
+        <v>33.333333333333329</v>
+      </c>
+      <c r="G12" s="28">
+        <f t="shared" si="2"/>
+        <v>73.333333333333329</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="3"/>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="K12" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="L12" s="32">
+        <v>22</v>
+      </c>
+      <c r="M12" s="32">
+        <v>31</v>
+      </c>
+      <c r="N12" s="32">
+        <v>40</v>
+      </c>
+      <c r="O12" s="32">
+        <v>50</v>
+      </c>
+      <c r="P12" s="32">
+        <v>59</v>
+      </c>
+      <c r="Q12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V12" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W12" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="27">
+        <v>24</v>
+      </c>
+      <c r="D13" s="27">
+        <v>44.8</v>
+      </c>
+      <c r="E13" s="28">
+        <f t="shared" si="0"/>
+        <v>11.160714285714286</v>
+      </c>
+      <c r="F13" s="28">
+        <f t="shared" si="1"/>
+        <v>38.839285714285715</v>
+      </c>
+      <c r="G13" s="28">
+        <f t="shared" si="2"/>
+        <v>78.839285714285708</v>
+      </c>
+      <c r="H13" s="28">
+        <f t="shared" si="3"/>
+        <v>3.5319999999999996</v>
+      </c>
+      <c r="I13" s="28">
+        <f t="shared" si="4"/>
+        <v>26.785714285714285</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="27">
+        <v>25</v>
+      </c>
+      <c r="D14" s="27">
+        <v>29.1</v>
+      </c>
+      <c r="E14" s="28">
+        <f t="shared" si="0"/>
+        <v>17.182130584192439</v>
+      </c>
+      <c r="F14" s="28">
+        <f t="shared" si="1"/>
+        <v>32.817869415807564</v>
+      </c>
+      <c r="G14" s="28">
+        <f t="shared" si="2"/>
+        <v>72.817869415807564</v>
+      </c>
+      <c r="H14" s="28">
+        <f t="shared" si="3"/>
+        <v>2.1190000000000002</v>
+      </c>
+      <c r="I14" s="28">
+        <f t="shared" si="4"/>
+        <v>41.237113402061851</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="27">
+        <v>26</v>
+      </c>
+      <c r="D15" s="27">
+        <v>28.7</v>
+      </c>
+      <c r="E15" s="28">
+        <f t="shared" si="0"/>
+        <v>17.421602787456447</v>
+      </c>
+      <c r="F15" s="28">
+        <f t="shared" si="1"/>
+        <v>32.57839721254355</v>
+      </c>
+      <c r="G15" s="28">
+        <f t="shared" si="2"/>
+        <v>72.57839721254355</v>
+      </c>
+      <c r="H15" s="28">
+        <f t="shared" si="3"/>
+        <v>2.0830000000000002</v>
+      </c>
+      <c r="I15" s="28">
+        <f t="shared" si="4"/>
+        <v>41.811846689895468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="27">
+        <v>28</v>
+      </c>
+      <c r="D16" s="27">
+        <v>30.7</v>
+      </c>
+      <c r="E16" s="28">
+        <f t="shared" si="0"/>
+        <v>16.286644951140065</v>
+      </c>
+      <c r="F16" s="28">
+        <f t="shared" si="1"/>
+        <v>33.713355048859938</v>
+      </c>
+      <c r="G16" s="28">
+        <f t="shared" si="2"/>
+        <v>73.713355048859938</v>
+      </c>
+      <c r="H16" s="28">
+        <f t="shared" si="3"/>
+        <v>2.2629999999999999</v>
+      </c>
+      <c r="I16" s="28">
+        <f t="shared" si="4"/>
+        <v>39.087947882736159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="27">
+        <v>29</v>
+      </c>
+      <c r="D17" s="27">
+        <v>51.4</v>
+      </c>
+      <c r="E17" s="28">
+        <f t="shared" si="0"/>
+        <v>9.7276264591439698</v>
+      </c>
+      <c r="F17" s="28">
+        <f t="shared" si="1"/>
+        <v>40.27237354085603</v>
+      </c>
+      <c r="G17" s="28">
+        <f t="shared" si="2"/>
+        <v>80.272373540856023</v>
+      </c>
+      <c r="H17" s="28">
+        <f t="shared" si="3"/>
+        <v>4.1259999999999994</v>
+      </c>
+      <c r="I17" s="28">
+        <f t="shared" si="4"/>
+        <v>23.346303501945524</v>
+      </c>
+      <c r="K17" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="27">
+        <v>30</v>
+      </c>
+      <c r="D18" s="27">
+        <v>31.7</v>
+      </c>
+      <c r="E18" s="28">
+        <f t="shared" si="0"/>
+        <v>15.772870662460567</v>
+      </c>
+      <c r="F18" s="28">
+        <f t="shared" si="1"/>
+        <v>34.227129337539431</v>
+      </c>
+      <c r="G18" s="28">
+        <f t="shared" si="2"/>
+        <v>74.227129337539438</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" si="3"/>
+        <v>2.3530000000000002</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" si="4"/>
+        <v>37.854889589905362</v>
+      </c>
+      <c r="K18" s="29"/>
+      <c r="L18" s="30">
+        <v>1</v>
+      </c>
+      <c r="M18" s="30">
+        <v>2</v>
+      </c>
+      <c r="N18" s="30">
+        <v>3</v>
+      </c>
+      <c r="O18" s="30">
+        <v>4</v>
+      </c>
+      <c r="P18" s="30">
+        <v>5</v>
+      </c>
+      <c r="Q18" s="30">
+        <v>6</v>
+      </c>
+      <c r="R18" s="30">
+        <v>7</v>
+      </c>
+      <c r="S18" s="30">
+        <v>8</v>
+      </c>
+      <c r="T18" s="30">
+        <v>9</v>
+      </c>
+      <c r="U18" s="30">
+        <v>10</v>
+      </c>
+      <c r="V18" s="30">
+        <v>11</v>
+      </c>
+      <c r="W18" s="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="27">
+        <v>31</v>
+      </c>
+      <c r="D19" s="27">
+        <v>23</v>
+      </c>
+      <c r="E19" s="28">
+        <f t="shared" si="0"/>
+        <v>21.739130434782609</v>
+      </c>
+      <c r="F19" s="28">
+        <f t="shared" si="1"/>
+        <v>28.260869565217391</v>
+      </c>
+      <c r="G19" s="28">
+        <f t="shared" si="2"/>
+        <v>68.260869565217391</v>
+      </c>
+      <c r="H19" s="28">
+        <f t="shared" si="3"/>
+        <v>1.57</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="4"/>
+        <v>52.173913043478258</v>
+      </c>
+      <c r="K19" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V19" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W19" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="27">
+        <v>32</v>
+      </c>
+      <c r="D20" s="27">
+        <v>18.7</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" si="0"/>
+        <v>26.737967914438503</v>
+      </c>
+      <c r="F20" s="28">
+        <f t="shared" si="1"/>
+        <v>23.262032085561497</v>
+      </c>
+      <c r="G20" s="28">
+        <f t="shared" si="2"/>
+        <v>63.262032085561501</v>
+      </c>
+      <c r="H20" s="28">
+        <f t="shared" si="3"/>
+        <v>1.1830000000000001</v>
+      </c>
+      <c r="I20" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="31" t="s">
+        <v>75</v>
+      </c>
+      <c r="L20" s="32"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="32"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W20" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" s="27">
+        <v>33</v>
+      </c>
+      <c r="D21" s="27">
+        <v>56.8</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" si="0"/>
+        <v>8.8028169014084519</v>
+      </c>
+      <c r="F21" s="28">
+        <f t="shared" si="1"/>
+        <v>41.197183098591552</v>
+      </c>
+      <c r="G21" s="28">
+        <f t="shared" si="2"/>
+        <v>81.197183098591552</v>
+      </c>
+      <c r="H21" s="28">
+        <f t="shared" si="3"/>
+        <v>4.6120000000000001</v>
+      </c>
+      <c r="I21" s="28">
+        <f t="shared" si="4"/>
+        <v>21.126760563380284</v>
+      </c>
+      <c r="K21" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="L21" s="32"/>
+      <c r="M21" s="32"/>
+      <c r="N21" s="32"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="32"/>
+      <c r="Q21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V21" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W21" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="27">
+        <v>34</v>
+      </c>
+      <c r="D22" s="27">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="E22" s="28">
+        <f t="shared" si="0"/>
+        <v>26.881720430107524</v>
+      </c>
+      <c r="F22" s="28">
+        <f t="shared" si="1"/>
+        <v>23.118279569892476</v>
+      </c>
+      <c r="G22" s="28">
+        <f t="shared" si="2"/>
+        <v>63.118279569892479</v>
+      </c>
+      <c r="H22" s="28">
+        <f t="shared" si="3"/>
+        <v>1.1740000000000002</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="32"/>
+      <c r="Q22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V22" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W22" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C23" s="27">
+        <v>35</v>
+      </c>
+      <c r="D23" s="27">
+        <v>17.25</v>
+      </c>
+      <c r="E23" s="28">
+        <f t="shared" si="0"/>
+        <v>28.985507246376812</v>
+      </c>
+      <c r="F23" s="28">
+        <f t="shared" si="1"/>
+        <v>21.014492753623188</v>
+      </c>
+      <c r="G23" s="28">
+        <f t="shared" si="2"/>
+        <v>61.014492753623188</v>
+      </c>
+      <c r="H23" s="28">
+        <f t="shared" si="3"/>
+        <v>1.0525</v>
+      </c>
+      <c r="I23" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="L23" s="32"/>
+      <c r="M23" s="32"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="32"/>
+      <c r="Q23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V23" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W23" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="27">
+        <v>37</v>
+      </c>
+      <c r="D24" s="27">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" si="0"/>
+        <v>15.243902439024392</v>
+      </c>
+      <c r="F24" s="28">
+        <f t="shared" si="1"/>
+        <v>34.756097560975604</v>
+      </c>
+      <c r="G24" s="28">
+        <f t="shared" si="2"/>
+        <v>74.756097560975604</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" si="3"/>
+        <v>2.4519999999999995</v>
+      </c>
+      <c r="I24" s="28">
+        <f t="shared" si="4"/>
+        <v>36.585365853658537</v>
+      </c>
+      <c r="K24" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="L24" s="32"/>
+      <c r="M24" s="32"/>
+      <c r="N24" s="32"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="32"/>
+      <c r="Q24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V24" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W24" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="27">
+        <v>38</v>
+      </c>
+      <c r="D25" s="27">
+        <v>13.55</v>
+      </c>
+      <c r="E25" s="28">
+        <f t="shared" si="0"/>
+        <v>36.900369003690038</v>
+      </c>
+      <c r="F25" s="28">
+        <f t="shared" si="1"/>
+        <v>13.099630996309962</v>
+      </c>
+      <c r="G25" s="28">
+        <f t="shared" si="2"/>
+        <v>53.099630996309962</v>
+      </c>
+      <c r="H25" s="28">
+        <f t="shared" si="3"/>
+        <v>0.71950000000000003</v>
+      </c>
+      <c r="I25" t="s">
+        <v>22</v>
+      </c>
+      <c r="K25" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="32"/>
+      <c r="M25" s="32"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V25" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W25" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="27">
+        <v>39</v>
+      </c>
+      <c r="D26" s="27">
+        <v>73.2</v>
+      </c>
+      <c r="E26" s="28">
+        <f t="shared" si="0"/>
+        <v>6.8306010928961749</v>
+      </c>
+      <c r="F26" s="28">
+        <f t="shared" si="1"/>
+        <v>43.169398907103826</v>
+      </c>
+      <c r="G26" s="28">
+        <f t="shared" si="2"/>
+        <v>83.169398907103826</v>
+      </c>
+      <c r="H26" s="28">
+        <f t="shared" si="3"/>
+        <v>6.0880000000000001</v>
+      </c>
+      <c r="I26" s="28">
+        <f t="shared" si="4"/>
+        <v>16.393442622950818</v>
+      </c>
+      <c r="K26" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="L26" s="39"/>
+      <c r="M26" s="32"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="32"/>
+      <c r="Q26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="R26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="S26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="T26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="U26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="V26" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="W26" s="29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="27">
+        <v>40</v>
+      </c>
+      <c r="D27" s="27">
+        <v>16.05</v>
+      </c>
+      <c r="E27" s="28">
+        <f t="shared" si="0"/>
+        <v>31.15264797507788</v>
+      </c>
+      <c r="F27" s="28">
+        <f t="shared" si="1"/>
+        <v>18.84735202492212</v>
+      </c>
+      <c r="G27" s="28">
+        <f t="shared" si="2"/>
+        <v>58.847352024922117</v>
+      </c>
+      <c r="H27" s="28">
+        <f t="shared" si="3"/>
+        <v>0.94450000000000001</v>
+      </c>
+      <c r="I27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="27">
+        <v>41</v>
+      </c>
+      <c r="D28" s="27">
+        <v>11.2</v>
+      </c>
+      <c r="E28" s="28">
+        <f t="shared" si="0"/>
+        <v>44.642857142857146</v>
+      </c>
+      <c r="F28" s="28">
+        <f t="shared" si="1"/>
+        <v>5.3571428571428541</v>
+      </c>
+      <c r="G28" s="28">
+        <f t="shared" si="2"/>
+        <v>45.357142857142854</v>
+      </c>
+      <c r="H28" s="28">
+        <f t="shared" si="3"/>
+        <v>0.5079999999999999</v>
+      </c>
+      <c r="I28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="27">
+        <v>42</v>
+      </c>
+      <c r="D29" s="27">
+        <v>36.9</v>
+      </c>
+      <c r="E29" s="28">
+        <f t="shared" si="0"/>
+        <v>13.550135501355014</v>
+      </c>
+      <c r="F29" s="28">
+        <f t="shared" si="1"/>
+        <v>36.449864498644985</v>
+      </c>
+      <c r="G29" s="28">
+        <f t="shared" si="2"/>
+        <v>76.449864498644985</v>
+      </c>
+      <c r="H29" s="28">
+        <f t="shared" si="3"/>
+        <v>2.8210000000000002</v>
+      </c>
+      <c r="I29" s="28">
+        <f t="shared" si="4"/>
+        <v>32.520325203252035</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="27">
+        <v>43</v>
+      </c>
+      <c r="D30" s="27">
+        <v>26</v>
+      </c>
+      <c r="E30" s="28">
+        <f t="shared" si="0"/>
+        <v>19.23076923076923</v>
+      </c>
+      <c r="F30" s="28">
+        <f t="shared" si="1"/>
+        <v>30.76923076923077</v>
+      </c>
+      <c r="G30" s="28">
+        <f t="shared" si="2"/>
+        <v>70.769230769230774</v>
+      </c>
+      <c r="H30" s="28">
+        <f t="shared" si="3"/>
+        <v>1.84</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" si="4"/>
+        <v>46.153846153846153</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="27">
+        <v>44</v>
+      </c>
+      <c r="D31" s="27">
+        <v>12.75</v>
+      </c>
+      <c r="E31" s="28">
+        <f t="shared" si="0"/>
+        <v>39.215686274509807</v>
+      </c>
+      <c r="F31" s="28">
+        <f t="shared" si="1"/>
+        <v>10.784313725490193</v>
+      </c>
+      <c r="G31" s="28">
+        <f t="shared" si="2"/>
+        <v>50.784313725490193</v>
+      </c>
+      <c r="H31" s="28">
+        <f t="shared" si="3"/>
+        <v>0.64749999999999996</v>
+      </c>
+      <c r="I31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="27">
+        <v>45</v>
+      </c>
+      <c r="D32" s="27">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="E32" s="28">
+        <f t="shared" si="0"/>
+        <v>6.5445026178010464</v>
+      </c>
+      <c r="F32" s="28">
+        <f t="shared" si="1"/>
+        <v>43.455497382198956</v>
+      </c>
+      <c r="G32" s="28">
+        <f t="shared" si="2"/>
+        <v>83.455497382198956</v>
+      </c>
+      <c r="H32" s="28">
+        <f t="shared" si="3"/>
+        <v>6.3760000000000012</v>
+      </c>
+      <c r="I32" s="28">
+        <f t="shared" si="4"/>
+        <v>15.706806282722511</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="27">
+        <v>46</v>
+      </c>
+      <c r="D33" s="27">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="E33" s="28">
+        <f t="shared" si="0"/>
+        <v>6.9832402234636879</v>
+      </c>
+      <c r="F33" s="28">
+        <f t="shared" si="1"/>
+        <v>43.016759776536311</v>
+      </c>
+      <c r="G33" s="28">
+        <f t="shared" si="2"/>
+        <v>83.016759776536318</v>
+      </c>
+      <c r="H33" s="28">
+        <f t="shared" si="3"/>
+        <v>5.944</v>
+      </c>
+      <c r="I33" s="28">
+        <f t="shared" si="4"/>
+        <v>16.759776536312849</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="27">
+        <v>47</v>
+      </c>
+      <c r="D34" s="27">
+        <v>45.9</v>
+      </c>
+      <c r="E34" s="28">
+        <f t="shared" si="0"/>
+        <v>10.893246187363834</v>
+      </c>
+      <c r="F34" s="28">
+        <f t="shared" si="1"/>
+        <v>39.106753812636164</v>
+      </c>
+      <c r="G34" s="28">
+        <f t="shared" si="2"/>
+        <v>79.106753812636171</v>
+      </c>
+      <c r="H34" s="28">
+        <f t="shared" si="3"/>
+        <v>3.6309999999999998</v>
+      </c>
+      <c r="I34" s="28">
+        <f t="shared" si="4"/>
+        <v>26.143790849673202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C35" s="27">
+        <v>50</v>
+      </c>
+      <c r="D35" s="27">
+        <v>44.3</v>
+      </c>
+      <c r="E35" s="28">
+        <f t="shared" si="0"/>
+        <v>11.286681715575622</v>
+      </c>
+      <c r="F35" s="28">
+        <f t="shared" si="1"/>
+        <v>38.713318284424375</v>
+      </c>
+      <c r="G35" s="28">
+        <f t="shared" si="2"/>
+        <v>78.713318284424375</v>
+      </c>
+      <c r="H35" s="28">
+        <f t="shared" si="3"/>
+        <v>3.4869999999999997</v>
+      </c>
+      <c r="I35" s="28">
+        <f t="shared" si="4"/>
+        <v>27.088036117381488</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C36" s="27">
+        <v>51</v>
+      </c>
+      <c r="D36" s="27">
+        <v>24.6</v>
+      </c>
+      <c r="E36" s="28">
+        <f t="shared" si="0"/>
+        <v>20.325203252032519</v>
+      </c>
+      <c r="F36" s="28">
+        <f t="shared" si="1"/>
+        <v>29.674796747967481</v>
+      </c>
+      <c r="G36" s="28">
+        <f t="shared" si="2"/>
+        <v>69.674796747967477</v>
+      </c>
+      <c r="H36" s="28">
+        <f t="shared" si="3"/>
+        <v>1.714</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" si="4"/>
+        <v>48.780487804878049</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" s="27">
+        <v>52</v>
+      </c>
+      <c r="D37" s="27">
+        <v>40.1</v>
+      </c>
+      <c r="E37" s="28">
+        <f t="shared" si="0"/>
+        <v>12.468827930174562</v>
+      </c>
+      <c r="F37" s="28">
+        <f t="shared" si="1"/>
+        <v>37.531172069825438</v>
+      </c>
+      <c r="G37" s="28">
+        <f t="shared" si="2"/>
+        <v>77.531172069825431</v>
+      </c>
+      <c r="H37" s="28">
+        <f t="shared" si="3"/>
+        <v>3.109</v>
+      </c>
+      <c r="I37" s="28">
+        <f t="shared" si="4"/>
+        <v>29.92518703241895</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" s="27">
+        <v>53</v>
+      </c>
+      <c r="D38" s="27">
+        <v>10.25</v>
+      </c>
+      <c r="E38" s="28">
+        <f t="shared" si="0"/>
+        <v>48.780487804878049</v>
+      </c>
+      <c r="F38" s="28">
+        <f t="shared" si="1"/>
+        <v>1.2195121951219505</v>
+      </c>
+      <c r="G38" s="28">
+        <f t="shared" si="2"/>
+        <v>41.219512195121951</v>
+      </c>
+      <c r="H38" s="28">
+        <f t="shared" si="3"/>
+        <v>0.42249999999999999</v>
+      </c>
+      <c r="I38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="27">
+        <v>54</v>
+      </c>
+      <c r="D39" s="27">
+        <v>72.2</v>
+      </c>
+      <c r="E39" s="28">
+        <f t="shared" si="0"/>
+        <v>6.9252077562326866</v>
+      </c>
+      <c r="F39" s="28">
+        <f t="shared" si="1"/>
+        <v>43.074792243767313</v>
+      </c>
+      <c r="G39" s="28">
+        <f t="shared" si="2"/>
+        <v>83.07479224376732</v>
+      </c>
+      <c r="H39" s="28">
+        <f t="shared" si="3"/>
+        <v>5.9980000000000011</v>
+      </c>
+      <c r="I39" s="28">
+        <f t="shared" si="4"/>
+        <v>16.620498614958446</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B40" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" s="27">
+        <v>55</v>
+      </c>
+      <c r="D40" s="27">
+        <v>55.5</v>
+      </c>
+      <c r="E40" s="28">
+        <f t="shared" si="0"/>
+        <v>9.0090090090090094</v>
+      </c>
+      <c r="F40" s="28">
+        <f t="shared" si="1"/>
+        <v>40.990990990990994</v>
+      </c>
+      <c r="G40" s="28">
+        <f t="shared" si="2"/>
+        <v>80.990990990990994</v>
+      </c>
+      <c r="H40" s="28">
+        <f t="shared" si="3"/>
+        <v>4.4950000000000001</v>
+      </c>
+      <c r="I40" s="28">
+        <f t="shared" si="4"/>
+        <v>21.621621621621621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" s="27">
+        <v>56</v>
+      </c>
+      <c r="D41" s="27">
+        <v>60.4</v>
+      </c>
+      <c r="E41" s="28">
+        <f t="shared" si="0"/>
+        <v>8.2781456953642394</v>
+      </c>
+      <c r="F41" s="28">
+        <f t="shared" si="1"/>
+        <v>41.721854304635762</v>
+      </c>
+      <c r="G41" s="28">
+        <f t="shared" si="2"/>
+        <v>81.721854304635755</v>
+      </c>
+      <c r="H41" s="28">
+        <f t="shared" si="3"/>
+        <v>4.9359999999999991</v>
+      </c>
+      <c r="I41" s="28">
+        <f t="shared" si="4"/>
+        <v>19.867549668874172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="27">
+        <v>57</v>
+      </c>
+      <c r="D42" s="27">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="E42" s="28">
+        <f t="shared" si="0"/>
+        <v>14.367816091954024</v>
+      </c>
+      <c r="F42" s="28">
+        <f t="shared" si="1"/>
+        <v>35.632183908045974</v>
+      </c>
+      <c r="G42" s="28">
+        <f t="shared" si="2"/>
+        <v>75.632183908045974</v>
+      </c>
+      <c r="H42" s="28">
+        <f t="shared" si="3"/>
+        <v>2.6319999999999997</v>
+      </c>
+      <c r="I42" s="28">
+        <f t="shared" si="4"/>
+        <v>34.482758620689658</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43" s="27">
+        <v>59</v>
+      </c>
+      <c r="D43" s="27">
+        <v>19.95</v>
+      </c>
+      <c r="E43" s="28">
+        <f t="shared" si="0"/>
+        <v>25.062656641604011</v>
+      </c>
+      <c r="F43" s="28">
+        <f t="shared" si="1"/>
+        <v>24.937343358395989</v>
+      </c>
+      <c r="G43" s="28">
+        <f t="shared" si="2"/>
+        <v>64.937343358395992</v>
+      </c>
+      <c r="H43" s="28">
+        <f t="shared" si="3"/>
+        <v>1.2955000000000001</v>
+      </c>
+      <c r="I43" s="28">
+        <f t="shared" si="4"/>
+        <v>60.150375939849624</v>
+      </c>
+      <c r="J43" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H4:H43">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>1.2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="36" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B47553-AD92-3A4E-A1D2-704B4666022D}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="14" max="14" width="86.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" s="36" customFormat="1" ht="69" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B1" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D2" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="39" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C1" s="37" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="E1" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="38" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="38" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="38" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="L1" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2">
+        <v>60</v>
+      </c>
+      <c r="D2">
+        <v>20211028</v>
+      </c>
+      <c r="E2">
+        <v>28.4</v>
+      </c>
+      <c r="F2">
+        <v>28.2</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G7" si="0">(E2+F2)/2</f>
+        <v>28.299999999999997</v>
+      </c>
+      <c r="H2">
+        <v>13.6</v>
+      </c>
+      <c r="I2">
+        <v>13.7</v>
+      </c>
+      <c r="J2">
+        <f>(H2+I2)/2</f>
+        <v>13.649999999999999</v>
+      </c>
+      <c r="K2">
+        <v>8.4</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="27">
-        <v>2</v>
-      </c>
-      <c r="D3" s="27">
-        <v>22</v>
-      </c>
-      <c r="E3" s="31">
-        <f>500/D3</f>
-        <v>22.727272727272727</v>
-      </c>
-      <c r="F3" s="31">
-        <f>50-E3</f>
-        <v>27.272727272727273</v>
-      </c>
-      <c r="G3" s="31">
-        <f>90-E3</f>
-        <v>67.27272727272728</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="33">
-        <v>1</v>
-      </c>
-      <c r="K3" s="33">
-        <v>2</v>
-      </c>
-      <c r="L3" s="33">
-        <v>3</v>
-      </c>
-      <c r="M3" s="33">
-        <v>4</v>
-      </c>
-      <c r="N3" s="33">
-        <v>5</v>
-      </c>
-      <c r="O3" s="33">
-        <v>6</v>
-      </c>
-      <c r="P3" s="33">
-        <v>7</v>
-      </c>
-      <c r="Q3" s="33">
-        <v>8</v>
-      </c>
-      <c r="R3" s="33">
-        <v>9</v>
-      </c>
-      <c r="S3" s="33">
-        <v>10</v>
-      </c>
-      <c r="T3" s="33">
-        <v>11</v>
-      </c>
-      <c r="U3" s="33">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>61</v>
+      </c>
+      <c r="D3">
+        <v>20211028</v>
+      </c>
+      <c r="E3">
+        <v>35.4</v>
+      </c>
+      <c r="F3">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>35.299999999999997</v>
+      </c>
+      <c r="H3">
+        <v>18.2</v>
+      </c>
+      <c r="I3">
+        <v>18.2</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J10" si="1">(H3+I3)/2</f>
+        <v>18.2</v>
+      </c>
+      <c r="K3">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="27">
-        <v>4</v>
-      </c>
-      <c r="D4" s="27">
-        <v>21.4</v>
-      </c>
-      <c r="E4" s="31">
-        <f t="shared" ref="E4:E42" si="0">500/D4</f>
-        <v>23.364485981308412</v>
-      </c>
-      <c r="F4" s="31">
-        <f t="shared" ref="F4:F42" si="1">50-E4</f>
-        <v>26.635514018691588</v>
-      </c>
-      <c r="G4" s="31">
-        <f t="shared" ref="G4:G42" si="2">90-E4</f>
-        <v>66.635514018691595</v>
-      </c>
-      <c r="I4" s="34" t="s">
-        <v>73</v>
-      </c>
-      <c r="J4" s="35">
-        <v>2</v>
-      </c>
-      <c r="K4" s="35">
-        <v>23</v>
-      </c>
-      <c r="L4" s="35">
+        <v>27</v>
+      </c>
+      <c r="B4" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4">
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>20211028</v>
+      </c>
+      <c r="E4">
+        <v>52.4</v>
+      </c>
+      <c r="F4">
+        <v>52.2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>52.3</v>
+      </c>
+      <c r="H4">
+        <v>19.5</v>
+      </c>
+      <c r="I4">
+        <v>19.5</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="1"/>
+        <v>19.5</v>
+      </c>
+      <c r="K4">
+        <v>8.4</v>
+      </c>
+      <c r="L4" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5">
+        <v>63</v>
+      </c>
+      <c r="D5">
+        <v>20211028</v>
+      </c>
+      <c r="E5">
+        <v>55.8</v>
+      </c>
+      <c r="F5">
+        <v>55.6</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>55.7</v>
+      </c>
+      <c r="H5">
         <v>32</v>
       </c>
-      <c r="M4" s="35">
-        <v>41</v>
-      </c>
-      <c r="N4" s="35">
+      <c r="I5">
+        <v>32</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="K5">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="L5" t="s">
+        <v>61</v>
+      </c>
+      <c r="M5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N5" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="O4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T4" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U4" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="27">
-        <v>6</v>
-      </c>
-      <c r="D5" s="27">
-        <v>21.3</v>
-      </c>
-      <c r="E5" s="31">
+      <c r="B6" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6">
+        <v>64</v>
+      </c>
+      <c r="D6">
+        <v>20211028</v>
+      </c>
+      <c r="E6">
+        <v>101</v>
+      </c>
+      <c r="F6">
+        <v>101</v>
+      </c>
+      <c r="G6">
         <f t="shared" si="0"/>
-        <v>23.474178403755868</v>
-      </c>
-      <c r="F5" s="31">
+        <v>101</v>
+      </c>
+      <c r="H6">
+        <v>49.4</v>
+      </c>
+      <c r="I6">
+        <v>49.4</v>
+      </c>
+      <c r="J6">
         <f t="shared" si="1"/>
-        <v>26.525821596244132</v>
-      </c>
-      <c r="G5" s="31">
-        <f t="shared" si="2"/>
-        <v>66.525821596244128</v>
-      </c>
-      <c r="I5" s="34" t="s">
-        <v>75</v>
-      </c>
-      <c r="J5" s="35">
-        <v>4</v>
-      </c>
-      <c r="K5" s="35">
-        <v>24</v>
-      </c>
-      <c r="L5" s="35">
-        <v>33</v>
-      </c>
-      <c r="M5" s="35">
-        <v>42</v>
-      </c>
-      <c r="N5" s="35">
-        <v>52</v>
-      </c>
-      <c r="O5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T5" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U5" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="27">
-        <v>16</v>
-      </c>
-      <c r="D6" s="27">
-        <v>34</v>
-      </c>
-      <c r="E6" s="31">
-        <f t="shared" si="0"/>
-        <v>14.705882352941176</v>
-      </c>
-      <c r="F6" s="31">
-        <f t="shared" si="1"/>
-        <v>35.294117647058826</v>
-      </c>
-      <c r="G6" s="31">
-        <f t="shared" si="2"/>
-        <v>75.294117647058826</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>76</v>
-      </c>
-      <c r="J6" s="35">
-        <v>6</v>
-      </c>
-      <c r="K6" s="35">
-        <v>25</v>
-      </c>
-      <c r="L6" s="35">
-        <v>34</v>
-      </c>
-      <c r="M6" s="35">
-        <v>43</v>
-      </c>
-      <c r="N6" s="35">
-        <v>53</v>
-      </c>
-      <c r="O6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T6" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U6" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+        <v>49.4</v>
+      </c>
+      <c r="K6">
+        <v>8.4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="27">
-        <v>17</v>
-      </c>
-      <c r="D7" s="27">
-        <v>30.8</v>
-      </c>
-      <c r="E7" s="31">
+      <c r="C7">
+        <v>65</v>
+      </c>
+      <c r="D7">
+        <v>20211029</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>29.8</v>
+      </c>
+      <c r="G7">
         <f t="shared" si="0"/>
-        <v>16.233766233766232</v>
-      </c>
-      <c r="F7" s="31">
+        <v>29.9</v>
+      </c>
+      <c r="H7">
+        <v>19.2</v>
+      </c>
+      <c r="I7">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
-        <v>33.766233766233768</v>
-      </c>
-      <c r="G7" s="31">
-        <f t="shared" si="2"/>
-        <v>73.766233766233768</v>
-      </c>
-      <c r="I7" s="34" t="s">
-        <v>77</v>
-      </c>
-      <c r="J7" s="35">
-        <v>16</v>
-      </c>
-      <c r="K7" s="35">
-        <v>26</v>
-      </c>
-      <c r="L7" s="35">
-        <v>35</v>
-      </c>
-      <c r="M7" s="35">
-        <v>44</v>
-      </c>
-      <c r="N7" s="35">
-        <v>54</v>
-      </c>
-      <c r="O7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T7" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U7" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="K7" s="40">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="L7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="27">
-        <v>18</v>
-      </c>
-      <c r="D8" s="27">
-        <v>16.399999999999999</v>
-      </c>
-      <c r="E8" s="31">
-        <f t="shared" si="0"/>
-        <v>30.487804878048784</v>
-      </c>
-      <c r="F8" s="31">
+      <c r="C8">
+        <v>66</v>
+      </c>
+      <c r="D8">
+        <v>20211029</v>
+      </c>
+      <c r="E8">
+        <v>46.8</v>
+      </c>
+      <c r="F8">
+        <v>46.6</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G10" si="2">(E8+F8)/2</f>
+        <v>46.7</v>
+      </c>
+      <c r="H8">
+        <v>48.6</v>
+      </c>
+      <c r="I8">
+        <v>48.6</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
-        <v>19.512195121951216</v>
-      </c>
-      <c r="G8" s="31">
+        <v>48.6</v>
+      </c>
+      <c r="K8" s="40">
+        <v>9.1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>33</v>
+      </c>
+      <c r="M8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9">
+        <v>68</v>
+      </c>
+      <c r="D9">
+        <v>20211029</v>
+      </c>
+      <c r="E9">
+        <v>46.4</v>
+      </c>
+      <c r="F9">
+        <v>46.4</v>
+      </c>
+      <c r="G9">
         <f t="shared" si="2"/>
-        <v>59.512195121951216</v>
-      </c>
-      <c r="I8" s="34" t="s">
-        <v>78</v>
-      </c>
-      <c r="J8" s="35">
-        <v>17</v>
-      </c>
-      <c r="K8" s="35">
-        <v>28</v>
-      </c>
-      <c r="L8" s="35">
-        <v>37</v>
-      </c>
-      <c r="M8" s="35">
-        <v>45</v>
-      </c>
-      <c r="N8" s="35">
-        <v>55</v>
-      </c>
-      <c r="O8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T8" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U8" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
+        <v>46.4</v>
+      </c>
+      <c r="H9">
+        <v>31.8</v>
+      </c>
+      <c r="I9">
+        <v>31.8</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="1"/>
+        <v>31.8</v>
+      </c>
+      <c r="K9" s="40">
+        <v>5.6</v>
+      </c>
+      <c r="L9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10">
+        <v>67</v>
+      </c>
+      <c r="D10">
+        <v>20211029</v>
+      </c>
+      <c r="E10">
+        <v>62.8</v>
+      </c>
+      <c r="F10">
+        <v>62.6</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>62.7</v>
+      </c>
+      <c r="H10">
+        <v>27</v>
+      </c>
+      <c r="I10">
+        <v>27</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="K10" s="40">
+        <v>8.9</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
+      </c>
+      <c r="M10" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="27">
-        <v>21</v>
-      </c>
-      <c r="D9" s="27">
-        <v>36.799999999999997</v>
-      </c>
-      <c r="E9" s="31">
-        <f t="shared" si="0"/>
-        <v>13.586956521739131</v>
-      </c>
-      <c r="F9" s="31">
-        <f t="shared" si="1"/>
-        <v>36.413043478260867</v>
-      </c>
-      <c r="G9" s="31">
-        <f t="shared" si="2"/>
-        <v>76.413043478260875</v>
-      </c>
-      <c r="I9" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="35">
-        <v>18</v>
-      </c>
-      <c r="K9" s="35">
-        <v>29</v>
-      </c>
-      <c r="L9" s="35">
-        <v>38</v>
-      </c>
-      <c r="M9" s="35">
-        <v>46</v>
-      </c>
-      <c r="N9" s="35">
-        <v>56</v>
-      </c>
-      <c r="O9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T9" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U9" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="27">
-        <v>22</v>
-      </c>
-      <c r="D10" s="27">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="E10" s="31">
-        <f t="shared" si="0"/>
-        <v>13.227513227513228</v>
-      </c>
-      <c r="F10" s="31">
-        <f t="shared" si="1"/>
-        <v>36.772486772486772</v>
-      </c>
-      <c r="G10" s="31">
-        <f t="shared" si="2"/>
-        <v>76.772486772486772</v>
-      </c>
-      <c r="I10" s="34" t="s">
-        <v>80</v>
-      </c>
-      <c r="J10" s="35">
-        <v>21</v>
-      </c>
-      <c r="K10" s="35">
-        <v>30</v>
-      </c>
-      <c r="L10" s="35">
-        <v>39</v>
-      </c>
-      <c r="M10" s="35">
-        <v>47</v>
-      </c>
-      <c r="N10" s="35">
-        <v>57</v>
-      </c>
-      <c r="O10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T10" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U10" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="B11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="27">
-        <v>23</v>
-      </c>
-      <c r="D11" s="27">
-        <v>30</v>
-      </c>
-      <c r="E11" s="31">
-        <f t="shared" si="0"/>
-        <v>16.666666666666668</v>
-      </c>
-      <c r="F11" s="31">
-        <f t="shared" si="1"/>
-        <v>33.333333333333329</v>
-      </c>
-      <c r="G11" s="31">
-        <f t="shared" si="2"/>
-        <v>73.333333333333329</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="J11" s="35">
-        <v>22</v>
-      </c>
-      <c r="K11" s="35">
-        <v>31</v>
-      </c>
-      <c r="L11" s="35">
-        <v>40</v>
-      </c>
-      <c r="M11" s="35">
-        <v>50</v>
-      </c>
-      <c r="N11" s="35">
-        <v>59</v>
-      </c>
-      <c r="O11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="P11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="R11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="S11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="T11" s="32" t="s">
-        <v>74</v>
-      </c>
-      <c r="U11" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="27">
-        <v>24</v>
-      </c>
-      <c r="D12" s="27">
-        <v>44.8</v>
-      </c>
-      <c r="E12" s="31">
-        <f t="shared" si="0"/>
-        <v>11.160714285714286</v>
-      </c>
-      <c r="F12" s="31">
-        <f t="shared" si="1"/>
-        <v>38.839285714285715</v>
-      </c>
-      <c r="G12" s="31">
-        <f t="shared" si="2"/>
-        <v>78.839285714285708</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="27">
-        <v>25</v>
-      </c>
-      <c r="D13" s="27">
-        <v>29.1</v>
-      </c>
-      <c r="E13" s="31">
-        <f t="shared" si="0"/>
-        <v>17.182130584192439</v>
-      </c>
-      <c r="F13" s="31">
-        <f t="shared" si="1"/>
-        <v>32.817869415807564</v>
-      </c>
-      <c r="G13" s="31">
-        <f t="shared" si="2"/>
-        <v>72.817869415807564</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="27">
-        <v>26</v>
-      </c>
-      <c r="D14" s="27">
-        <v>28.7</v>
-      </c>
-      <c r="E14" s="31">
-        <f t="shared" si="0"/>
-        <v>17.421602787456447</v>
-      </c>
-      <c r="F14" s="31">
-        <f t="shared" si="1"/>
-        <v>32.57839721254355</v>
-      </c>
-      <c r="G14" s="31">
-        <f t="shared" si="2"/>
-        <v>72.57839721254355</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="27">
-        <v>28</v>
-      </c>
-      <c r="D15" s="27">
-        <v>30.7</v>
-      </c>
-      <c r="E15" s="31">
-        <f t="shared" si="0"/>
-        <v>16.286644951140065</v>
-      </c>
-      <c r="F15" s="31">
-        <f t="shared" si="1"/>
-        <v>33.713355048859938</v>
-      </c>
-      <c r="G15" s="31">
-        <f t="shared" si="2"/>
-        <v>73.713355048859938</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="27">
-        <v>29</v>
-      </c>
-      <c r="D16" s="27">
-        <v>51.4</v>
-      </c>
-      <c r="E16" s="31">
-        <f t="shared" si="0"/>
-        <v>9.7276264591439698</v>
-      </c>
-      <c r="F16" s="31">
-        <f t="shared" si="1"/>
-        <v>40.27237354085603</v>
-      </c>
-      <c r="G16" s="31">
-        <f t="shared" si="2"/>
-        <v>80.272373540856023</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C17" s="27">
-        <v>30</v>
-      </c>
-      <c r="D17" s="27">
-        <v>31.7</v>
-      </c>
-      <c r="E17" s="31">
-        <f t="shared" si="0"/>
-        <v>15.772870662460567</v>
-      </c>
-      <c r="F17" s="31">
-        <f t="shared" si="1"/>
-        <v>34.227129337539431</v>
-      </c>
-      <c r="G17" s="31">
-        <f t="shared" si="2"/>
-        <v>74.227129337539438</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="27">
-        <v>31</v>
-      </c>
-      <c r="D18" s="27">
-        <v>23</v>
-      </c>
-      <c r="E18" s="31">
-        <f t="shared" si="0"/>
-        <v>21.739130434782609</v>
-      </c>
-      <c r="F18" s="31">
-        <f t="shared" si="1"/>
-        <v>28.260869565217391</v>
-      </c>
-      <c r="G18" s="31">
-        <f t="shared" si="2"/>
-        <v>68.260869565217391</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="27">
-        <v>32</v>
-      </c>
-      <c r="D19" s="27">
-        <v>18.7</v>
-      </c>
-      <c r="E19" s="31">
-        <f t="shared" si="0"/>
-        <v>26.737967914438503</v>
-      </c>
-      <c r="F19" s="31">
-        <f t="shared" si="1"/>
-        <v>23.262032085561497</v>
-      </c>
-      <c r="G19" s="31">
-        <f t="shared" si="2"/>
-        <v>63.262032085561501</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="27">
-        <v>33</v>
-      </c>
-      <c r="D20" s="27">
-        <v>56.8</v>
-      </c>
-      <c r="E20" s="31">
-        <f t="shared" si="0"/>
-        <v>8.8028169014084519</v>
-      </c>
-      <c r="F20" s="31">
-        <f t="shared" si="1"/>
-        <v>41.197183098591552</v>
-      </c>
-      <c r="G20" s="31">
-        <f t="shared" si="2"/>
-        <v>81.197183098591552</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="27">
-        <v>34</v>
-      </c>
-      <c r="D21" s="27">
-        <v>18.600000000000001</v>
-      </c>
-      <c r="E21" s="31">
-        <f t="shared" si="0"/>
-        <v>26.881720430107524</v>
-      </c>
-      <c r="F21" s="31">
-        <f t="shared" si="1"/>
-        <v>23.118279569892476</v>
-      </c>
-      <c r="G21" s="31">
-        <f t="shared" si="2"/>
-        <v>63.118279569892479</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="27">
-        <v>35</v>
-      </c>
-      <c r="D22" s="27">
-        <v>17.25</v>
-      </c>
-      <c r="E22" s="31">
-        <f t="shared" si="0"/>
-        <v>28.985507246376812</v>
-      </c>
-      <c r="F22" s="31">
-        <f t="shared" si="1"/>
-        <v>21.014492753623188</v>
-      </c>
-      <c r="G22" s="31">
-        <f t="shared" si="2"/>
-        <v>61.014492753623188</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C23" s="27">
-        <v>37</v>
-      </c>
-      <c r="D23" s="27">
-        <v>32.799999999999997</v>
-      </c>
-      <c r="E23" s="31">
-        <f t="shared" si="0"/>
-        <v>15.243902439024392</v>
-      </c>
-      <c r="F23" s="31">
-        <f t="shared" si="1"/>
-        <v>34.756097560975604</v>
-      </c>
-      <c r="G23" s="31">
-        <f t="shared" si="2"/>
-        <v>74.756097560975604</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" s="27">
-        <v>38</v>
-      </c>
-      <c r="D24" s="27">
-        <v>13.55</v>
-      </c>
-      <c r="E24" s="31">
-        <f t="shared" si="0"/>
-        <v>36.900369003690038</v>
-      </c>
-      <c r="F24" s="31">
-        <f t="shared" si="1"/>
-        <v>13.099630996309962</v>
-      </c>
-      <c r="G24" s="31">
-        <f t="shared" si="2"/>
-        <v>53.099630996309962</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="27">
-        <v>39</v>
-      </c>
-      <c r="D25" s="27">
-        <v>73.2</v>
-      </c>
-      <c r="E25" s="31">
-        <f t="shared" si="0"/>
-        <v>6.8306010928961749</v>
-      </c>
-      <c r="F25" s="31">
-        <f t="shared" si="1"/>
-        <v>43.169398907103826</v>
-      </c>
-      <c r="G25" s="31">
-        <f t="shared" si="2"/>
-        <v>83.169398907103826</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B26" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="27">
-        <v>40</v>
-      </c>
-      <c r="D26" s="27">
-        <v>16.05</v>
-      </c>
-      <c r="E26" s="31">
-        <f t="shared" si="0"/>
-        <v>31.15264797507788</v>
-      </c>
-      <c r="F26" s="31">
-        <f t="shared" si="1"/>
-        <v>18.84735202492212</v>
-      </c>
-      <c r="G26" s="31">
-        <f t="shared" si="2"/>
-        <v>58.847352024922117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B27" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C27" s="27">
-        <v>41</v>
-      </c>
-      <c r="D27" s="27">
-        <v>11.2</v>
-      </c>
-      <c r="E27" s="31">
-        <f t="shared" si="0"/>
-        <v>44.642857142857146</v>
-      </c>
-      <c r="F27" s="31">
-        <f t="shared" si="1"/>
-        <v>5.3571428571428541</v>
-      </c>
-      <c r="G27" s="31">
-        <f t="shared" si="2"/>
-        <v>45.357142857142854</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="27">
-        <v>42</v>
-      </c>
-      <c r="D28" s="27">
-        <v>36.9</v>
-      </c>
-      <c r="E28" s="31">
-        <f t="shared" si="0"/>
-        <v>13.550135501355014</v>
-      </c>
-      <c r="F28" s="31">
-        <f t="shared" si="1"/>
-        <v>36.449864498644985</v>
-      </c>
-      <c r="G28" s="31">
-        <f t="shared" si="2"/>
-        <v>76.449864498644985</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="B29" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="27">
-        <v>43</v>
-      </c>
-      <c r="D29" s="27">
-        <v>26</v>
-      </c>
-      <c r="E29" s="31">
-        <f t="shared" si="0"/>
-        <v>19.23076923076923</v>
-      </c>
-      <c r="F29" s="31">
-        <f t="shared" si="1"/>
-        <v>30.76923076923077</v>
-      </c>
-      <c r="G29" s="31">
-        <f t="shared" si="2"/>
-        <v>70.769230769230774</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B30" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" s="27">
-        <v>44</v>
-      </c>
-      <c r="D30" s="27">
-        <v>12.75</v>
-      </c>
-      <c r="E30" s="31">
-        <f t="shared" si="0"/>
-        <v>39.215686274509807</v>
-      </c>
-      <c r="F30" s="31">
-        <f t="shared" si="1"/>
-        <v>10.784313725490193</v>
-      </c>
-      <c r="G30" s="31">
-        <f t="shared" si="2"/>
-        <v>50.784313725490193</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C31" s="27">
-        <v>45</v>
-      </c>
-      <c r="D31" s="27">
-        <v>76.400000000000006</v>
-      </c>
-      <c r="E31" s="31">
-        <f t="shared" si="0"/>
-        <v>6.5445026178010464</v>
-      </c>
-      <c r="F31" s="31">
-        <f t="shared" si="1"/>
-        <v>43.455497382198956</v>
-      </c>
-      <c r="G31" s="31">
-        <f t="shared" si="2"/>
-        <v>83.455497382198956</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C32" s="27">
-        <v>46</v>
-      </c>
-      <c r="D32" s="27">
-        <v>71.599999999999994</v>
-      </c>
-      <c r="E32" s="31">
-        <f t="shared" si="0"/>
-        <v>6.9832402234636879</v>
-      </c>
-      <c r="F32" s="31">
-        <f t="shared" si="1"/>
-        <v>43.016759776536311</v>
-      </c>
-      <c r="G32" s="31">
-        <f t="shared" si="2"/>
-        <v>83.016759776536318</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C33" s="27">
-        <v>47</v>
-      </c>
-      <c r="D33" s="27">
-        <v>45.9</v>
-      </c>
-      <c r="E33" s="31">
-        <f t="shared" si="0"/>
-        <v>10.893246187363834</v>
-      </c>
-      <c r="F33" s="31">
-        <f t="shared" si="1"/>
-        <v>39.106753812636164</v>
-      </c>
-      <c r="G33" s="31">
-        <f t="shared" si="2"/>
-        <v>79.106753812636171</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B34" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="27">
-        <v>50</v>
-      </c>
-      <c r="D34" s="27">
-        <v>44.3</v>
-      </c>
-      <c r="E34" s="31">
-        <f t="shared" si="0"/>
-        <v>11.286681715575622</v>
-      </c>
-      <c r="F34" s="31">
-        <f t="shared" si="1"/>
-        <v>38.713318284424375</v>
-      </c>
-      <c r="G34" s="31">
-        <f t="shared" si="2"/>
-        <v>78.713318284424375</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C35" s="27">
-        <v>51</v>
-      </c>
-      <c r="D35" s="27">
-        <v>24.6</v>
-      </c>
-      <c r="E35" s="31">
-        <f t="shared" si="0"/>
-        <v>20.325203252032519</v>
-      </c>
-      <c r="F35" s="31">
-        <f t="shared" si="1"/>
-        <v>29.674796747967481</v>
-      </c>
-      <c r="G35" s="31">
-        <f t="shared" si="2"/>
-        <v>69.674796747967477</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B36" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C36" s="27">
-        <v>52</v>
-      </c>
-      <c r="D36" s="27">
-        <v>40.1</v>
-      </c>
-      <c r="E36" s="31">
-        <f t="shared" si="0"/>
-        <v>12.468827930174562</v>
-      </c>
-      <c r="F36" s="31">
-        <f t="shared" si="1"/>
-        <v>37.531172069825438</v>
-      </c>
-      <c r="G36" s="31">
-        <f t="shared" si="2"/>
-        <v>77.531172069825431</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C37" s="27">
-        <v>53</v>
-      </c>
-      <c r="D37" s="27">
-        <v>10.25</v>
-      </c>
-      <c r="E37" s="31">
-        <f t="shared" si="0"/>
-        <v>48.780487804878049</v>
-      </c>
-      <c r="F37" s="31">
-        <f t="shared" si="1"/>
-        <v>1.2195121951219505</v>
-      </c>
-      <c r="G37" s="31">
-        <f t="shared" si="2"/>
-        <v>41.219512195121951</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="27">
-        <v>54</v>
-      </c>
-      <c r="D38" s="27">
-        <v>72.2</v>
-      </c>
-      <c r="E38" s="31">
-        <f t="shared" si="0"/>
-        <v>6.9252077562326866</v>
-      </c>
-      <c r="F38" s="31">
-        <f t="shared" si="1"/>
-        <v>43.074792243767313</v>
-      </c>
-      <c r="G38" s="31">
-        <f t="shared" si="2"/>
-        <v>83.07479224376732</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C39" s="27">
-        <v>55</v>
-      </c>
-      <c r="D39" s="27">
-        <v>55.5</v>
-      </c>
-      <c r="E39" s="31">
-        <f t="shared" si="0"/>
-        <v>9.0090090090090094</v>
-      </c>
-      <c r="F39" s="31">
-        <f t="shared" si="1"/>
-        <v>40.990990990990994</v>
-      </c>
-      <c r="G39" s="31">
-        <f t="shared" si="2"/>
-        <v>80.990990990990994</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A40" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" s="27">
-        <v>56</v>
-      </c>
-      <c r="D40" s="27">
-        <v>60.4</v>
-      </c>
-      <c r="E40" s="31">
-        <f t="shared" si="0"/>
-        <v>8.2781456953642394</v>
-      </c>
-      <c r="F40" s="31">
-        <f t="shared" si="1"/>
-        <v>41.721854304635762</v>
-      </c>
-      <c r="G40" s="31">
-        <f t="shared" si="2"/>
-        <v>81.721854304635755</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="C41" s="27">
-        <v>57</v>
-      </c>
-      <c r="D41" s="27">
-        <v>34.799999999999997</v>
-      </c>
-      <c r="E41" s="31">
-        <f t="shared" si="0"/>
-        <v>14.367816091954024</v>
-      </c>
-      <c r="F41" s="31">
-        <f t="shared" si="1"/>
-        <v>35.632183908045974</v>
-      </c>
-      <c r="G41" s="31">
-        <f t="shared" si="2"/>
-        <v>75.632183908045974</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A42" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B42" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C42" s="27">
-        <v>59</v>
-      </c>
-      <c r="D42" s="27">
-        <v>19.95</v>
-      </c>
-      <c r="E42" s="31">
-        <f t="shared" si="0"/>
-        <v>25.062656641604011</v>
-      </c>
-      <c r="F42" s="31">
-        <f t="shared" si="1"/>
-        <v>24.937343358395989</v>
-      </c>
-      <c r="G42" s="31">
-        <f t="shared" si="2"/>
-        <v>64.937343358395992</v>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+      <c r="L11" t="s">
+        <v>22</v>
+      </c>
+      <c r="M11" t="s">
+        <v>22</v>
+      </c>
+      <c r="N11" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
+  <conditionalFormatting sqref="M1">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",M1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
prep for RNASeq for the re-extracted corals
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D83D2EEB-77AB-5F48-A52A-8AB54291BAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA4CFEA-CD3B-BE4D-90E3-2E160D319E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="98">
   <si>
     <t>ColonyID</t>
   </si>
@@ -337,12 +337,6 @@
     <t>Re-extraction Date</t>
   </si>
   <si>
-    <t>RNASeq platemap to ship (by extraction ID)</t>
-  </si>
-  <si>
-    <t>Not enough - reextract</t>
-  </si>
-  <si>
     <t>Couldn’t find this fragment - we may not have any left. Just send the RNA we have from the first round</t>
   </si>
   <si>
@@ -350,6 +344,15 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Send as much as possible</t>
+  </si>
+  <si>
+    <t>see below</t>
+  </si>
+  <si>
+    <t>RNASeq shipped in individual 1.5 mL tubes (labeled by extraction ID)</t>
   </si>
 </sst>
 </file>
@@ -605,7 +608,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -649,8 +652,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -5208,10 +5215,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W43"/>
+  <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5226,40 +5233,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="41" t="s">
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="J1" s="41"/>
+      <c r="J1" s="45"/>
     </row>
     <row r="2" spans="1:23" s="5" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="45" t="s">
+      <c r="A2" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="44" t="s">
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="48" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44" t="s">
+      <c r="F2" s="48"/>
+      <c r="G2" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="41" t="s">
+      <c r="H2" s="48"/>
+      <c r="I2" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="J2" s="41"/>
+      <c r="J2" s="45"/>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" s="35" t="s">
@@ -5397,7 +5404,7 @@
         <v>1.4259999999999999</v>
       </c>
       <c r="I5" s="28">
-        <f t="shared" ref="I5:I43" si="4">1.2/(D5/1000)</f>
+        <f t="shared" ref="I5:I52" si="4">1.2/(D5/1000)</f>
         <v>56.074766355140184</v>
       </c>
       <c r="K5" s="31" t="s">
@@ -5691,6 +5698,9 @@
       <c r="I9" t="s">
         <v>22</v>
       </c>
+      <c r="J9" t="s">
+        <v>96</v>
+      </c>
       <c r="K9" s="31" t="s">
         <v>78</v>
       </c>
@@ -6017,6 +6027,9 @@
         <f t="shared" si="4"/>
         <v>41.237113402061851</v>
       </c>
+      <c r="K14" s="33" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
@@ -6119,9 +6132,6 @@
         <f t="shared" si="4"/>
         <v>23.346303501945524</v>
       </c>
-      <c r="K17" s="33" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
@@ -6156,43 +6166,19 @@
         <f t="shared" si="4"/>
         <v>37.854889589905362</v>
       </c>
-      <c r="K18" s="29"/>
-      <c r="L18" s="30">
-        <v>1</v>
-      </c>
-      <c r="M18" s="30">
-        <v>2</v>
-      </c>
-      <c r="N18" s="30">
-        <v>3</v>
-      </c>
-      <c r="O18" s="30">
-        <v>4</v>
-      </c>
-      <c r="P18" s="30">
-        <v>5</v>
-      </c>
-      <c r="Q18" s="30">
-        <v>6</v>
-      </c>
-      <c r="R18" s="30">
-        <v>7</v>
-      </c>
-      <c r="S18" s="30">
-        <v>8</v>
-      </c>
-      <c r="T18" s="30">
-        <v>9</v>
-      </c>
-      <c r="U18" s="30">
-        <v>10</v>
-      </c>
-      <c r="V18" s="30">
-        <v>11</v>
-      </c>
-      <c r="W18" s="30">
-        <v>12</v>
-      </c>
+      <c r="K18" s="40"/>
+      <c r="L18" s="41"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="41"/>
+      <c r="P18" s="41"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
@@ -6227,35 +6213,19 @@
         <f t="shared" si="4"/>
         <v>52.173913043478258</v>
       </c>
-      <c r="K19" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="32"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="32"/>
-      <c r="O19" s="32"/>
-      <c r="P19" s="32"/>
-      <c r="Q19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V19" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W19" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="K19" s="42"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
@@ -6289,35 +6259,22 @@
       <c r="I20" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="31" t="s">
-        <v>75</v>
-      </c>
-      <c r="L20" s="32"/>
-      <c r="M20" s="32"/>
-      <c r="N20" s="32"/>
-      <c r="O20" s="32"/>
-      <c r="P20" s="32"/>
-      <c r="Q20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V20" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W20" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="J20" t="s">
+        <v>96</v>
+      </c>
+      <c r="K20" s="42"/>
+      <c r="L20" s="43"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="43"/>
+      <c r="O20" s="43"/>
+      <c r="P20" s="43"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
@@ -6352,35 +6309,19 @@
         <f t="shared" si="4"/>
         <v>21.126760563380284</v>
       </c>
-      <c r="K21" s="31" t="s">
-        <v>76</v>
-      </c>
-      <c r="L21" s="32"/>
-      <c r="M21" s="32"/>
-      <c r="N21" s="32"/>
-      <c r="O21" s="32"/>
-      <c r="P21" s="32"/>
-      <c r="Q21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V21" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W21" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="K21" s="42"/>
+      <c r="L21" s="43"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="43"/>
+      <c r="O21" s="43"/>
+      <c r="P21" s="43"/>
+      <c r="Q21" s="40"/>
+      <c r="R21" s="40"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="40"/>
+      <c r="U21" s="40"/>
+      <c r="V21" s="40"/>
+      <c r="W21" s="40"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
@@ -6414,35 +6355,22 @@
       <c r="I22" t="s">
         <v>22</v>
       </c>
-      <c r="K22" s="31" t="s">
-        <v>77</v>
-      </c>
-      <c r="L22" s="32"/>
-      <c r="M22" s="32"/>
-      <c r="N22" s="32"/>
-      <c r="O22" s="32"/>
-      <c r="P22" s="32"/>
-      <c r="Q22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V22" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W22" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="J22" t="s">
+        <v>96</v>
+      </c>
+      <c r="K22" s="42"/>
+      <c r="L22" s="43"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="43"/>
+      <c r="Q22" s="40"/>
+      <c r="R22" s="40"/>
+      <c r="S22" s="40"/>
+      <c r="T22" s="40"/>
+      <c r="U22" s="40"/>
+      <c r="V22" s="40"/>
+      <c r="W22" s="40"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
@@ -6476,35 +6404,22 @@
       <c r="I23" t="s">
         <v>22</v>
       </c>
-      <c r="K23" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="L23" s="32"/>
-      <c r="M23" s="32"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="32"/>
-      <c r="Q23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V23" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W23" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="J23" t="s">
+        <v>96</v>
+      </c>
+      <c r="K23" s="42"/>
+      <c r="L23" s="43"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="43"/>
+      <c r="O23" s="43"/>
+      <c r="P23" s="43"/>
+      <c r="Q23" s="40"/>
+      <c r="R23" s="40"/>
+      <c r="S23" s="40"/>
+      <c r="T23" s="40"/>
+      <c r="U23" s="40"/>
+      <c r="V23" s="40"/>
+      <c r="W23" s="40"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
@@ -6539,35 +6454,19 @@
         <f t="shared" si="4"/>
         <v>36.585365853658537</v>
       </c>
-      <c r="K24" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="L24" s="32"/>
-      <c r="M24" s="32"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="32"/>
-      <c r="Q24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V24" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W24" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="K24" s="42"/>
+      <c r="L24" s="43"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="43"/>
+      <c r="P24" s="43"/>
+      <c r="Q24" s="40"/>
+      <c r="R24" s="40"/>
+      <c r="S24" s="40"/>
+      <c r="T24" s="40"/>
+      <c r="U24" s="40"/>
+      <c r="V24" s="40"/>
+      <c r="W24" s="40"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A25" s="5" t="s">
@@ -6601,35 +6500,22 @@
       <c r="I25" t="s">
         <v>22</v>
       </c>
-      <c r="K25" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="L25" s="32"/>
-      <c r="M25" s="32"/>
-      <c r="N25" s="32"/>
-      <c r="O25" s="32"/>
-      <c r="P25" s="32"/>
-      <c r="Q25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V25" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W25" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="J25" t="s">
+        <v>96</v>
+      </c>
+      <c r="K25" s="42"/>
+      <c r="L25" s="43"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="43"/>
+      <c r="O25" s="43"/>
+      <c r="P25" s="43"/>
+      <c r="Q25" s="40"/>
+      <c r="R25" s="40"/>
+      <c r="S25" s="40"/>
+      <c r="T25" s="40"/>
+      <c r="U25" s="40"/>
+      <c r="V25" s="40"/>
+      <c r="W25" s="40"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="5" t="s">
@@ -6664,35 +6550,19 @@
         <f t="shared" si="4"/>
         <v>16.393442622950818</v>
       </c>
-      <c r="K26" s="31" t="s">
-        <v>81</v>
-      </c>
-      <c r="L26" s="39"/>
-      <c r="M26" s="32"/>
-      <c r="N26" s="32"/>
-      <c r="O26" s="32"/>
-      <c r="P26" s="32"/>
-      <c r="Q26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="R26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="S26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="T26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="U26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="V26" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="W26" s="29" t="s">
-        <v>74</v>
-      </c>
+      <c r="K26" s="42"/>
+      <c r="L26" s="44"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="43"/>
+      <c r="O26" s="43"/>
+      <c r="P26" s="43"/>
+      <c r="Q26" s="40"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="40"/>
+      <c r="T26" s="40"/>
+      <c r="U26" s="40"/>
+      <c r="V26" s="40"/>
+      <c r="W26" s="40"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A27" s="5" t="s">
@@ -6726,6 +6596,22 @@
       <c r="I27" t="s">
         <v>22</v>
       </c>
+      <c r="J27" t="s">
+        <v>96</v>
+      </c>
+      <c r="K27" s="43"/>
+      <c r="L27" s="43"/>
+      <c r="M27" s="43"/>
+      <c r="N27" s="43"/>
+      <c r="O27" s="43"/>
+      <c r="P27" s="43"/>
+      <c r="Q27" s="43"/>
+      <c r="R27" s="43"/>
+      <c r="S27" s="43"/>
+      <c r="T27" s="43"/>
+      <c r="U27" s="43"/>
+      <c r="V27" s="43"/>
+      <c r="W27" s="43"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A28" s="5" t="s">
@@ -6759,6 +6645,22 @@
       <c r="I28" t="s">
         <v>22</v>
       </c>
+      <c r="J28" t="s">
+        <v>96</v>
+      </c>
+      <c r="K28" s="43"/>
+      <c r="L28" s="43"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="43"/>
+      <c r="O28" s="43"/>
+      <c r="P28" s="43"/>
+      <c r="Q28" s="43"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="43"/>
+      <c r="T28" s="43"/>
+      <c r="U28" s="43"/>
+      <c r="V28" s="43"/>
+      <c r="W28" s="43"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A29" s="5" t="s">
@@ -6860,6 +6762,9 @@
       <c r="I31" t="s">
         <v>22</v>
       </c>
+      <c r="J31" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
@@ -7097,6 +7002,9 @@
       <c r="I38" t="s">
         <v>22</v>
       </c>
+      <c r="J38" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="5" t="s">
@@ -7268,7 +7176,277 @@
         <v>60.150375939849624</v>
       </c>
       <c r="J43" t="s">
-        <v>93</v>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A44" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B44" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44">
+        <v>60</v>
+      </c>
+      <c r="D44" s="27">
+        <v>28.3</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" t="s">
+        <v>22</v>
+      </c>
+      <c r="G44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H44" t="s">
+        <v>22</v>
+      </c>
+      <c r="I44" s="28">
+        <f t="shared" si="4"/>
+        <v>42.402826855123671</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A45" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C45">
+        <v>61</v>
+      </c>
+      <c r="D45" s="27">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="E45" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" t="s">
+        <v>22</v>
+      </c>
+      <c r="G45" t="s">
+        <v>22</v>
+      </c>
+      <c r="H45" t="s">
+        <v>22</v>
+      </c>
+      <c r="I45" s="28">
+        <f t="shared" si="4"/>
+        <v>33.994334277620396</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A46" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B46" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46">
+        <v>62</v>
+      </c>
+      <c r="D46" s="27">
+        <v>52.3</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+      <c r="F46" t="s">
+        <v>22</v>
+      </c>
+      <c r="G46" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" t="s">
+        <v>22</v>
+      </c>
+      <c r="I46" s="28">
+        <f t="shared" si="4"/>
+        <v>22.94455066921606</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A47" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47">
+        <v>63</v>
+      </c>
+      <c r="D47" s="27">
+        <v>55.7</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+      <c r="F47" t="s">
+        <v>22</v>
+      </c>
+      <c r="G47" t="s">
+        <v>22</v>
+      </c>
+      <c r="H47" t="s">
+        <v>22</v>
+      </c>
+      <c r="I47" s="28">
+        <f t="shared" si="4"/>
+        <v>21.543985637342907</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B48" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48">
+        <v>64</v>
+      </c>
+      <c r="D48" s="27">
+        <v>101</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
+      </c>
+      <c r="F48" t="s">
+        <v>22</v>
+      </c>
+      <c r="G48" t="s">
+        <v>22</v>
+      </c>
+      <c r="H48" t="s">
+        <v>22</v>
+      </c>
+      <c r="I48" s="28">
+        <f t="shared" si="4"/>
+        <v>11.881188118811879</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A49" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B49" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49">
+        <v>65</v>
+      </c>
+      <c r="D49" s="27">
+        <v>29.9</v>
+      </c>
+      <c r="E49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F49" t="s">
+        <v>22</v>
+      </c>
+      <c r="G49" t="s">
+        <v>22</v>
+      </c>
+      <c r="H49" t="s">
+        <v>22</v>
+      </c>
+      <c r="I49" s="28">
+        <f t="shared" si="4"/>
+        <v>40.133779264214049</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A50" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50">
+        <v>66</v>
+      </c>
+      <c r="D50" s="27">
+        <v>46.7</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+      <c r="F50" t="s">
+        <v>22</v>
+      </c>
+      <c r="G50" t="s">
+        <v>22</v>
+      </c>
+      <c r="H50" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="28">
+        <f t="shared" si="4"/>
+        <v>25.695931477516055</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51">
+        <v>67</v>
+      </c>
+      <c r="D51" s="27">
+        <v>62.7</v>
+      </c>
+      <c r="E51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F51" t="s">
+        <v>22</v>
+      </c>
+      <c r="G51" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="28">
+        <f t="shared" si="4"/>
+        <v>19.138755980861241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B52" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52">
+        <v>68</v>
+      </c>
+      <c r="D52" s="27">
+        <v>46.4</v>
+      </c>
+      <c r="E52" t="s">
+        <v>22</v>
+      </c>
+      <c r="F52" t="s">
+        <v>22</v>
+      </c>
+      <c r="G52" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" t="s">
+        <v>22</v>
+      </c>
+      <c r="I52" s="28">
+        <f t="shared" si="4"/>
+        <v>25.862068965517242</v>
       </c>
     </row>
   </sheetData>
@@ -7295,8 +7473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4B47553-AD92-3A4E-A1D2-704B4666022D}">
   <dimension ref="A1:N11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7371,7 +7549,7 @@
         <v>28.2</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G7" si="0">(E2+F2)/2</f>
+        <f t="shared" ref="G2:G10" si="0">(E2+F2)/2</f>
         <v>28.299999999999997</v>
       </c>
       <c r="H2">
@@ -7381,7 +7559,7 @@
         <v>13.7</v>
       </c>
       <c r="J2">
-        <f>(H2+I2)/2</f>
+        <f t="shared" ref="J2:J10" si="1">(H2+I2)/2</f>
         <v>13.649999999999999</v>
       </c>
       <c r="K2">
@@ -7424,7 +7602,7 @@
         <v>18.2</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J10" si="1">(H3+I3)/2</f>
+        <f t="shared" si="1"/>
         <v>18.2</v>
       </c>
       <c r="K3">
@@ -7480,7 +7658,7 @@
         <v>33</v>
       </c>
       <c r="N4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -7526,7 +7704,7 @@
         <v>33</v>
       </c>
       <c r="N5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -7572,7 +7750,7 @@
         <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -7608,7 +7786,7 @@
         <f t="shared" si="1"/>
         <v>19.149999999999999</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="39">
         <v>8.1999999999999993</v>
       </c>
       <c r="L7" t="s">
@@ -7638,7 +7816,7 @@
         <v>46.6</v>
       </c>
       <c r="G8">
-        <f t="shared" ref="G8:G10" si="2">(E8+F8)/2</f>
+        <f t="shared" si="0"/>
         <v>46.7</v>
       </c>
       <c r="H8">
@@ -7651,7 +7829,7 @@
         <f t="shared" si="1"/>
         <v>48.6</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="39">
         <v>9.1</v>
       </c>
       <c r="L8" t="s">
@@ -7663,94 +7841,94 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C9">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D9">
         <v>20211029</v>
       </c>
       <c r="E9">
-        <v>46.4</v>
+        <v>62.8</v>
       </c>
       <c r="F9">
-        <v>46.4</v>
+        <v>62.6</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
-        <v>46.4</v>
+        <f t="shared" si="0"/>
+        <v>62.7</v>
       </c>
       <c r="H9">
-        <v>31.8</v>
+        <v>27</v>
       </c>
       <c r="I9">
-        <v>31.8</v>
+        <v>27</v>
       </c>
       <c r="J9">
         <f t="shared" si="1"/>
-        <v>31.8</v>
-      </c>
-      <c r="K9" s="40">
-        <v>5.6</v>
+        <v>27</v>
+      </c>
+      <c r="K9" s="39">
+        <v>8.9</v>
       </c>
       <c r="L9" t="s">
         <v>61</v>
       </c>
       <c r="M9" t="s">
-        <v>96</v>
+        <v>33</v>
       </c>
       <c r="N9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B10" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C10">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10">
         <v>20211029</v>
       </c>
       <c r="E10">
-        <v>62.8</v>
+        <v>46.4</v>
       </c>
       <c r="F10">
-        <v>62.6</v>
+        <v>46.4</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
-        <v>62.7</v>
+        <f t="shared" si="0"/>
+        <v>46.4</v>
       </c>
       <c r="H10">
-        <v>27</v>
+        <v>31.8</v>
       </c>
       <c r="I10">
-        <v>27</v>
+        <v>31.8</v>
       </c>
       <c r="J10">
         <f t="shared" si="1"/>
-        <v>27</v>
-      </c>
-      <c r="K10" s="40">
-        <v>8.9</v>
+        <v>31.8</v>
+      </c>
+      <c r="K10" s="39">
+        <v>5.6</v>
       </c>
       <c r="L10" t="s">
         <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="N10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -7794,10 +7972,15 @@
         <v>22</v>
       </c>
       <c r="N11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:N1" xr:uid="{B4B47553-AD92-3A4E-A1D2-704B4666022D}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N11">
+      <sortCondition ref="C1:C11"/>
+    </sortState>
+  </autoFilter>
   <conditionalFormatting sqref="M1">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",M1)))</formula>

</xml_diff>

<commit_message>
molecular labwork shipping TagSeq samples
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFA4CFEA-CD3B-BE4D-90E3-2E160D319E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED37FD8-BFCC-5348-A69A-A93498560208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="2" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="4" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
     <sheet name="DNARNA-Extractions" sheetId="2" r:id="rId2"/>
     <sheet name="Gene-Exp-Prep" sheetId="3" r:id="rId3"/>
     <sheet name="Re-extractions" sheetId="4" r:id="rId4"/>
+    <sheet name="Samples sequenced" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNARNA-Extractions'!$A$1:$O$60</definedName>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="827" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="99">
   <si>
     <t>ColonyID</t>
   </si>
@@ -343,16 +344,19 @@
     <t>DNA is much more degraded than the December fragments</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Send as much as possible</t>
-  </si>
-  <si>
     <t>see below</t>
   </si>
   <si>
     <t>RNASeq shipped in individual 1.5 mL tubes (labeled by extraction ID)</t>
+  </si>
+  <si>
+    <t>Sending 52.2 uL (that is all we had left)</t>
+  </si>
+  <si>
+    <t>RNASeq</t>
+  </si>
+  <si>
+    <t>WGBS, ITS2, 16S</t>
   </si>
 </sst>
 </file>
@@ -2265,7 +2269,7 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5217,8 +5221,8 @@
   </sheetPr>
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5229,7 +5233,7 @@
     <col min="6" max="6" width="26.5" customWidth="1"/>
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="9" width="18.83203125" customWidth="1"/>
-    <col min="10" max="10" width="21" customWidth="1"/>
+    <col min="10" max="10" width="34" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -5699,7 +5703,7 @@
         <v>22</v>
       </c>
       <c r="J9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K9" s="31" t="s">
         <v>78</v>
@@ -6028,7 +6032,7 @@
         <v>41.237113402061851</v>
       </c>
       <c r="K14" s="33" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -6260,7 +6264,7 @@
         <v>22</v>
       </c>
       <c r="J20" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K20" s="42"/>
       <c r="L20" s="43"/>
@@ -6356,7 +6360,7 @@
         <v>22</v>
       </c>
       <c r="J22" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K22" s="42"/>
       <c r="L22" s="43"/>
@@ -6405,7 +6409,7 @@
         <v>22</v>
       </c>
       <c r="J23" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K23" s="42"/>
       <c r="L23" s="43"/>
@@ -6501,7 +6505,7 @@
         <v>22</v>
       </c>
       <c r="J25" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K25" s="42"/>
       <c r="L25" s="43"/>
@@ -6597,7 +6601,7 @@
         <v>22</v>
       </c>
       <c r="J27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K27" s="43"/>
       <c r="L27" s="43"/>
@@ -6646,7 +6650,7 @@
         <v>22</v>
       </c>
       <c r="J28" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K28" s="43"/>
       <c r="L28" s="43"/>
@@ -6763,7 +6767,7 @@
         <v>22</v>
       </c>
       <c r="J31" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.2">
@@ -7003,7 +7007,7 @@
         <v>22</v>
       </c>
       <c r="J38" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -7176,7 +7180,7 @@
         <v>60.150375939849624</v>
       </c>
       <c r="J43" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -7474,7 +7478,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7925,7 +7929,7 @@
         <v>61</v>
       </c>
       <c r="M10" t="s">
-        <v>94</v>
+        <v>33</v>
       </c>
       <c r="N10" t="s">
         <v>93</v>
@@ -7989,4 +7993,1167 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A087B238-F7D8-014B-B799-EF98309A325B}">
+  <dimension ref="A1:I52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="F1" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="F2" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27">
+        <v>22</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="27">
+        <v>2</v>
+      </c>
+      <c r="I4" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27">
+        <v>21.4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="27">
+        <v>4</v>
+      </c>
+      <c r="I5" s="27">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="27">
+        <v>6</v>
+      </c>
+      <c r="D6" s="27">
+        <v>21.3</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="27">
+        <v>6</v>
+      </c>
+      <c r="I6" s="27">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="27">
+        <v>16</v>
+      </c>
+      <c r="D7" s="27">
+        <v>34</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="27">
+        <v>16</v>
+      </c>
+      <c r="I7" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="27">
+        <v>17</v>
+      </c>
+      <c r="D8" s="27">
+        <v>30.8</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="27">
+        <v>17</v>
+      </c>
+      <c r="I8" s="27">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="27">
+        <v>21</v>
+      </c>
+      <c r="D9" s="27">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="27">
+        <v>18</v>
+      </c>
+      <c r="I9" s="27">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="27">
+        <v>22</v>
+      </c>
+      <c r="D10" s="27">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="27">
+        <v>21</v>
+      </c>
+      <c r="I10" s="27">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="27">
+        <v>23</v>
+      </c>
+      <c r="D11" s="27">
+        <v>30</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="27">
+        <v>22</v>
+      </c>
+      <c r="I11" s="27">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="27">
+        <v>24</v>
+      </c>
+      <c r="D12" s="27">
+        <v>44.8</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H12" s="27">
+        <v>23</v>
+      </c>
+      <c r="I12" s="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="27">
+        <v>25</v>
+      </c>
+      <c r="D13" s="27">
+        <v>29.1</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="27">
+        <v>24</v>
+      </c>
+      <c r="I13" s="27">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="27">
+        <v>26</v>
+      </c>
+      <c r="D14" s="27">
+        <v>28.7</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H14" s="27">
+        <v>25</v>
+      </c>
+      <c r="I14" s="27">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="27">
+        <v>28</v>
+      </c>
+      <c r="D15" s="27">
+        <v>30.7</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="27">
+        <v>26</v>
+      </c>
+      <c r="I15" s="27">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="27">
+        <v>29</v>
+      </c>
+      <c r="D16" s="27">
+        <v>51.4</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="27">
+        <v>28</v>
+      </c>
+      <c r="I16" s="27">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="27">
+        <v>30</v>
+      </c>
+      <c r="D17" s="27">
+        <v>31.7</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="27">
+        <v>29</v>
+      </c>
+      <c r="I17" s="27">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="27">
+        <v>31</v>
+      </c>
+      <c r="D18" s="27">
+        <v>23</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H18" s="27">
+        <v>30</v>
+      </c>
+      <c r="I18" s="27">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="27">
+        <v>33</v>
+      </c>
+      <c r="D19" s="27">
+        <v>56.8</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="27">
+        <v>31</v>
+      </c>
+      <c r="I19" s="27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="27">
+        <v>37</v>
+      </c>
+      <c r="D20" s="27">
+        <v>32.799999999999997</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H20" s="27">
+        <v>32</v>
+      </c>
+      <c r="I20" s="27">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="27">
+        <v>39</v>
+      </c>
+      <c r="D21" s="27">
+        <v>73.2</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H21" s="27">
+        <v>33</v>
+      </c>
+      <c r="I21" s="27">
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="27">
+        <v>42</v>
+      </c>
+      <c r="D22" s="27">
+        <v>36.9</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="27">
+        <v>34</v>
+      </c>
+      <c r="I22" s="27">
+        <v>18.600000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="27">
+        <v>43</v>
+      </c>
+      <c r="D23" s="27">
+        <v>26</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="27">
+        <v>35</v>
+      </c>
+      <c r="I23" s="27">
+        <v>17.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="27">
+        <v>45</v>
+      </c>
+      <c r="D24" s="27">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" s="27">
+        <v>37</v>
+      </c>
+      <c r="I24" s="27">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="27">
+        <v>46</v>
+      </c>
+      <c r="D25" s="27">
+        <v>71.599999999999994</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="27">
+        <v>38</v>
+      </c>
+      <c r="I25" s="27">
+        <v>13.55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="27">
+        <v>47</v>
+      </c>
+      <c r="D26" s="27">
+        <v>45.9</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" s="27">
+        <v>39</v>
+      </c>
+      <c r="I26" s="27">
+        <v>73.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="27">
+        <v>50</v>
+      </c>
+      <c r="D27" s="27">
+        <v>44.3</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" s="27">
+        <v>40</v>
+      </c>
+      <c r="I27" s="27">
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="27">
+        <v>51</v>
+      </c>
+      <c r="D28" s="27">
+        <v>24.6</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H28" s="27">
+        <v>41</v>
+      </c>
+      <c r="I28" s="27">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="27">
+        <v>52</v>
+      </c>
+      <c r="D29" s="27">
+        <v>40.1</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H29" s="27">
+        <v>42</v>
+      </c>
+      <c r="I29" s="27">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="27">
+        <v>54</v>
+      </c>
+      <c r="D30" s="27">
+        <v>72.2</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H30" s="27">
+        <v>43</v>
+      </c>
+      <c r="I30" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="27">
+        <v>55</v>
+      </c>
+      <c r="D31" s="27">
+        <v>55.5</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H31" s="27">
+        <v>44</v>
+      </c>
+      <c r="I31" s="27">
+        <v>12.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="27">
+        <v>56</v>
+      </c>
+      <c r="D32" s="27">
+        <v>60.4</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H32" s="27">
+        <v>45</v>
+      </c>
+      <c r="I32" s="27">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="27">
+        <v>57</v>
+      </c>
+      <c r="D33" s="27">
+        <v>34.799999999999997</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H33" s="27">
+        <v>46</v>
+      </c>
+      <c r="I33" s="27">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="27">
+        <v>59</v>
+      </c>
+      <c r="D34" s="27">
+        <v>19.95</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="27">
+        <v>47</v>
+      </c>
+      <c r="I34" s="27">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35" s="27">
+        <v>28.3</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H35" s="27">
+        <v>50</v>
+      </c>
+      <c r="I35" s="27">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>61</v>
+      </c>
+      <c r="D36" s="27">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H36" s="27">
+        <v>51</v>
+      </c>
+      <c r="I36" s="27">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37">
+        <v>62</v>
+      </c>
+      <c r="D37" s="27">
+        <v>52.3</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37" s="27">
+        <v>52</v>
+      </c>
+      <c r="I37" s="27">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38">
+        <v>63</v>
+      </c>
+      <c r="D38" s="27">
+        <v>55.7</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H38" s="27">
+        <v>53</v>
+      </c>
+      <c r="I38" s="27">
+        <v>10.25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39">
+        <v>64</v>
+      </c>
+      <c r="D39" s="27">
+        <v>101</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H39" s="27">
+        <v>54</v>
+      </c>
+      <c r="I39" s="27">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>65</v>
+      </c>
+      <c r="D40" s="27">
+        <v>29.9</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H40" s="27">
+        <v>55</v>
+      </c>
+      <c r="I40" s="27">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41">
+        <v>66</v>
+      </c>
+      <c r="D41" s="27">
+        <v>46.7</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H41" s="27">
+        <v>56</v>
+      </c>
+      <c r="I41" s="27">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42">
+        <v>67</v>
+      </c>
+      <c r="D42" s="27">
+        <v>62.7</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H42" s="27">
+        <v>57</v>
+      </c>
+      <c r="I42" s="27">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43">
+        <v>68</v>
+      </c>
+      <c r="D43" s="27">
+        <v>46.4</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H43" s="27">
+        <v>59</v>
+      </c>
+      <c r="I43" s="27">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F44" s="5"/>
+      <c r="G44" s="6"/>
+      <c r="I44" s="27"/>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F45" s="5"/>
+      <c r="G45" s="6"/>
+      <c r="I45" s="27"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F46" s="5"/>
+      <c r="G46" s="25"/>
+      <c r="I46" s="27"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F47" s="5"/>
+      <c r="G47" s="25"/>
+      <c r="I47" s="27"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F48" s="5"/>
+      <c r="G48" s="25"/>
+      <c r="I48" s="27"/>
+    </row>
+    <row r="49" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F49" s="5"/>
+      <c r="G49" s="6"/>
+      <c r="I49" s="27"/>
+    </row>
+    <row r="50" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F50" s="5"/>
+      <c r="G50" s="6"/>
+      <c r="I50" s="27"/>
+    </row>
+    <row r="51" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F51" s="5"/>
+      <c r="G51" s="25"/>
+      <c r="I51" s="27"/>
+    </row>
+    <row r="52" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F52" s="5"/>
+      <c r="G52" s="25"/>
+      <c r="I52" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
molecular lab work updates and shipment files
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED37FD8-BFCC-5348-A69A-A93498560208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD88C6-E969-0041-B609-F53260C0F101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="4" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="5" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Gene-Exp-Prep" sheetId="3" r:id="rId3"/>
     <sheet name="Re-extractions" sheetId="4" r:id="rId4"/>
     <sheet name="Samples sequenced" sheetId="5" r:id="rId5"/>
+    <sheet name="RNASeq" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNARNA-Extractions'!$A$1:$O$60</definedName>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="999" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="99">
   <si>
     <t>ColonyID</t>
   </si>
@@ -7999,8 +8000,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A087B238-F7D8-014B-B799-EF98309A325B}">
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9156,4 +9157,616 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B445F5-4F40-E543-B7D9-2FD2FB7E6D8B}">
+  <dimension ref="A1:D43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="27">
+        <v>2</v>
+      </c>
+      <c r="D4" s="27">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="27">
+        <v>4</v>
+      </c>
+      <c r="D5" s="27">
+        <v>21.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="27">
+        <v>6</v>
+      </c>
+      <c r="D6" s="27">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="27">
+        <v>16</v>
+      </c>
+      <c r="D7" s="27">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="27">
+        <v>17</v>
+      </c>
+      <c r="D8" s="27">
+        <v>30.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="27">
+        <v>21</v>
+      </c>
+      <c r="D9" s="27">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="27">
+        <v>22</v>
+      </c>
+      <c r="D10" s="27">
+        <v>37.799999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="27">
+        <v>23</v>
+      </c>
+      <c r="D11" s="27">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="27">
+        <v>24</v>
+      </c>
+      <c r="D12" s="27">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="27">
+        <v>25</v>
+      </c>
+      <c r="D13" s="27">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="27">
+        <v>26</v>
+      </c>
+      <c r="D14" s="27">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="27">
+        <v>28</v>
+      </c>
+      <c r="D15" s="27">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="27">
+        <v>29</v>
+      </c>
+      <c r="D16" s="27">
+        <v>51.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="27">
+        <v>30</v>
+      </c>
+      <c r="D17" s="27">
+        <v>31.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="27">
+        <v>31</v>
+      </c>
+      <c r="D18" s="27">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="27">
+        <v>33</v>
+      </c>
+      <c r="D19" s="27">
+        <v>56.8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="27">
+        <v>37</v>
+      </c>
+      <c r="D20" s="27">
+        <v>32.799999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="27">
+        <v>39</v>
+      </c>
+      <c r="D21" s="27">
+        <v>73.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="27">
+        <v>42</v>
+      </c>
+      <c r="D22" s="27">
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="27">
+        <v>43</v>
+      </c>
+      <c r="D23" s="27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="27">
+        <v>45</v>
+      </c>
+      <c r="D24" s="27">
+        <v>76.400000000000006</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="27">
+        <v>46</v>
+      </c>
+      <c r="D25" s="27">
+        <v>71.599999999999994</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="27">
+        <v>47</v>
+      </c>
+      <c r="D26" s="27">
+        <v>45.9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="27">
+        <v>50</v>
+      </c>
+      <c r="D27" s="27">
+        <v>44.3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="27">
+        <v>51</v>
+      </c>
+      <c r="D28" s="27">
+        <v>24.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="27">
+        <v>52</v>
+      </c>
+      <c r="D29" s="27">
+        <v>40.1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="27">
+        <v>54</v>
+      </c>
+      <c r="D30" s="27">
+        <v>72.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="27">
+        <v>55</v>
+      </c>
+      <c r="D31" s="27">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32" s="27">
+        <v>56</v>
+      </c>
+      <c r="D32" s="27">
+        <v>60.4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B33" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C33" s="27">
+        <v>57</v>
+      </c>
+      <c r="D33" s="27">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="27">
+        <v>59</v>
+      </c>
+      <c r="D34" s="27">
+        <v>19.95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35">
+        <v>60</v>
+      </c>
+      <c r="D35" s="27">
+        <v>28.3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C36">
+        <v>61</v>
+      </c>
+      <c r="D36" s="27">
+        <v>35.299999999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37">
+        <v>62</v>
+      </c>
+      <c r="D37" s="27">
+        <v>52.3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B38" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38">
+        <v>63</v>
+      </c>
+      <c r="D38" s="27">
+        <v>55.7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39">
+        <v>64</v>
+      </c>
+      <c r="D39" s="27">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40">
+        <v>65</v>
+      </c>
+      <c r="D40" s="27">
+        <v>29.9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C41">
+        <v>66</v>
+      </c>
+      <c r="D41" s="27">
+        <v>46.7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42">
+        <v>67</v>
+      </c>
+      <c r="D42" s="27">
+        <v>62.7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C43">
+        <v>68</v>
+      </c>
+      <c r="D43" s="27">
+        <v>46.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data readme and molecular labwork spreadsheet
</commit_message>
<xml_diff>
--- a/data/Molecular-labwork.xlsx
+++ b/data/Molecular-labwork.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emmastrand/MyProjects/HI_Bleaching_Timeseries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADD88C6-E969-0041-B609-F53260C0F101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456BB793-9334-7E4F-9827-42A7DFFD7A5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5820" yWindow="460" windowWidth="27780" windowHeight="18960" activeTab="5" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
+    <workbookView xWindow="37060" yWindow="960" windowWidth="27780" windowHeight="18960" activeTab="7" xr2:uid="{A494CC7D-A20D-2E4C-9497-7BF4F462E6C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Master-ID-List" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="Re-extractions" sheetId="4" r:id="rId4"/>
     <sheet name="Samples sequenced" sheetId="5" r:id="rId5"/>
     <sheet name="RNASeq" sheetId="6" r:id="rId6"/>
+    <sheet name="ITS_Seq" sheetId="7" r:id="rId7"/>
+    <sheet name="16S_Seq" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'DNARNA-Extractions'!$A$1:$O$60</definedName>
@@ -61,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1085" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1097" uniqueCount="107">
   <si>
     <t>ColonyID</t>
   </si>
@@ -358,6 +360,30 @@
   </si>
   <si>
     <t>WGBS, ITS2, 16S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kevin Wong did molecular lab work </t>
+  </si>
+  <si>
+    <t>Emma Strand did molecular lab work processing</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1lLvCp-RoRiBSGZ4NBPwi6cmZuozmfS20OJ7hBIueldU/edit#gid=0</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1hFIY0g74x_yjGrz7F8n_IFccVfC5TheEPZtd7_je3uI/edit#gid=1693868430</t>
+  </si>
+  <si>
+    <t>Sequencing submission:</t>
+  </si>
+  <si>
+    <t>Processing information:</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/spreadsheets/d/1Zs6nKV5QTHoSMigXAZXgNoiaDMglZ9uycr6kK0upcTU/edit#gid=1607182602</t>
+  </si>
+  <si>
+    <t>Google spreadsheet links here</t>
   </si>
 </sst>
 </file>
@@ -8001,7 +8027,7 @@
   <dimension ref="A1:I52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D43"/>
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9163,7 +9189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7B445F5-4F40-E543-B7D9-2FD2FB7E6D8B}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -9769,4 +9795,94 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056D86C6-5F04-A042-BC5A-533ABB4D623D}">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8EF5F71-E667-4D49-9523-669C7A5949BC}">
+  <dimension ref="A2:A9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>